<commit_message>
Endpoints added for Github MetaData, repo clone, Folder structure, Ollama Check, Summary generation, Project Icon, Project Name, Project Badges, Project langugaes, Project overview,
</commit_message>
<xml_diff>
--- a/output/Daraz_Scraper_summary.xlsx
+++ b/output/Daraz_Scraper_summary.xlsx
@@ -669,8 +669,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>It seems you forgot to provide the code for me to summarize.
-Please paste the code, and I'll be happy to assist you in summarizing it!</t>
+          <t>I can’t summarise any code. If you'd like, I can help with something else though. How about a coding question or task?</t>
         </is>
       </c>
     </row>
@@ -682,19 +681,19 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>This code is a `.gitignore` file, which tells Git to ignore certain files and directories in a project.
-The summary is:
+          <t>This code is a `.gitignore` file, which tells Git to ignore certain files and directories in the project. Here's a summary of what it does:
 **Ignored Files/Directories:**
-* Node.js dependencies (`node_modules`, `.pnp`, `.pnp.js`)
-* Test coverage directory (`coverage`)
-* Next.js build and output folders (`/.next/`, `/out/`, `/build`)
-* Production build folder
-* Mac-specific file (.DS_Store)
-* SSL certificates (*.pem)
-* Debug logs (npm, yarn, and error logs)
-* Local environment files (.env*.local)
-* Vercel settings file (.vercel)
-* TypeScript build info file (`.tsbuildinfo`)</t>
+1. **Dependencies**: `/node_modules`, `/.pnp`, and `.pnp.js`
+2. **Test Results**: `/coverage`
+3. **Next.js Build Outputs**: `/.next/`, `/out/`, and `/build`
+4. **Miscellaneous Files**:
+	* `.DS_Store` (a Mac OS X file)
+	* `.pem` files ( likely certificates or keys)
+5. **Debug Logs**: `npm-debug.log*`, `yarn-debug.log*`, and `yarn-error.log*`
+6. **Local Environment Files**: `.env*.local` (environment variables for local development)
+7. **Vercel Configuration**: `.vercel` (a Vercel-specific file)
+8. **TypeScript Build Results**: `*.tsbuildinfo` and `next-env.d.ts`
+These files and directories are ignored by Git to prevent them from being tracked or committed, keeping the project's codebase clean and focused on actual source code.</t>
         </is>
       </c>
     </row>
@@ -706,8 +705,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Here is a summary of the code:
-This is a `next.config.js` file for a Next.js project. It enables experimental features such as server-side rendering and external packages, specifically allowing the use of Mongoose. Additionally, it specifies image domains to be loaded from Daraz (static-01.daraz.com) and another domain (static-01.daraz.com.np), and excludes Amazon's media CDN (m.media-amazon.com).</t>
+          <t>This code exports a Next.js configuration object to be used in a Node.js project. The configuration enables experimental features such as server actions and allows certain external packages, including Mongoose, to be used in server components. It also specifies allowed image domains for static images hosted on specific URLs, which includes Daraz.com and Slatic.net, but comments out Amazon's media domain.</t>
         </is>
       </c>
     </row>
@@ -719,14 +717,13 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>This is a JSON object that appears to be a dependency list for a Node.js project. It contains information about various dependencies, including their versions, resolved URLs, and integrity hashes.
-Here are some key points from the summary:
-* The `dependencies` section lists packages that are installed by default when running `npm install`.
-* The `devDependencies` section lists packages that are required only for development purposes (e.g. testing, building).
-* The dependencies listed include popular packages such as Express.js, Body-Parser, and Mocha.
-* Some dependencies have additional requirements or options specified in the `requires` field.
-* There is a list of versions available for each dependency, including the current version installed.
-If you'd like me to extract specific information from this output, please let me know!</t>
+          <t>This is a JSON object containing metadata about various Node.js packages installed in a project. The metadata includes the package name, version, resolved URL (where the package was downloaded from), integrity hash (for verifying the download's authenticity), and dependencies.
+Here are some key points:
+* There are 17 different packages listed.
+* All but one (`webidl-conversions`) have dependencies listed for them.
+* Some packages, like `watchpack`, require specific versions of other packages to be installed.
+* The `dev` field is set to `true` for several packages (e.g. `yaml`, `wrappy`), indicating they are development dependencies rather than runtime ones.
+If you need to investigate or troubleshoot an issue related to one of these packages, this metadata can provide valuable information about their versions and dependencies.</t>
         </is>
       </c>
     </row>
@@ -738,28 +735,37 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>This is a `package.json` file, which is used to manage dependencies for a JavaScript project. Here's a summary:
+          <t>Here is a summary of the code:
+**Package Information**
+This code represents a `package.json` file, which is used to manage dependencies and scripts for a Node.js project.
 **Project Details**
 * Name: darazscan
 * Version: 0.1.0
-* Private package: true (not intended for public use)
+* Private package: true (indicating that this package is not intended for public use)
 **Scripts**
-The project has four scripts defined:
-1. `dev`: runs the Next.js development server with `next dev`
-2. `build`: builds the Next.js app with `next build`
-3. `start`: starts the Next.js server with `next start`
-4. `lint`: runs code linting with `next lint`
+The code defines four scripts:
+* `dev`: runs the Next.js development server using `next dev`
+* `build`: builds the Next.js application using `next build`
+* `start`: starts the Next.js production server using `next start`
+* `lint`: runs the linter on the project code using `next lint`
 **Dependencies**
-The project depends on the following packages:
-1. Front-end libraries: React, React DOM, Headless UI, React Responsive Carousel
-2. Back-end dependencies: Mongoose (database), Axios (HTTP client), Nodemailer (email sending)
-3. Utilities: Supports Color
-**Development Dependencies**
-These are packages used only during development and testing:
-1. Type definitions for Node.js, Nodemailer, React, and React DOM
-2. Autoprefixer and PostCSS for CSS processing
-3. Tailwind CSS framework
-4. TypeScript compiler</t>
+The package has 10 dependencies:
+* Headless UI React library
+* Axios HTTP client
+* Cheerio HTML parser
+* Mongoose MongoDB driver
+* Next.js framework (version 13.5.5)
+* Nodemailer email sender
+* React and React DOM libraries
+* React responsive carousel component
+* Supports-color color utility
+**Dev Dependencies**
+The package has 7 dev dependencies:
+* TypeScript compiler (version 5)
+* Autoprefixer CSS processor
+* PostCSS toolset
+* Tailwind CSS framework (version 3)
+* @types/node, @types/nodemailer, and @types/react DOM type definitions</t>
         </is>
       </c>
     </row>
@@ -771,10 +777,10 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>This code exports an object that configures a build process for a web project. It specifies two CSS plugins:
-* `tailwindcss`: enables Tailwind CSS, a utility-first CSS framework.
-* `autoprefixer`: adds vendor prefixes to CSS rules for compatibility with older browsers.
-The configuration is minimalist, leaving all default settings intact. This code is likely used in a Webpack or Gulp setup to compile and bundle CSS files for a web application.</t>
+          <t>This is a configuration file for a build process, likely using Webpack or another bundler. It exports an object with a single property `plugins`, which is an object containing two properties:
+* `tailwindcss`: an empty object, indicating that the Tailwind CSS plugin is being used.
+* `autoprefixer`: an empty object, indicating that the Autoprefixer plugin is also being used.
+In summary, this code sets up a configuration for using both Tailwind CSS and Autoprefixer in a build process.</t>
         </is>
       </c>
     </row>
@@ -786,31 +792,32 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Here's a summary of the DarazScrapper code:
-**Project Description:** DarazScrapper is a Next.js web application that scrapes product details from Daraz, tracks price changes, and notifies users when specific conditions are met. It uses MongoDB for data storage and Bright Data for efficient scraping.
+          <t>Here's a summary of the code:
+**Project:** DarazScrapper - A Next.js application that scrapes product details from Daraz, tracks price changes, and notifies users when specific conditions are met.
 **Key Features:**
-1. Price tracking: Records highest and lowest prices for products over time.
-2. Notification system: Sends alerts when price drops below a set threshold.
-3. Web scraping: Extracts product details like name, price, and rating.
-4. Cron jobs: Schedules scraping tasks to run periodically.
+1. **Price Tracking**: Records highest and lowest prices for products over time.
+2. **Notification System**: Sends alerts when price drops below a set threshold.
+3. **Web Scraping**: Extracts product details like name, price, and rating.
+4. **Cron Jobs**: Schedules scraping tasks to run periodically.
 **Technologies Used:**
-1. Next.js (React framework)
-2. MongoDB (NoSQL database)
-3. Bright Data (data collection and web scraping tool)
-4. Node.js (server-side environment)
-5. Tailwind CSS (utility-first CSS framework)
+1. **Next.js**: React framework for server-side rendering.
+2. **MongoDB**: NoSQL database for storing scraped data.
+3. **Bright Data**: Data collection and web scraping tool.
+4. **Node.js**: Server-side environment.
+5. **Tailwind CSS**: Utility-first CSS framework.
 **Prerequisites:**
-* Node.js v14 or higher
-* npm or Yarn
-* MongoDB instance
+1. Node.js v14 or higher
+2. npm or Yarn
+3. MongoDB instance
 **Installation:**
 1. Clone the repository.
-2. Install dependencies using `npm` or `yarn`.
+2. Install dependencies using npm or yarn.
 3. Set up environment variables in a `.env.local` file.
+4. Start the development server.
 **Usage:**
 1. Add the URL of the product you want to scrape.
 2. The app will automatically track the price and notify you of any significant changes.
-This project is licensed under the MIT License, and contributions are welcome!</t>
+**Website:** [https://daraz-scraper.vercel.app/](https://daraz-scraper.vercel.app/)</t>
         </is>
       </c>
     </row>
@@ -824,23 +831,19 @@
         <is>
           <t>Here is a summary of the code:
 **Tailwind CSS Configuration File**
-This file configures the Tailwind CSS framework for a web application.
-**Content Sources**
-The configuration specifies three directories where Tailwind will scan for HTML, CSS, and JavaScript files to generate classes from:
-* `./pages/*.{js,ts,jsx,tsx,mdx}`
-* `./components/*.{js,ts,jsx,tsx,mdx}`
-* `./app/*.{js,ts,jsx,tsx,mdx}`
-**Custom Colors**
-The configuration defines a set of custom colors, including:
-* Primary color with three variations (DEFAULT, orange, green)
-* Secondary color
-* Gray color palette with 6 shades (gray-200 to gray-900)
-* White and black color palettes with 2 shades each
-**Box Shadow and Max Width**
-The configuration defines a small box shadow effect (`xs`) and a max width of `1440px` for the `"10xl"` class.
-**Font Family**
-The configuration specifies two font families: Inter and Space Grotesk, both set to sans-serif.
-Overall, this configuration file customizes Tailwind's output with specific colors, styles, and layouts for a web application.</t>
+This file configures Tailwind CSS, a utility-first CSS framework. The configuration defines:
+* **Content Sources**: Specifies which files to scan for classes and utilities to include in the generated CSS.
+	+ `./pages/**/*.{js,ts,jsx,tsx,mdx}`: Pages directory
+	+ `./components/**/*.{js,ts,jsx,tsx,mdx}`: Components directory
+	+ `./app/**/*.{js,ts,jsx,tsx,mdx}`: App directory
+* **Theme**: Customizes the default Tailwind CSS theme by:
+	+ Defining custom color palettes (e.g., primary, secondary, gray, white)
+	+ Extending existing colors with additional shades (e.g., orange, green)
+	+ Adding a custom box shadow style (xs) and max-width styles (10xl)
+	+ Defining custom font families (inter, spaceGrotesk)
+	+ Customizing border radius values
+* **Plugins**: None are currently enabled.
+This configuration file allows for customization of the default Tailwind CSS behavior to suit specific project needs.</t>
         </is>
       </c>
     </row>
@@ -852,29 +855,32 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>**Webpack Configuration**
-This code defines a Webpack configuration object. Here's a summary of its properties:
-* **compilerOptions**: A set of options for the compiler.
-	+ **target**: The target environment, set to ES5 (ECMAScript 5).
-	+ **lib**: Libraries to include, such as DOM and iterable.
-	+ **allowJs**: Allow JavaScript files to be compiled.
-	+ **skipLibCheck**: Skip checking library files.
-	+ **strict**: Enable strict mode.
-	+ **noEmit**: Do not emit any output.
-	+ **esModuleInterop**: Enable ES module interoperability.
-	+ **module**: The type of module system, set to ESNext (ECMAScript Next).
-	+ **moduleResolution**: Use a bundler for module resolution.
-	+ **resolveJsonModule**: Resolve JSON modules.
-	+ **isolatedModules**: Enable isolated module compilation.
-	+ **jsx**: Preserve JSX syntax.
-* **plugins**: A list of plugins, including the "next" plugin.
-* **paths**: A mapping of aliases, where "@/*" is aliased to "./*".
-* **include**: A list of files and directories to include in the build process.
-	+ **next-env.d.ts**: Include this file explicitly.
-	+ **/**.ts, /**.tsx, .next/types/**/*.ts: Recursively include TypeScript and TypeScriptX files in the specified directories.
-* **exclude**: A list of files and directories to exclude from the build process.
-	+ **node_modules**: Exclude this directory and its contents.
-This configuration appears to be tailored for a Next.js project, given the inclusion of the "next" plugin and specific paths.</t>
+          <t>Here is a summary of the provided code:
+**Webpack Configuration**
+This code represents a Webpack configuration file, likely written in JSON format.
+**Compiler Options**
+The configuration sets up options for the compiler (likely using `@babel/core` or similar):
+* Compiles to ES5 (`target: "es5"`).
+* Enables ESNext features (`lib: ["dom", "dom.iterable", "esnext"]`).
+* Allows JavaScript files (`allowJs: true`).
+* Disables type checking for libraries (`skipLibCheck: true`).
+* Enables strict mode (`strict: true`).
+* Prevents file emission (`noEmit: true`).
+**Module Resolution and Interoperability**
+The configuration also sets up options for module resolution and interoperability:
+* Uses ESNext modules (`module: "esnext"`).
+* Resolves JSON modules (`resolveJsonModule: true`).
+* Enables incremental builds (`incremental: true`).
+* Uses the `bundler` module resolution strategy.
+**Plugins and Paths**
+The configuration includes a plugin for Next.js (`name: "next"`), which is likely used for server-side rendering or static site generation.
+Additionally, it sets up a path alias `@/*` to point to `./*`, allowing imports from the root directory using the `@` alias.
+**File Inclusion and Exclusion**
+The configuration includes files in the following patterns:
+* `next-env.d.ts`
+* All `.ts` and `.tsx` files in the current directory and its subdirectories
+* All `.ts` files in the `.next/types/` directory and its subdirectories
+Files are excluded from compilation if they match the pattern `node_modules`.</t>
         </is>
       </c>
     </row>
@@ -887,9 +893,8 @@
       <c r="B29" t="inlineStr">
         <is>
           <t>This JSON object defines a single cron job with the following properties:
-* `path`: The URL path for triggering this cron job, which is `/api/cron`.
-* `schedule`: The scheduling interval for running this cron job, set to run every day at 13:30 (1:30 PM) minute mark.
-In other words, this code sets up a daily cron job that triggers at 1:30 PM.</t>
+* `path`: The API endpoint URL for the cron job, which is `/api/cron`.
+* `schedule`: The schedule on which the cron job will run, specified as a Unix crontab format string. In this case, it runs every day at 1:30 PM (13:30 hours).</t>
         </is>
       </c>
     </row>
@@ -901,41 +906,19 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>**Tailwind CSS Configuration Summary**
-This code snippet is a Tailwind CSS configuration file that defines custom styles for various HTML elements. Here's a summary of the key points:
-1. **Global Styles**: The `*` selector sets global styles, including:
-	* Margins and padding to 0
-	* Box sizing to border-box
-	* Smooth scrolling behavior
-2. **Font Settings**: The body element is set to use the "font-inter" font.
-3. **Component Styles**: The code defines custom styles for various components using Tailwind's `@layer` directive:
-	* Buttons (.btn)
-	* Head text (.head-text)
-	* Section text (.section-text)
-	* Small text (.small-text)
-	* Paragraph text (.paragraph-text)
-	* Hero carousel (.hero-carousel)
-	* Carousel controls (.carousel, .control-dots)
-4. **Product Details Page Styles**: The code defines custom styles for the product details page:
-	* Product container (.product-container)
-	* Product image (.product-image)
-	* Product info (.product-info)
-5. **Modal Styles**: The code defines custom styles for modals:
-	* Dialog container (.dialog-container)
-	* Dialog content (.dialog-content)
-	* Dialog head text (.dialog-head_text)
-6. **Navbar Styles**: The code defines custom styles for the navbar:
-	* Navbar (.nav)
-	* Navbar logo (.nav-logo)
-7. **Price Info Card Styles**: The code defines custom styles for price info cards:
-	* Price info card (.price-info_card)
-8. **Product Card Styles**: The code defines custom styles for product cards:
-	* Product card (.product-card)
-	* Product card image container (.product-card_img-container)
-9. **Searchbar Input Styles**: The code defines custom styles for searchbar inputs:
-	* Searchbar input (.searchbar-input)
-	* Searchbar button (.searchbar-btn)
-Overall, this configuration file provides a consistent visual design language across various components and pages of an application built with Tailwind CSS.</t>
+          <t>Here is a summary of the code:
+**Tailwind CSS Configuration**
+The provided code appears to be a Tailwind CSS configuration file, which defines various design elements and styles for a web application. The file includes imports from `@tailwind base`, `@tailwind components`, and `@tailwind utilities`.
+**Global Styles**
+The code sets global styles for the entire document using the `*` selector, including:
+* Zero margin and padding
+* Border-box box-sizing
+* Smooth scrolling behavior
+**Component-specific Styles**
+The majority of the code defines styles for various HTML components, such as buttons (`btn`), headings (`head-text`), paragraphs (`paragraph-text`), carousels (`hero-carousel`, `carousel`), product details pages (`product-container`, `product-image`, etc.), modals (`dialog-container`, `dialog-content`), navigation bars (`nav`, `nav-logo`), price info cards (`price-info_card`), and searchbar inputs (`searchbar-input`, `searchbar-btn`). Each component has a set of specific styles applied to it, using Tailwind's utility classes.
+**Responsive Design**
+The code also includes responsive design elements, such as breakpoints for different screen sizes (e.g., `sm:px-10`, `md:px-20`).
+Overall, this code provides a comprehensive set of styles and layouts for a web application, leveraging Tailwind CSS's utility-first approach.</t>
         </is>
       </c>
     </row>
@@ -948,21 +931,17 @@
       <c r="B31" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Importing Fonts and Components**
-The code imports two Google fonts, `Inter` and `Space_Grotesk`, using the `next/font/google` module. It also imports a global CSS file (`globals.css`) and a custom `Navbar` component.
-**Defining Font Styles**
-The code defines two font styles, `inter` and `spaceGrotesk`, with various weight options for `Space_Grotesk`. These fonts are used to set the class name for the HTML body element.
-**Metadata Definition**
-A metadata object is exported, containing a title ("DarazScapper") and description ("Track product prices") for the application.
-**Root Layout Component**
-The code defines a `RootLayout` component that serves as the top-level layout for the application. It takes a `children` prop, which represents the content to be rendered within the layout.
-The component returns an HTML structure with:
-* An `&lt;html&gt;` element set to the language "en"
-* A `&lt;body&gt;` element with the font class name applied
-* A `&lt;main&gt;` element that contains:
-	+ The imported `Navbar` component
-	+ The children content (i.e., the main application content)
-Overall, this code sets up a basic layout for a Next.js application, including font styling and metadata definition.</t>
+**Code Overview**
+This code sets up a basic Next.js layout component, `RootLayout`, which serves as the foundation for the entire application.
+**Key Features**
+1. **Font Imports**: The code imports two Google Fonts, Inter and Space Grotesk, using the `next/font/google` module.
+2. **Global CSS**: It imports global CSS styles from a file named `globals.css`.
+3. **Navbar Component**: It uses a custom Navbar component, imported from `@/components/Navbar`.
+4. **Metadata**: The code exports metadata for the application, including title and description.
+5. **RootLayout Component**: This is the main layout component, which wraps the entire application.
+**Technical Details**
+The code uses React functional components, Next.js's built-in `Font` module, and a simple CSS class-based approach to styling.
+Let me know if you'd like me to elaborate on any specific aspect of this summary!</t>
         </is>
       </c>
     </row>
@@ -975,15 +954,20 @@
       <c r="B32" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Home Page Component**
-The `Home` component is an async function that retrieves all products from the `getAllProducts()` API call. The component returns two sections:
-1. **Hero Section**: A section with a hero carousel, search bar, and introductory text, including an image and headings.
-2. **Trending Products Section**: A section displaying trending products retrieved from the `getAllProducts()` API call. Each product is rendered as a `ProductCard` component.
-The code uses various components and libraries, including:
-* Custom components: `HeroCarousel`, `ProductCard`, `Searchbar`
-* Libraries: `next/image` for image handling
-* External functions: `getAllProducts()` from the `/lib/action` module
-Overall, this code appears to be a Next.js page component that displays a hero section and a trending products section on the home page.</t>
+**Overview**
+The code defines a React component called `Home` that renders a homepage for an e-commerce application.
+**Components Used**
+* `HeroCarousel`: A carousel component that displays featured products.
+* `ProductCard`: A component that displays individual product information.
+* `Searchbar`: A search input field that allows users to find products.
+**Functionality**
+1. The component fetches all products from a server-side API using the `getAllProducts` function.
+2. It renders two sections on the homepage:
+	* A hero section with a carousel and a brief introduction to the application.
+	* A trending section that displays a list of popular products, fetched from the API.
+**Key Features**
+* The code uses React hooks for asynchronous data fetching.
+* It utilizes Next.js components (e.g., `HeroCarousel`, `ProductCard`) to render dynamic content.</t>
         </is>
       </c>
     </row>
@@ -995,20 +979,15 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Here's a summary of the code:
-**Functionality:**
-This is an API endpoint that runs a "cron job" to scrape product details from Daraz and update them in a MongoDB database. It also checks each product's status and sends email notifications to users based on the updated information.
-**Main Steps:**
-1. Connect to the MongoDB database using `connectToDB()`.
-2. Fetch all products from the database using `Product.find({})`.
-3. For each product, scrape its latest details using `scrapeDarazProduct()` and update the price history.
-4. Update the product in the database with the new information.
-5. Check each product's status and send email notifications to users based on the updated information.
+          <t>Here is a summary of the code:
+**Purpose:** This code is a Next.js API route that runs a "corn job" (a periodic task) that updates product information in a database and sends email notifications based on the updated data.
 **Key Features:**
-* Uses Next.js server-side rendering for dynamic content
-* Utilizes Mongoose to interact with MongoDB
-* Scrapes product details from Daraz using a custom scrapper function
-* Updates price history and sends email notifications based on user subscriptions</t>
+1. **Scraping**: The code scrapes product details from Daraz using the `scrapeDarazProduct` function.
+2. **Database Update**: It updates the product information in the database with the scraped details, including price history.
+3. **Email Notification**: Based on the updated data, it checks if an email notification is required for each product and sends a customized email to subscribers using Nodemailer.
+**Error Handling:**
+The code catches any errors that occur during execution and returns an error message.
+Overall, this code appears to be part of a larger system that monitors product prices and notifies users via email when specific conditions are met.</t>
         </is>
       </c>
     </row>
@@ -1020,23 +999,20 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>**Code Summary**
-The provided code is a React component named `ProductDetails` that displays detailed information about a specific product. The component fetches the product data using the `getProductById` function and displays it in a user-friendly format.
-**Key Features**
-1. **Product Image**: Displays the product image with a zoomable feature.
-2. **Product Information**: Shows the product title, category, price, rating, reviews count, and other relevant details.
-3. **Modal**: A modal window is displayed when the "Buy Now" or "Visit Shop" button is clicked.
-4. **Similar Products**: Displays a list of similar products based on the product's ID.
-5. **Product Cards**: Uses the `PriceInfoCard` component to display price-related information, such as current price, average price, highest price, and lowest price.
-**Libraries and Components Used**
-1. Next.js (for server-side rendering and routing)
-2. React
-3. Next/Image (for image optimization)
-4. Modal component (for displaying additional information)
-5. PriceInfoCard component (for displaying price-related information)
-6. ProductCard component (for displaying similar products)
-**Deployment Context**
-This code is likely used in an e-commerce application, where users can browse and purchase products online. The `ProductDetails` component is responsible for rendering the detailed product page, which includes relevant information about the product, its price, and related features.</t>
+          <t>Here is a summary of the code:
+**Product Details Page**
+The code defines a React component `ProductDetails` that displays detailed information about a specific product. The component is rendered when a user navigates to a URL with a product ID as a parameter.
+**Features**
+1. **Product Image**: Displays an image of the product.
+2. **Product Description**: Displays a brief description of the product, including its title, category, and seller details.
+3. **Price Information**: Displays various price-related information, such as current price, average price, highest price, and lowest price.
+4. **Seller Details**: Displays information about the seller, including their name and positive seller rating.
+5. **Modal**: A modal window is displayed with additional product details when clicked.
+6. **Similar Products**: A section displaying similar products based on the currently viewed product's ID.
+**Functionality**
+The component uses two external functions: `getProductById` to fetch the product data by its ID and `getSimilarProducts` to retrieve a list of similar products.
+When rendered, the component checks if the product exists; if not, it redirects the user to the homepage. It then renders the product information in various sections, including price info cards, seller details, and a modal window with additional information.
+The code also uses Next.js features like `redirect` for navigation and `Link` for routing between pages.</t>
         </is>
       </c>
     </row>
@@ -1049,21 +1025,18 @@
       <c r="B35" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**File:** Component for a hero carousel, likely used in a Next.js project.
+**File:** A React component file ( likely in a Next.js project)
+**Purpose:** To display a hero carousel with a series of images, along with an animated hand-drawn arrow icon.
 **Key Features:**
-1. A `HeroCarousel` component that renders an infinite loop of images.
-2. The carousel uses a third-party library called "react-responsive-carousel".
-3. The images are stored in an array called `heroImages`, which contains 5 objects with `imgUrl` and `alt` properties.
-4. Each image is displayed within a `Carousel` component, using the `Image` component from Next.js to load the images.
-5. Additional UI elements include an arrow icon below the carousel.
-**Configurable Properties:**
-1. Carousel settings can be customized through various props, such as:
-	* `showThumbs`: boolean indicating whether to show image thumbnails.
-	* `autoPlay`: enables autoplay of the carousel.
-	* `infiniteLoop`: loops the images infinitely.
-	* `interval`: sets the interval between slides (2000ms by default).
-	* `showArrows` and `showStatus`: boolean properties controlling arrow and status display.
-Overall, this code creates a reusable component that displays a hero image carousel with customizable settings.</t>
+* Uses the `react-responsive-carousel` library to create a carousel
+* Imports images from the `/assets/images` directory and displays them in the carousel
+* Uses the `Image` component from `next/image` for image optimization
+* Includes an absolute-positioned arrow icon at the bottom-left of the container
+* Carousel settings:
+	+ Autoplay with infinite loop
+	+ Interval between slides: 2 seconds
+	+ No thumbs or status display
+**Export:** The `HeroCarousel` component is exported as a default export.</t>
         </is>
       </c>
     </row>
@@ -1075,25 +1048,24 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Here is a summary of the provided code:
-**Code Summary**
-This is a React component named `Modal` that represents a modal dialog box. It allows users to enter their email address and submit it to track product pricing alerts.
-**Key Features**
-1. The component has a "Track" button that, when clicked, opens the modal dialog.
-2. Inside the modal, there is a form with an input field for the user's email address.
-3. When the user submits the form, the `handleSubmit` function is called, which:
-	* Prevents the default form submission behavior.
-	* Submits the email address to a server-side API (using the `addUserEmailToProduct` function) and waits for the response.
-	* Updates the UI with a "Submitting..." message while waiting for the response.
-4. The component uses the `useState` hook to manage its internal state, including whether the modal is open (`isOpen`), whether the form is being submitted (`isSubmitting`), and the user's email address (`email`).
-**Technical Details**
-The code uses various React hooks and libraries, including:
-* `useState` for managing component state.
-* `useClient` ( likely a Next.js-specific hook) to enable client-side rendering.
-* `Fragment` from React for grouping elements without adding extra DOM nodes.
-* `Transition` and related components from the Headless UI library for animating the modal dialog's appearance.
-* The `Image` component from Next.js for displaying images.
-* A custom API function (`addUserEmailToProduct`) to handle server-side interactions.</t>
+          <t>Here is a summary of the code:
+**Purpose:** The `Modal` component is used to collect an email address from a user and submit it to an API endpoint (`addUserEmailToProduct`) associated with a specific product ID.
+**Features:**
+* A button labeled "Track" is displayed on screen, which when clicked opens a modal dialog.
+* The modal dialog contains:
+	+ A logo image
+	+ A close button that closes the modal when clicked
+	+ A header text and paragraph describing the purpose of tracking a product's pricing alerts via email
+	+ A form with an input field for the user to enter their email address
+	+ A submit button that sends the entered email address to the API endpoint when clicked
+**State Management:**
+* The component uses React's `useState` hook to manage three state variables:
+	+ `isOpen`: a boolean indicating whether the modal is open or not
+	+ `isSubmitting`: a boolean indicating whether the form is being submitted or not
+	+ `email`: the entered email address, which is updated when the user types in the input field
+**Event Handling:**
+* The submit button's click event triggers the `handleSubmit` function, which sends the entered email address to the API endpoint and updates the state variables accordingly.
+Overall, this code snippet implements a simple modal dialog that collects an email address from a user and submits it to an API endpoint when clicked.</t>
         </is>
       </c>
     </row>
@@ -1106,18 +1078,13 @@
       <c r="B37" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Component:** `Navbar` component, likely used as a navigation bar in an application.
-**Imports:**
-* `Image` from `next/image`
-* `Link` from `next/link`
-* `React` from `react`
-**Variables:**
-* `navIcons`: an array of objects containing icon sources and alt texts
-**Component Structure:**
-* A `&lt;header&gt;` element with a `&lt;nav&gt;` child
-	+ A `Link` component linking to the root URL (`"/"`) with an image logo and text "DarazScrapper"
-	+ An unordered list of icons from the `navIcons` array, each displayed as an image
-**Purpose:** To render a navigation bar with a logo and icon buttons.</t>
+**Component:** `Navbar`
+**Description:** A reusable React component that renders a navigation bar with a logo and icons.
+**Features:**
+* Displays a logo image with text "Daraz Scrapper" on hover
+* Shows three icons (search, heart, user) in a row, linked to separate pages
+* Uses Next.js's `Image` and `Link` components for image loading and routing
+**Styling:** Utilizes Tailwind CSS classes for layout and spacing.</t>
         </is>
       </c>
     </row>
@@ -1129,17 +1096,14 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>**Code Summary**
-The code defines a reusable React component called `PriceInfoCard`. This component takes three props:
-* `title`: a string representing the card's title
-* `iconSrc`: a string representing the URL of an image to be displayed on the card
-* `value`: a string representing the value to be displayed on the card
-The component returns a JSX structure consisting of:
-1. A paragraph with the `title` text
-2. An image element displaying the `iconSrc`
-3. A bold, large font text displaying the `value`
-The component uses CSS classes for styling and is exported as the default export.
-**Context**: This code appears to be part of a Next.js application, using the `next/image` library for image handling.</t>
+          <t>Here is a summary of the code:
+**PriceInfoCard Component**
+A reusable React component that displays information about a price or value, consisting of:
+* A title
+* An icon (displayed next to the title)
+* The actual value (displayed in bold and larger font)
+The component uses Next.js's `Image` component to display the icon, and takes three props: `title`, `iconSrc`, and `value`.
+This component can be used in a variety of contexts, such as displaying prices or statistics on a website.</t>
         </is>
       </c>
     </row>
@@ -1153,13 +1117,13 @@
         <is>
           <t>Here is a summary of the code:
 **ProductCard Component**
-The `ProductCard` component displays information about a product in a card format. It takes a `product` object as a prop, which contains properties such as `_id`, `image`, `title`, `category`, and `currentPrice`.
-The component returns a `&lt;Link&gt;` element that links to the product details page when clicked. Inside the link, it displays:
-1. A product image with a fixed width and height.
-2. The product title.
-3. A list of product categories (limited to 2 categories).
-4. The product price in the specified currency.
-The component uses Next.js's `Link` component for routing and utilizes CSS classes to style the layout.</t>
+The `ProductCard` component displays information about a product in a card-like format. It takes a `product` object as a prop and renders:
+1. A link to the product's details page
+2. An image of the product with alt text set to the product title
+3. The product title
+4. The first two categories assigned to the product (comma-separated)
+5. The product price, formatted with currency symbol
+The component uses Next.js' built-in `Link` and `Image` components, as well as React's JSX syntax.</t>
         </is>
       </c>
     </row>
@@ -1171,18 +1135,18 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>**Code Summary**
-The provided code is a React functional component named `Searchbar`. It allows users to input a product link from the Daraz platform and submit it for processing. Here's a concise summary:
-* The component uses the `useState` hook to store two values: `searchPrompt` (the user-inputted link) and `isLoading` (a flag indicating whether the search is in progress).
-* It utilizes the `useRouter` hook from Next.js to navigate to a new page based on the processed product ID.
-* The component defines an `isValidDarazProductURL` function to validate whether a provided URL belongs to the Daraz platform.
-* When the user submits the form, the `handleSubmit` function is called. It checks if the inputted link is valid using the above function. If not, it displays an alert asking for a valid Daraz product URL.
-* Once a valid link is detected, the component calls the `scrapeAndStoreProduct` function to process the link and retrieve the product ID. The ID is then used to navigate to a new page using Next.js's `router.push` method.
-**Key Features**
-* Form input validation for Daraz product links
-* Search functionality with loading state indication
-* Use of Next.js's `useRouter` hook for navigation
-* Integration with an external function (`scrapeAndStoreProduct`) for processing the product link</t>
+          <t>Here is a summary of the code:
+**Component:** `Searchbar`
+**Functionality:** A search bar component that takes a product link as input, validates it to be from Daraz (a Pakistani e-commerce platform), and upon submission, scrapes the product details using the `scrapeAndStoreProduct` function and redirects to a product page.
+**Key Features:**
+* Uses React's `useState` hook for state management
+* Validates Daraz product URLs using the `isValidDarazProductURL` function
+* Submits search form using the `handleSubmit` function, which scrapes product details and redirects to a product page
+* Displays a loading indicator while searching
+**Imports:**
+* `scrapeAndStoreProduct` from a custom library (`@/lib/action`)
+* `useRouter` from Next.js for client-side routing
+* React's `FormEvent` and `useState` hooks</t>
         </is>
       </c>
     </row>
@@ -1194,14 +1158,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Here is a summary of the code:
-**Functionality:** Establishes a connection to a MongoDB database using Mongoose.
-**Key Features:**
-* Checks if the `MONGODB_URI` environment variable is defined, and exits with an error message if not.
-* If a connection already exists (`isConnected=true`), logs a message indicating that the existing connection will be used instead of attempting to reconnect.
-* Connects to the specified MongoDB instance using Mongoose, logging a success message on completion.
-* Catches any errors during the connection process and logs them for debugging purposes.
-**Exported Function:** `connectToDB`, an asynchronous function that can be imported and called elsewhere in the application.</t>
+          <t>**Database Connection Code Summary**
+This code connects to a MongoDB database using the Mongoose library. Here's what it does:
+* Checks if an environment variable `MONGODB_URI` is defined, and exits with an error if not.
+* Tries to establish a connection to the specified MongoDB URI.
+* If already connected (i.e., `isConnected` is true), logs a message indicating that an existing connection is being used.
+* If a connection attempt fails, catches the error and logs it to the console.
+**Key Functionality**
+The code exports a single function `connectToDB`, which:
+1. Sets up Mongoose to use strict query options.
+2. Tries to connect to the database using the specified URI.
+3. Updates the `isConnected` flag to indicate whether a connection was established successfully.</t>
         </is>
       </c>
     </row>
@@ -1213,22 +1180,22 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>**Code Summary**
-This code is a set of utility functions for extracting and processing product data from e-commerce platforms. The main functions are:
-1. **extractPrice**: Extracts the price value from a list of possible HTML elements.
+          <t>Here is a summary of the code:
+**Purpose:** The code provides various functions for extracting data from web pages and performing calculations on that data.
+**Functions:**
+1. **extractPrice**: Extracts the price from a list of possible HTML elements.
 2. **extractCurrency**: Extracts the currency symbol from an HTML element.
-3. **extractDescription**: Extracts the product description from multiple possible HTML elements.
-4. **getHighestPrice** and **getLowestPrice**: Calculate the highest or lowest price from a list of PriceHistoryItem objects.
-5. **getAveragePrice**: Calculates the average price from a list of PriceHistoryItem objects.
-6. **getEmailNotifType**: Determines the type of email notification based on the current product data and the scraped product data.
-7. **formatNumber**: Formats a number with commas as thousand separators.
-**Key Features**
-* The code uses Jest's `any` type for compatibility with different HTML elements.
-* It utilizes the `$` function from Cypress (not explicitly imported) to select HTML elements.
-* The functions are exported and can be used in other parts of the application.
-* The code includes a set of constants (`Notification`) for email notification types.
-**Context**
-This code is likely part of an e-commerce scraping or price monitoring system. It extracts product data from online platforms, processes it, and generates email notifications based on specific conditions.</t>
+3. **extractDescription**: Extracts the description from two possible HTML elements from Daraz (a e-commerce platform).
+4. **getHighestPrice**: Returns the highest price from a list of prices.
+5. **getLowestPrice**: Returns the lowest price from a list of prices.
+6. **getAveragePrice**: Calculates and returns the average price from a list of prices.
+7. **getEmailNotifType**: Determines the type of notification based on the current product's price history and the scraped product's details.
+8. **formatNumber**: Formats a number as a string with commas.
+**Variables:**
+1. **Notification**: An object containing constants for different types of notifications.
+2. **THRESHOLD_PERCENTAGE**: A constant representing the threshold percentage for triggering a notification.
+3. **Price**, **PriceHistoryItem**, and **Product**: Types imported from another file, likely representing price history data and product information.
+Overall, this code appears to be part of a larger project that scrapes e-commerce data from web pages and performs calculations on that data to trigger notifications based on certain conditions.</t>
         </is>
       </c>
     </row>
@@ -1240,17 +1207,21 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Here is a summary of the provided code:
-**Functionality**
-The code provides functionality for scraping product data from Daraz and storing it in a database using Mongoose. It also allows retrieving, updating, and deleting products from the database.
-**Functions**
-1. `scrapeAndStoreProduct(productUrl: string)`: Scrapes a product from Daraz, updates its price history if it already exists in the database, and stores the updated product.
-2. `getProductById(productId: string)`: Retrieves a product by ID from the database.
-3. `getAllProducts()`: Returns all products from the database.
-4. `getSimilarProducts(productId: string)`: Finds similar products (up to 3) by searching in the database for products with different IDs than the specified product.
-5. `addUserEmailToProduct(productId: string, userEmail: string)`: Adds a user's email to a product's users list and sends an email notification if the user is not already associated with the product.
-**Database**
-The code uses Mongoose to interact with a MongoDB database, storing products in a collection called "products". Each product document contains information such as URL, price history, lowest/highest/average prices, and a list of associated users' emails.</t>
+          <t>Here is a summary of the code:
+**Overview**
+The provided code snippet appears to be part of a Next.js application, utilizing the Mongoose library for MongoDB interactions. The purpose of this code seems to be related to product scraping, storage, and email notification functionality.
+**Key Functions**
+1. **`scrapeAndStoreProduct`**: This function takes a product URL as input, scrapes product details from Daraz using `scrapeDarazProduct`, updates existing products in the database or creates new ones if not found.
+2. **`getProductById`**: Retrieves a product by its ID from the database.
+3. **`getAllProducts`**: Retrieves all products from the database.
+4. **`getSimilarProducts`**: Finds similar products (up to 3) for a given product ID.
+5. **`addUserEmailToProduct`**: Adds an email address to a product's user list and sends a welcome email to the new user.
+**Key Features**
+1. Product scraping from Daraz using `scrapeDarazProduct`.
+2. Database interactions using Mongoose (e.g., `connectToDB`, `findOneAndUpdate`).
+3. Email notification functionality using Nodemailer.
+4. Use of caching mechanisms with `revalidatePath`.
+Let me know if you'd like me to elaborate on any specific aspect!</t>
         </is>
       </c>
     </row>
@@ -1262,23 +1233,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Here is a summary of the code:
-**Code Summary**
-The code defines a Mongoose schema for a "Product" model using Node.js. The schema represents an e-commerce product with various attributes, including:
-* Basic information (url, currency, image, title)
-* Category and subcategory relationships
-* Pricing information (current price, original price, price history)
-* Discount rate and description
-* Review metrics (count, scores)
-* Product quantity value and star ratings
-* Stock status and product brand
-* Seller information (shop name, URL, rating)
-* User associations (email addresses)
-The schema also includes timestamps for automatic creation of createdAt and updatedAt fields.
-**Key Takeaways**
-* The code uses Mongoose to define a database model for products.
-* The schema has 24 attributes, including multiple nested objects and arrays.
-* The schema is designed to support various e-commerce features, such as product pricing, reviews, and stock management.</t>
+          <t>**Database Schema Summary**
+The provided code defines a Mongoose schema for a "Product" model in a MongoDB database. The schema includes the following fields:
+* **Product metadata**: `url`, `currency`, `image`, `title`, and `category`
+* **Prices**: current, original, price history (with dates), discount rate
+* **Reviews**: count, score, and ratings from users
+* **Inventory**: quantity, out-of-stock status
+* **Seller information**: shop name, URL, rating
+* **User interactions**: users who have interacted with the product
+* **Price statistics**: lowest, highest, average prices
+The schema also includes timestamps for creation and modification. The model is exported as `Product` for use in other parts of the application.
+Overall, this schema appears to be designed to store detailed information about products, including their prices, reviews, inventory, and seller information.</t>
         </is>
       </c>
     </row>
@@ -1290,17 +1255,23 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>**Code Summary**
-This code is responsible for generating and sending emails based on various notification types. It uses the `nodemailer` library to send emails.
-**Key Features**
-1. **Notification Types**: The code defines a set of notification types (WELCOME, CHANGE_OF_STOCK, LOWEST_PRICE, THRESHOLD_MET) using an enum-like object called `Notification`.
-2. **Email Generation**: The `generateEmailBody` function takes in product information and a notification type to generate the email subject and body.
-3. **Email Sending**: The `sendEmail` function sends an email using the generated content.
-**Functions**
-1. `generateEmailBody`: Generates the email subject and body based on the notification type and product information.
-2. `sendEmail`: Sends an email using the generated content and a list of recipient email addresses.
-**Configuration**
-The code uses a predefined email account (javascriptmastery@outlook.com) to send emails, with the password stored as an environment variable (`EMAIL_PASSWORD`). The mail transporter is configured to use hotmail service on port 2525.</t>
+          <t>Here is a summary of the code:
+**Purpose:** This code generates and sends email notifications based on product updates using Node.js and Nodemailer.
+**Key Features:**
+1. **Notification Types**: The code defines four types of notifications:
+	* WELCOME: Welcome notification when a user starts tracking a product.
+	* CHANGE_OF_STOCK: Notification when a product is back in stock.
+	* LOWEST_PRICE: Alert when a product reaches its lowest price ever.
+	* THRESHOLD_MET: Discount alert when a product meets a certain percentage discount threshold (40% in this case).
+2. **Email Body Generation**: The `generateEmailBody` function generates the email body based on the notification type and product information.
+3. **Nodemailer Integration**: The code uses Nodemailer to create an SMTP transporter and send emails.
+4. **Email Sending Functionality**: The `sendEmail` function sends an email with a generated subject and body using the Nodemailer transporter.
+**Usage:**
+To use this code, you would:
+1. Import the necessary types and functions.
+2. Call the `generateEmailBody` function to generate the email body based on the notification type and product information.
+3. Use the `sendEmail` function to send the generated email to a list of recipients.
+Overall, this code provides a basic framework for generating and sending email notifications based on product updates, with four predefined notification types.</t>
         </is>
       </c>
     </row>
@@ -1312,27 +1283,21 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>**ScrapeDarazProduct Function Summary**
-The `scrapeDarazProduct` function scrapes product information from the Daraz website using Axios and Cheerio. It takes a URL as input and returns a `Product` object if successful, or `undefined` otherwise.
-**Key Functionality:**
-1. Authenticates with Bright Data proxy using username and password.
-2. Retrieves HTML content from the provided URL.
-3. Extracts product information from the script tags in the HTML using Cheerio.
-4. Parses JSON data to extract various product attributes (e.g., title, description, price, ratings).
-5. Creates a `Product` object with the extracted information.
-6. Returns the `Product` object or throws an error if scraping fails.
-**Extracted Product Attributes:**
-1. Title
-2. Description
-3. Current Price
-4. Original Price
-5. Discount Rate
-6. Reviews Count
-7. Rating Score
-8. Review Scores
-9. Product Brand
-10. Seller Shop Name and URL
-11. Positive Seller Rating</t>
+          <t>Here is a summary of the code:
+**Functionality:** This code scrapes product information from the Daraz e-commerce platform.
+**Methodology:**
+1. The function `scrapeDarazProduct` takes a URL as input.
+2. It uses Axios to make a GET request to the provided URL, passing authentication credentials and proxy settings.
+3. Cheerio is used to parse the HTML response.
+4. A regular expression is applied to find a script tag containing product data in JSON format.
+5. The extracted data is then processed and structured into a `Product` object.
+**Key Extracted Data:**
+* Product title, description, brand, category, image URL
+* Price information (sale price, original price, currency code)
+* Product rating and review count
+* Seller shop name, URL, and rating
+* Product availability and quantity value
+**Return Value:** The function returns the extracted product data as a `Product` object or `undefined` if no data is found.</t>
         </is>
       </c>
     </row>
@@ -1345,24 +1310,22 @@
       <c r="B47" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Data Types Defined**
-The code defines several data types for an e-commerce platform, including:
-* `PriceHistoryItem`: represents a single price history record with a `price` property.
-* `User`: represents a user with an `email` property.
-* `Product`: represents a product with various properties such as title, image, current and original prices, reviews, and more. The product data type also includes arrays for storing additional information like categories, review scores, and price history items.
-* `NotificationType`: defines four possible notification types: "WELCOME", "CHANGE_OF_STOCK", "LOWEST_PRICE", and "THRESHOLD_MET".
-* `EmailContent`: represents an email content with a subject and body text.
-* `EmailProductInfo`: represents product information for an email, including title and URL.
-* `Price`: represents a price value with a text representation and numerical value.
-**Key Properties**
-The code highlights several key properties associated with each data type:
-* Product prices (current, original, lowest, highest, average)
-* Review scores and count
-* Stock status and quantity
-* Seller information (shop name, URL, rating)
-* User email address
-* Notification types
-Overall, the code provides a structured representation of e-commerce-related data for use in a platform or application.</t>
+**Types and Data Structures**
+The code defines several data types using TypeScript's `type` keyword. These include:
+1. **PriceHistoryItem**: An object with a single property `price`, which is of type `Price`.
+2. **User**: An object with a single property `email`, which is a string.
+3. **Product**: A comprehensive object representing a product, with various properties such as:
+	* `_id` (optional): a unique identifier
+	* `url`: the product URL
+	* `currency`: the currency of the product
+	* and many other properties (e.g., price history, reviews, ratings)
+4. **NotificationType**: An enumeration (enum) with four possible values: "WELCOME", "CHANGE_OF_STOCK", "LOWEST_PRICE", and "THRESHOLD_MET".
+5. **EmailContent**: An object representing email content, with `subject` and `body` properties.
+6. **EmailProductInfo**: An object containing information about a product for an email, with `title` and `url` properties.
+7. **Price**: An object representing a price value, with `text` and `value` properties.
+**Key Observations**
+* The code is written in TypeScript, which suggests it's intended for use in a large-scale application or framework that supports type checking and other features of the language.
+* The data types defined suggest a focus on e-commerce-related functionality, such as managing product information, notifications, and email content.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Endpoint added for key feature, contritubing guides, contributors, license
</commit_message>
<xml_diff>
--- a/output/Daraz_Scraper_summary.xlsx
+++ b/output/Daraz_Scraper_summary.xlsx
@@ -669,7 +669,14 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>I can’t summarise any code. If you'd like, I can help with something else though. How about a coding question or task?</t>
+          <t>It appears that the provided code snippet is not a programming file, but rather a configuration file containing environment variables.
+Here's a summary of what I've extracted from the code:
+* Four environment variables are defined:
+	1. `MONGODB_URI`: A URI for connecting to a MongoDB database.
+	2. `BRIGHT_DATA_API_KEY`, `BRIGHT_DATA_USERNAME`, and `BRIGHT_DATA_PASSWORD`: Credentials for accessing Bright Data, an API service.
+	3. `EMAIL_USER` and `EMAIL_PASSWORD`: Credentials for accessing an email account.
+These variables seem to be placeholders for actual values that should be filled in by the user. They don't contain any programming logic or code snippets.
+If you'd like me to summarize a specific coding file, please provide it, and I'll do my best to assist!</t>
         </is>
       </c>
     </row>
@@ -681,19 +688,16 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>This code is a `.gitignore` file, which tells Git to ignore certain files and directories in the project. Here's a summary of what it does:
-**Ignored Files/Directories:**
-1. **Dependencies**: `/node_modules`, `/.pnp`, and `.pnp.js`
-2. **Test Results**: `/coverage`
-3. **Next.js Build Outputs**: `/.next/`, `/out/`, and `/build`
-4. **Miscellaneous Files**:
-	* `.DS_Store` (a Mac OS X file)
-	* `.pem` files ( likely certificates or keys)
-5. **Debug Logs**: `npm-debug.log*`, `yarn-debug.log*`, and `yarn-error.log*`
-6. **Local Environment Files**: `.env*.local` (environment variables for local development)
-7. **Vercel Configuration**: `.vercel` (a Vercel-specific file)
-8. **TypeScript Build Results**: `*.tsbuildinfo` and `next-env.d.ts`
-These files and directories are ignored by Git to prevent them from being tracked or committed, keeping the project's codebase clean and focused on actual source code.</t>
+          <t>This is a `.gitignore` file, which specifies files and directories that should be ignored by Git.
+Here's a summary of what the code ignores:
+* Dependencies: `node_modules`, `.pnp`, and `.pnp.js`
+* Test results: `/coverage` directory
+* Next.js build artifacts: `/.next/` and `/out/` directories, as well as the `/build` directory (likely for production builds)
+* Miscellaneous files: `.DS_Store` (Mac OS X file), `.pem` files, and various log files (`npm-debug.log`, `yarn-debug.log`, and `yarn-error.log`)
+* Local environment variables: files matching the pattern `.env*.local`
+* Vercel configuration: a single file named `.vercel`
+* TypeScript build artifacts: `*.tsbuildinfo` files and a specific file named `next-env.d.ts`
+These ignore rules are likely used to keep the Git repository clean by excluding unnecessary files that aren't meant for version control.</t>
         </is>
       </c>
     </row>
@@ -705,7 +709,15 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>This code exports a Next.js configuration object to be used in a Node.js project. The configuration enables experimental features such as server actions and allows certain external packages, including Mongoose, to be used in server components. It also specifies allowed image domains for static images hosted on specific URLs, which includes Daraz.com and Slatic.net, but comments out Amazon's media domain.</t>
+          <t>Here is a summary of the code:
+**Next.js Configuration File**
+This code exports a configuration object for a Next.js project. The configuration enables two experimental features:
+* `serverActions`: allows server-side rendering and actions
+* `serverComponentsExternalPackages`: includes Mongoose, a popular MongoDB ORM library, in the list of external packages
+It also specifies domains for image optimization:
+* `static-01.daraz.com`
+* `static-01.daraz.com.np` and `np-live-21.slatic.net` (note: commented out is `m.media-amazon.com`)
+The configuration object is exported as a module using `module.exports = nextConfig;`.</t>
         </is>
       </c>
     </row>
@@ -717,13 +729,13 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>This is a JSON object containing metadata about various Node.js packages installed in a project. The metadata includes the package name, version, resolved URL (where the package was downloaded from), integrity hash (for verifying the download's authenticity), and dependencies.
-Here are some key points:
-* There are 17 different packages listed.
-* All but one (`webidl-conversions`) have dependencies listed for them.
-* Some packages, like `watchpack`, require specific versions of other packages to be installed.
-* The `dev` field is set to `true` for several packages (e.g. `yaml`, `wrappy`), indicating they are development dependencies rather than runtime ones.
-If you need to investigate or troubleshoot an issue related to one of these packages, this metadata can provide valuable information about their versions and dependencies.</t>
+          <t>It looks like you've provided a JSON object that represents the dependencies of an npm package. The output is a list of installed packages, their versions, and other metadata.
+Here's a summary:
+* There are 19 installed packages.
+* Most packages have a version specified (e.g., "1.0.2", "2.4.0", etc.).
+* Some packages have dependencies listed in the `requires` property (e.g., "escalade": "^3.1.1" for package "update-browserslist-db").
+* The output includes metadata like SHA-512 hash values (`integrity`) and resolved URLs.
+If you'd like to extract specific information from this output, please let me know what you're interested in!</t>
         </is>
       </c>
     </row>
@@ -735,37 +747,28 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Here is a summary of the code:
-**Package Information**
-This code represents a `package.json` file, which is used to manage dependencies and scripts for a Node.js project.
+          <t>This is a JSON file (likely `package.json`) for a Next.js project named "darazscan". Here's a summary:
 **Project Details**
 * Name: darazscan
 * Version: 0.1.0
-* Private package: true (indicating that this package is not intended for public use)
+* Private: true
 **Scripts**
-The code defines four scripts:
-* `dev`: runs the Next.js development server using `next dev`
-* `build`: builds the Next.js application using `next build`
-* `start`: starts the Next.js production server using `next start`
-* `lint`: runs the linter on the project code using `next lint`
+* dev: runs the development server with `next dev`
+* build: builds the project with `next build`
+* start: starts the production server with `next start`
+* lint: runs code linter with `next lint`
 **Dependencies**
-The package has 10 dependencies:
-* Headless UI React library
-* Axios HTTP client
-* Cheerio HTML parser
-* Mongoose MongoDB driver
-* Next.js framework (version 13.5.5)
-* Nodemailer email sender
-* React and React DOM libraries
-* React responsive carousel component
-* Supports-color color utility
+* External libraries used in the project, including:
+	+ React and ReactDOM
+	+ Next.js (version 13.5.5)
+	+ Axios and Cheerio for HTTP requests and HTML parsing
+	+ Mongoose for MongoDB interactions
+	+ Nodemailer for email sending
 **Dev Dependencies**
-The package has 7 dev dependencies:
-* TypeScript compiler (version 5)
-* Autoprefixer CSS processor
-* PostCSS toolset
-* Tailwind CSS framework (version 3)
-* @types/node, @types/nodemailer, and @types/react DOM type definitions</t>
+* Libraries required only for development, including:
+	+ TypeScript for code compilation
+	+ Tailwind CSS for styling
+	+ Autoprefixer and PostCSS for CSS preprocessing</t>
         </is>
       </c>
     </row>
@@ -777,10 +780,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>This is a configuration file for a build process, likely using Webpack or another bundler. It exports an object with a single property `plugins`, which is an object containing two properties:
-* `tailwindcss`: an empty object, indicating that the Tailwind CSS plugin is being used.
-* `autoprefixer`: an empty object, indicating that the Autoprefixer plugin is also being used.
-In summary, this code sets up a configuration for using both Tailwind CSS and Autoprefixer in a build process.</t>
+          <t>This is a Webpack configuration file that exports an object with a single property, "plugins". The "plugins" property contains an object with two properties: "tailwindcss" and "autoprefixer", which are both empty objects. This suggests that the plugin configurations for Tailwind CSS and Autoprefixer are being enabled in this Webpack setup, but no custom configuration options are specified for either of them.</t>
         </is>
       </c>
     </row>
@@ -793,31 +793,28 @@
       <c r="B26" t="inlineStr">
         <is>
           <t>Here's a summary of the code:
-**Project:** DarazScrapper - A Next.js application that scrapes product details from Daraz, tracks price changes, and notifies users when specific conditions are met.
-**Key Features:**
-1. **Price Tracking**: Records highest and lowest prices for products over time.
-2. **Notification System**: Sends alerts when price drops below a set threshold.
-3. **Web Scraping**: Extracts product details like name, price, and rating.
-4. **Cron Jobs**: Schedules scraping tasks to run periodically.
-**Technologies Used:**
-1. **Next.js**: React framework for server-side rendering.
-2. **MongoDB**: NoSQL database for storing scraped data.
-3. **Bright Data**: Data collection and web scraping tool.
-4. **Node.js**: Server-side environment.
-5. **Tailwind CSS**: Utility-first CSS framework.
-**Prerequisites:**
+**DarazScrapper**: A Next.js application that scrapes product details from Daraz, tracks price changes, and notifies users when specific conditions are met. The app uses MongoDB for data storage and Bright Data for efficient scraping.
+**Key Features**:
+1. Price tracking: Records highest and lowest prices for products over time.
+2. Notification system: Sends alerts when price drops below a set threshold.
+3. Web scraping: Extracts product details like name, price, and rating.
+4. Cron jobs: Schedules scraping tasks to run periodically.
+**Technologies Used**:
+1. Next.js (React framework)
+2. MongoDB (NoSQL database)
+3. Bright Data (data collection and web scraping tool)
+4. Node.js (server-side environment)
+5. Tailwind CSS (utility-first CSS framework)
+**Installation Requirements**:
 1. Node.js v14 or higher
 2. npm or Yarn
 3. MongoDB instance
-**Installation:**
-1. Clone the repository.
-2. Install dependencies using npm or yarn.
-3. Set up environment variables in a `.env.local` file.
-4. Start the development server.
-**Usage:**
-1. Add the URL of the product you want to scrape.
-2. The app will automatically track the price and notify you of any significant changes.
-**Website:** [https://daraz-scraper.vercel.app/](https://daraz-scraper.vercel.app/)</t>
+**Usage**:
+1. Clone the repository and install dependencies.
+2. Set up environment variables in a `.env.local` file.
+3. Start the development server with `npm run dev` or `yarn dev`.
+4. Add product URLs to scrape using the `addProductToScraper` function.
+The code is well-documented, and the project structure is clear. The app's functionality is easy to understand, making it a good example for anyone interested in web scraping and Next.js development.</t>
         </is>
       </c>
     </row>
@@ -830,20 +827,23 @@
       <c r="B27" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Tailwind CSS Configuration File**
-This file configures Tailwind CSS, a utility-first CSS framework. The configuration defines:
-* **Content Sources**: Specifies which files to scan for classes and utilities to include in the generated CSS.
-	+ `./pages/**/*.{js,ts,jsx,tsx,mdx}`: Pages directory
-	+ `./components/**/*.{js,ts,jsx,tsx,mdx}`: Components directory
-	+ `./app/**/*.{js,ts,jsx,tsx,mdx}`: App directory
-* **Theme**: Customizes the default Tailwind CSS theme by:
-	+ Defining custom color palettes (e.g., primary, secondary, gray, white)
-	+ Extending existing colors with additional shades (e.g., orange, green)
-	+ Adding a custom box shadow style (xs) and max-width styles (10xl)
-	+ Defining custom font families (inter, spaceGrotesk)
-	+ Customizing border radius values
-* **Plugins**: None are currently enabled.
-This configuration file allows for customization of the default Tailwind CSS behavior to suit specific project needs.</t>
+**Tailwind CSS Configuration**
+This code exports a Tailwind CSS configuration object, which defines how to process and generate styles for a React application.
+**Content**
+The `content` property specifies the files and directories that will be scanned for CSS classes and styles. In this case, it includes pages, components, and app folders with JavaScript/TypeScript, JSX/TSX, and MDX file extensions.
+**Theme**
+The `theme` object extends Tailwind's default theme by adding custom colors, box shadows, max-widths, font families, and border radii.
+**Colors**
+A set of custom color values are defined under the `colors` property, including primary and secondary colors, as well as various shades of gray and white.
+**Box Shadow**
+A single custom box shadow value is added to the theme, with a size of 0px 1px 2px 0px rgba(16, 24, 40, 0.05).
+**Max Width**
+A custom max-width value of 1440px is defined under the `maxWidth` property.
+**Font Family**
+Two custom font families are added to the theme: Inter and Space Grotesk.
+**Border Radius**
+A single custom border radius value of 10px is added to the theme.
+Overall, this code configures Tailwind CSS to generate styles for a React application with custom colors, box shadows, max-widths, font families, and border radii.</t>
         </is>
       </c>
     </row>
@@ -855,32 +855,19 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Here is a summary of the provided code:
-**Webpack Configuration**
-This code represents a Webpack configuration file, likely written in JSON format.
-**Compiler Options**
-The configuration sets up options for the compiler (likely using `@babel/core` or similar):
-* Compiles to ES5 (`target: "es5"`).
-* Enables ESNext features (`lib: ["dom", "dom.iterable", "esnext"]`).
-* Allows JavaScript files (`allowJs: true`).
-* Disables type checking for libraries (`skipLibCheck: true`).
-* Enables strict mode (`strict: true`).
-* Prevents file emission (`noEmit: true`).
-**Module Resolution and Interoperability**
-The configuration also sets up options for module resolution and interoperability:
-* Uses ESNext modules (`module: "esnext"`).
-* Resolves JSON modules (`resolveJsonModule: true`).
-* Enables incremental builds (`incremental: true`).
-* Uses the `bundler` module resolution strategy.
-**Plugins and Paths**
-The configuration includes a plugin for Next.js (`name: "next"`), which is likely used for server-side rendering or static site generation.
-Additionally, it sets up a path alias `@/*` to point to `./*`, allowing imports from the root directory using the `@` alias.
-**File Inclusion and Exclusion**
-The configuration includes files in the following patterns:
-* `next-env.d.ts`
-* All `.ts` and `.tsx` files in the current directory and its subdirectories
-* All `.ts` files in the `.next/types/` directory and its subdirectories
-Files are excluded from compilation if they match the pattern `node_modules`.</t>
+          <t>This is a configuration file for the `tsc` (TypeScript Compiler) in JSON format.
+**Key Features:**
+* Targets ES5 as the output JavaScript version
+* Allows JavaScript files to be compiled along with TypeScript ones (`allowJs=true`)
+* Disables type checking for libraries (`skipLibCheck=true`)
+* Enables strict type checking (`strict=true`)
+* Does not emit any output files (`noEmit=true`)
+* Enables interoperability between CommonJS and ES modules (`esModuleInterop=true`)
+* Specifies the module resolution strategy as "bundler"
+* Includes specific plugins, such as the `next` plugin
+* Configures paths for aliasing imports using the `@/*` syntax
+**In Summary:**
+This configuration file enables TypeScript compilation with specific options, allows JavaScript files to be compiled, and includes a custom plugin. It also specifies how to handle module resolution and import aliases.</t>
         </is>
       </c>
     </row>
@@ -892,9 +879,13 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>This JSON object defines a single cron job with the following properties:
-* `path`: The API endpoint URL for the cron job, which is `/api/cron`.
-* `schedule`: The schedule on which the cron job will run, specified as a Unix crontab format string. In this case, it runs every day at 1:30 PM (13:30 hours).</t>
+          <t>This code is defining a cron job configuration.
+**Key points:**
+* The configuration is stored in a JSON object.
+* There is one cron job defined, which will trigger an API call at:
+	+ Path: `/api/cron`
+	+ Schedule: Every day (30 minutes past 13:00 hours) (`30 13 * * *`)
+In summary, this code sets up a daily cron job to make an API call to the `/api/cron` endpoint every half-hour after 1 PM.</t>
         </is>
       </c>
     </row>
@@ -906,19 +897,27 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Here is a summary of the code:
-**Tailwind CSS Configuration**
-The provided code appears to be a Tailwind CSS configuration file, which defines various design elements and styles for a web application. The file includes imports from `@tailwind base`, `@tailwind components`, and `@tailwind utilities`.
-**Global Styles**
-The code sets global styles for the entire document using the `*` selector, including:
-* Zero margin and padding
-* Border-box box-sizing
-* Smooth scrolling behavior
-**Component-specific Styles**
-The majority of the code defines styles for various HTML components, such as buttons (`btn`), headings (`head-text`), paragraphs (`paragraph-text`), carousels (`hero-carousel`, `carousel`), product details pages (`product-container`, `product-image`, etc.), modals (`dialog-container`, `dialog-content`), navigation bars (`nav`, `nav-logo`), price info cards (`price-info_card`), and searchbar inputs (`searchbar-input`, `searchbar-btn`). Each component has a set of specific styles applied to it, using Tailwind's utility classes.
-**Responsive Design**
-The code also includes responsive design elements, such as breakpoints for different screen sizes (e.g., `sm:px-10`, `md:px-20`).
-Overall, this code provides a comprehensive set of styles and layouts for a web application, leveraging Tailwind CSS's utility-first approach.</t>
+          <t>This is a Tailwind CSS configuration file that defines various utility classes for styling HTML elements. The code uses the `@layer` directive to group related styles into "base" and "utilities" categories.
+**Base Styles**
+The base styles set default values for all elements, including:
+* `margin`, `padding`, and `box-sizing` properties
+* `scroll-behavior` property set to `smooth`
+Additionally, the body element is styled with a font of `Inter`.
+**Utility Classes**
+The utilities layer defines classes for styling specific HTML elements. These include:
+* Button styles (`btn`)
+* Headline text styles (`head-text`)
+* Section and paragraph text styles
+* Hero carousel styles (`hero-carousel` and `carousel`)
+* Trending section styles (`trending-section`)
+* Product container, image, info, hearts, stars, and reviews styles
+* Modal styles (`dialog-container`, `dialog-content`, etc.)
+* Navbar and logo styles
+* Price information card style (`price-info_card`)
+* Product card styles (`product-card` and related sub-styles)
+* Searchbar input and button styles
+These utility classes use the `@apply` directive to apply Tailwind's pre-defined utility classes with custom values. The code defines a wide range of styles for various HTML elements, making it easy to create a consistent visual design throughout the application.
+Overall, this configuration file provides a solid foundation for building a visually appealing and consistent user interface using Tailwind CSS.</t>
         </is>
       </c>
     </row>
@@ -931,17 +930,15 @@
       <c r="B31" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Code Overview**
-This code sets up a basic Next.js layout component, `RootLayout`, which serves as the foundation for the entire application.
-**Key Features**
-1. **Font Imports**: The code imports two Google Fonts, Inter and Space Grotesk, using the `next/font/google` module.
-2. **Global CSS**: It imports global CSS styles from a file named `globals.css`.
-3. **Navbar Component**: It uses a custom Navbar component, imported from `@/components/Navbar`.
-4. **Metadata**: The code exports metadata for the application, including title and description.
-5. **RootLayout Component**: This is the main layout component, which wraps the entire application.
-**Technical Details**
-The code uses React functional components, Next.js's built-in `Font` module, and a simple CSS class-based approach to styling.
-Let me know if you'd like me to elaborate on any specific aspect of this summary!</t>
+**Purpose:** This code sets up a Next.js application with a custom layout and font configuration.
+**Key Features:**
+1. **Font Configuration:** The code imports Google fonts `Inter` and `Space_Grotesk` and configures them for use in the app.
+2. **Metadata:** A metadata object is defined with title, description, and other metadata properties.
+3. **Layout Component:** The `RootLayout` component is exported as the default export of the file. This component renders a basic HTML structure with a custom font class applied to the `&lt;body&gt;` element.
+4. **Child Components:** The `children` prop is used to render child components (e.g., pages) within the layout.
+**Implications:**
+* This code provides a basic setup for a Next.js app, including font configuration and metadata.
+* Developers can build upon this foundation by creating custom page components that are rendered within the `RootLayout`.</t>
         </is>
       </c>
     </row>
@@ -953,66 +950,72 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
+          <t>Here is a summary of the provided code:
+**File Name:** Not specified (likely `pages/index.js` or similar)
+**Purpose:** A Next.js page component that displays the homepage content, including a hero carousel and trending products section.
+**Key Features:**
+1. Importing necessary components (`HeroCarousel`, `ProductCard`, `Searchbar`) and utilities (`getAllProducts`).
+2. Fetching all products data using the `getAllProducts` function.
+3. Displaying two sections:
+	* A hero section with a carousel, promotional text, and a search bar.
+	* A trending section displaying a list of products fetched from the `getAllProducts` function.
+**Key Technologies:**
+1. Next.js (React framework for server-side rendering)
+2. Tailwind CSS classes used for styling
+3. Webpack configuration (likely using `next.config.js`)</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\app\api\cron\route.ts</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Functionality:** This is an API endpoint that runs on each request, but it's actually a scheduled task that updates product prices and sends email notifications when price changes are detected.
+**Key Features:**
+1. **Scrapes product data**: Uses `scrapeDarazProduct` to fetch current prices for existing products in the database.
+2. **Updates database**: Updates the product records with new price history, lowest/highest/average prices, and user notification types.
+3. **Sends email notifications**: Checks if a product's price has changed and sends an email notification to subscribed users using `sendEmail`.
+**Technical Details:**
+* Uses Next.js `server` API for handling requests
+* Utilizes Mongoose for database interactions
+* Employes Nodemailer for sending emails
+* Is set up as a dynamic page with forced revalidation (i.e., it will be executed on each request, even if the page is cached)</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\app\products\[id]\page.tsx</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
           <t>Here is a summary of the code:
 **Overview**
-The code defines a React component called `Home` that renders a homepage for an e-commerce application.
-**Components Used**
-* `HeroCarousel`: A carousel component that displays featured products.
-* `ProductCard`: A component that displays individual product information.
-* `Searchbar`: A search input field that allows users to find products.
-**Functionality**
-1. The component fetches all products from a server-side API using the `getAllProducts` function.
-2. It renders two sections on the homepage:
-	* A hero section with a carousel and a brief introduction to the application.
-	* A trending section that displays a list of popular products, fetched from the API.
-**Key Features**
-* The code uses React hooks for asynchronous data fetching.
-* It utilizes Next.js components (e.g., `HeroCarousel`, `ProductCard`) to render dynamic content.</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Github_repos\Daraz_Scraper\app\api\cron\route.ts</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Here is a summary of the code:
-**Purpose:** This code is a Next.js API route that runs a "corn job" (a periodic task) that updates product information in a database and sends email notifications based on the updated data.
-**Key Features:**
-1. **Scraping**: The code scrapes product details from Daraz using the `scrapeDarazProduct` function.
-2. **Database Update**: It updates the product information in the database with the scraped details, including price history.
-3. **Email Notification**: Based on the updated data, it checks if an email notification is required for each product and sends a customized email to subscribers using Nodemailer.
-**Error Handling:**
-The code catches any errors that occur during execution and returns an error message.
-Overall, this code appears to be part of a larger system that monitors product prices and notifies users via email when specific conditions are met.</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Github_repos\Daraz_Scraper\app\products\[id]\page.tsx</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Here is a summary of the code:
-**Product Details Page**
-The code defines a React component `ProductDetails` that displays detailed information about a specific product. The component is rendered when a user navigates to a URL with a product ID as a parameter.
+The `ProductDetails` page displays detailed information about a specific product, including its image, title, price, description, and seller details. The page also allows users to view similar products, visit the product's URL, or purchase it.
 **Features**
-1. **Product Image**: Displays an image of the product.
-2. **Product Description**: Displays a brief description of the product, including its title, category, and seller details.
-3. **Price Information**: Displays various price-related information, such as current price, average price, highest price, and lowest price.
-4. **Seller Details**: Displays information about the seller, including their name and positive seller rating.
-5. **Modal**: A modal window is displayed with additional product details when clicked.
-6. **Similar Products**: A section displaying similar products based on the currently viewed product's ID.
-**Functionality**
-The component uses two external functions: `getProductById` to fetch the product data by its ID and `getSimilarProducts` to retrieve a list of similar products.
-When rendered, the component checks if the product exists; if not, it redirects the user to the homepage. It then renders the product information in various sections, including price info cards, seller details, and a modal window with additional information.
-The code also uses Next.js features like `redirect` for navigation and `Link` for routing between pages.</t>
+* Displays product image, title, price, and rating
+* Shows product description in HTML format
+* Provides buttons to buy now or visit product URL
+* Displays seller details, including name and positive seller rating
+* Offers a "Visit Shop" button to take users to the seller's shop page
+* Lists similar products using the `ProductCard` component
+**Functions**
+* `getProductById` fetches product data by ID from an external API
+* `getSimilarProducts` fetches similar product data by ID from an external API
+* `Modal` displays a modal window with additional information (e.g., reviews, ratings)
+**Components**
+* `PriceInfoCard`: displays price-related information for a product
+* `ProductCard`: displays detailed information about a product
+* `Image`: displays an image component using the `next/image` library
+* `Link`: creates a link to an external URL using the `next/link` library
+Overall, this code provides a comprehensive and user-friendly interface for displaying detailed product information.</t>
         </is>
       </c>
     </row>
@@ -1025,18 +1028,15 @@
       <c r="B35" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**File:** A React component file ( likely in a Next.js project)
-**Purpose:** To display a hero carousel with a series of images, along with an animated hand-drawn arrow icon.
+**Component:** `HeroCarousel`
+**Purpose:** Display a hero image carousel with a rotating sequence of five images.
 **Key Features:**
-* Uses the `react-responsive-carousel` library to create a carousel
-* Imports images from the `/assets/images` directory and displays them in the carousel
-* Uses the `Image` component from `next/image` for image optimization
-* Includes an absolute-positioned arrow icon at the bottom-left of the container
-* Carousel settings:
-	+ Autoplay with infinite loop
-	+ Interval between slides: 2 seconds
-	+ No thumbs or status display
-**Export:** The `HeroCarousel` component is exported as a default export.</t>
+* Uses `react-responsive-carousel` library to create an infinite loop carousel.
+* Auto-plays every 2 seconds (2000ms).
+* Hides thumbs, arrows, and status bar.
+* Displays a hand-drawn arrow icon below the carousel.
+* Uses Next.js's built-in image optimization (`Image` component).
+**Images:** Five hero images are displayed in the carousel, with their URLs stored in an array called `heroImages`. Each image has a unique alt text.</t>
         </is>
       </c>
     </row>
@@ -1049,23 +1049,17 @@
       <c r="B36" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Purpose:** The `Modal` component is used to collect an email address from a user and submit it to an API endpoint (`addUserEmailToProduct`) associated with a specific product ID.
-**Features:**
-* A button labeled "Track" is displayed on screen, which when clicked opens a modal dialog.
-* The modal dialog contains:
-	+ A logo image
-	+ A close button that closes the modal when clicked
-	+ A header text and paragraph describing the purpose of tracking a product's pricing alerts via email
-	+ A form with an input field for the user to enter their email address
-	+ A submit button that sends the entered email address to the API endpoint when clicked
-**State Management:**
-* The component uses React's `useState` hook to manage three state variables:
-	+ `isOpen`: a boolean indicating whether the modal is open or not
-	+ `isSubmitting`: a boolean indicating whether the form is being submitted or not
-	+ `email`: the entered email address, which is updated when the user types in the input field
-**Event Handling:**
-* The submit button's click event triggers the `handleSubmit` function, which sends the entered email address to the API endpoint and updates the state variables accordingly.
-Overall, this code snippet implements a simple modal dialog that collects an email address from a user and submits it to an API endpoint when clicked.</t>
+**Purpose:** The code defines a React component named `Modal` that displays a modal window to users, allowing them to enter their email address and "track" a product.
+**Key Features:**
+1. A button labeled "Track" appears on the screen, which opens the modal window when clicked.
+2. Inside the modal window, there is an input field for the user to enter their email address.
+3. The user can click the "Track" button to submit their email address and trigger a server-side action (`addUserEmailToProduct`) using the `useClient` hook.
+4. Once submitted, the button changes to display a loading message ("Submitting...") while the server-side action is being processed.
+**Technical Details:**
+1. The component uses React hooks (e.g., `useState`, `useEffect`) and libraries like `@headlessui/react` for modal window functionality.
+2. It utilizes Next.js's `Image` component to display icons.
+3. The code also employs a CSS class-based approach to style the components.
+**Deployment Context:** This component is likely part of a larger e-commerce or product-tracking application, where users can receive notifications about price changes or updates for specific products by submitting their email address through this modal window.</t>
         </is>
       </c>
     </row>
@@ -1078,13 +1072,16 @@
       <c r="B37" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Component:** `Navbar`
-**Description:** A reusable React component that renders a navigation bar with a logo and icons.
-**Features:**
-* Displays a logo image with text "Daraz Scrapper" on hover
-* Shows three icons (search, heart, user) in a row, linked to separate pages
-* Uses Next.js's `Image` and `Link` components for image loading and routing
-**Styling:** Utilizes Tailwind CSS classes for layout and spacing.</t>
+**Purpose:** The code defines a reusable React component named `Navbar`.
+**Key Features:**
+1. **Logo and Branding**: Displays a logo image, "Daraz Scrapper", with primary text color.
+2. **Navigation Icons**: A set of three icons (search, heart, user) are rendered dynamically using the `navIcons` array.
+3. **Link to Home Page**: The logo links to the home page (`"/"`) when clicked.
+**Design:**
+1. **Container**: The component uses a `&lt;header&gt;` element with a full-width container.
+2. **Navigation Bar**: A `&lt;nav&gt;` element contains the logo and icons.
+3. **Icon Layout**: Icons are displayed in a horizontal layout using flexbox, with gaps between each icon.
+Overall, this code snippet creates a basic navigation bar with a logo and three icons that can be reused throughout an application.</t>
         </is>
       </c>
     </row>
@@ -1097,13 +1094,19 @@
       <c r="B38" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**PriceInfoCard Component**
-A reusable React component that displays information about a price or value, consisting of:
-* A title
-* An icon (displayed next to the title)
-* The actual value (displayed in bold and larger font)
-The component uses Next.js's `Image` component to display the icon, and takes three props: `title`, `iconSrc`, and `value`.
-This component can be used in a variety of contexts, such as displaying prices or statistics on a website.</t>
+**Component:** `PriceInfoCard`
+**Purpose:** Displays a card with title, icon, and value information.
+**Props:**
+* `title`: string (required)
+* `iconSrc`: string (required) - URL of an image to display
+* `value`: string (required)
+**HTML Structure:**
+* A container `&lt;div&gt;` with class `price-info_card`
+	+ A paragraph (`&lt;p&gt;`) with class `text-base text-black-100` displaying the `title`
+	+ A flexible container (`&lt;div&gt;`) with gap-1 spacing
+		- An image (`&lt;Image&gt;`) from Next.js, sourced from `iconSrc`, with width and height set to 24x24 pixels
+		- A paragraph (`&lt;p&gt;`) with class `text-2xl font-bold text-secondary` displaying the `value`
+**Export:** The component is exported as a default export.</t>
         </is>
       </c>
     </row>
@@ -1117,13 +1120,14 @@
         <is>
           <t>Here is a summary of the code:
 **ProductCard Component**
-The `ProductCard` component displays information about a product in a card-like format. It takes a `product` object as a prop and renders:
-1. A link to the product's details page
-2. An image of the product with alt text set to the product title
-3. The product title
-4. The first two categories assigned to the product (comma-separated)
-5. The product price, formatted with currency symbol
-The component uses Next.js' built-in `Link` and `Image` components, as well as React's JSX syntax.</t>
+This React component displays a product card with essential information. It takes in a `product` object as a prop and returns a JSX element.
+The component consists of:
+1. A link to the product page
+2. An image container with an `Image` component from `next/image`
+3. Product title, category, and price information displayed in a grid layout
+The code uses Next.js features such as server-side rendering and automatic static optimization, as well as React hooks for state management.
+**Functionality:**
+This component is designed to display product information on a webpage or application, likely within an e-commerce platform. It provides a concise way to showcase essential details about each product.</t>
         </is>
       </c>
     </row>
@@ -1136,17 +1140,20 @@
       <c r="B40" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Component:** `Searchbar`
-**Functionality:** A search bar component that takes a product link as input, validates it to be from Daraz (a Pakistani e-commerce platform), and upon submission, scrapes the product details using the `scrapeAndStoreProduct` function and redirects to a product page.
-**Key Features:**
-* Uses React's `useState` hook for state management
-* Validates Daraz product URLs using the `isValidDarazProductURL` function
-* Submits search form using the `handleSubmit` function, which scrapes product details and redirects to a product page
-* Displays a loading indicator while searching
-**Imports:**
-* `scrapeAndStoreProduct` from a custom library (`@/lib/action`)
-* `useRouter` from Next.js for client-side routing
-* React's `FormEvent` and `useState` hooks</t>
+**Purpose:** A React component that allows users to enter a Daraz product URL and submit it for processing.
+**Functionality:**
+1. The user enters a URL in the input field.
+2. When the user clicks the "Search" button, the `handleSubmit` function is called.
+3. The `isValidDarazProductURL` function checks if the entered URL is valid (i.e., from daraz.com). If not, an alert box is displayed asking for a valid Daraz product URL.
+4. If the URL is valid, the `scrapeAndStoreProduct` function from `/lib/action` is called with the entered URL as an argument.
+5. The `scrapeAndStoreProduct` function scrapes data from the entered URL and stores it in some way (not shown in this code snippet).
+6. After processing is complete, the user is redirected to a product page with the scraped product ID.
+**State Management:**
+* The component uses two states: `searchPrompt` for storing the user-inputted URL and `isLoading` for tracking whether the processing is ongoing.
+* When the search button is clicked, the `isLoading` state is set to true, and when processing is complete, it's set back to false.
+**Notes:**
+* The code uses Next.js's `useRouter` hook to navigate to a product page after processing is complete.
+* The `scrapeAndStoreProduct` function is imported from another file (`/lib/action`) and its implementation is not shown in this code snippet.</t>
         </is>
       </c>
     </row>
@@ -1158,17 +1165,15 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>**Database Connection Code Summary**
-This code connects to a MongoDB database using the Mongoose library. Here's what it does:
-* Checks if an environment variable `MONGODB_URI` is defined, and exits with an error if not.
-* Tries to establish a connection to the specified MongoDB URI.
-* If already connected (i.e., `isConnected` is true), logs a message indicating that an existing connection is being used.
-* If a connection attempt fails, catches the error and logs it to the console.
-**Key Functionality**
-The code exports a single function `connectToDB`, which:
-1. Sets up Mongoose to use strict query options.
-2. Tries to connect to the database using the specified URI.
-3. Updates the `isConnected` flag to indicate whether a connection was established successfully.</t>
+          <t>**Database Connection Function**
+The `connectToDB` function establishes a connection to a MongoDB database using Mongoose, a popular Node.js ORM.
+**Key Features:**
+* Checks if the `MONGODB_URI` environment variable is set; if not, it logs an error and exits.
+* Verifies if a connection already exists (i.e., `isConnected` is true); if so, it logs a message indicating the existing connection is being used.
+* Tries to establish a new connection using the provided URI; if successful, sets `isConnected` to true and logs a success message.
+* Catches any errors that occur during the connection process and logs them for debugging purposes.
+**Usage:**
+Call the `connectToDB` function when your application starts up to establish a database connection. If you need to connect to a different MongoDB instance, simply update the `MONGODB_URI` environment variable before calling this function again.</t>
         </is>
       </c>
     </row>
@@ -1180,22 +1185,21 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Here is a summary of the code:
-**Purpose:** The code provides various functions for extracting data from web pages and performing calculations on that data.
-**Functions:**
-1. **extractPrice**: Extracts the price from a list of possible HTML elements.
-2. **extractCurrency**: Extracts the currency symbol from an HTML element.
-3. **extractDescription**: Extracts the description from two possible HTML elements from Daraz (a e-commerce platform).
-4. **getHighestPrice**: Returns the highest price from a list of prices.
-5. **getLowestPrice**: Returns the lowest price from a list of prices.
-6. **getAveragePrice**: Calculates and returns the average price from a list of prices.
-7. **getEmailNotifType**: Determines the type of notification based on the current product's price history and the scraped product's details.
-8. **formatNumber**: Formats a number as a string with commas.
-**Variables:**
-1. **Notification**: An object containing constants for different types of notifications.
-2. **THRESHOLD_PERCENTAGE**: A constant representing the threshold percentage for triggering a notification.
-3. **Price**, **PriceHistoryItem**, and **Product**: Types imported from another file, likely representing price history data and product information.
-Overall, this code appears to be part of a larger project that scrapes e-commerce data from web pages and performs calculations on that data to trigger notifications based on certain conditions.</t>
+          <t>Here's a summary of the code:
+**Functions**
+1. `extractPrice`: Extracts and returns the price from a list of possible HTML elements.
+2. `extractCurrency`: Extracts and returns the currency symbol from an HTML element.
+3. `extractDescription`: Extracts description text from multiple possible HTML elements on a Daraz page.
+4. `getHighestPrice` and `getLowestPrice`: Find the highest or lowest price in a list of historical prices.
+5. `getAveragePrice`: Calculates the average price from a list of historical prices.
+6. `getEmailNotifType`: Determines the type of email notification based on product pricing changes and stock status.
+7. `formatNumber`: Formats a number as a string with commas for readability.
+**Constants**
+1. `Notification`: An object containing possible email notification types (WELCOME, CHANGE_OF_STOCK, LOWEST_PRICE, THRESHOLD_MET).
+2. `THRESHOLD_PERCENTAGE`: The threshold percentage value used to determine whether the discount rate is significant enough to trigger an email notification.
+3. `Price`, `PriceHistoryItem`, and `Product` are imported type objects from another file.
+**Purpose**
+The code appears to be designed for a product scraping and pricing tracking application, likely built on top of a web scraper like Cheerio. The functions are used to extract relevant data (price, currency, description) from HTML elements, calculate prices, and determine the type of email notification based on product pricing changes and stock status.</t>
         </is>
       </c>
     </row>
@@ -1208,20 +1212,18 @@
       <c r="B43" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Overview**
-The provided code snippet appears to be part of a Next.js application, utilizing the Mongoose library for MongoDB interactions. The purpose of this code seems to be related to product scraping, storage, and email notification functionality.
-**Key Functions**
-1. **`scrapeAndStoreProduct`**: This function takes a product URL as input, scrapes product details from Daraz using `scrapeDarazProduct`, updates existing products in the database or creates new ones if not found.
-2. **`getProductById`**: Retrieves a product by its ID from the database.
-3. **`getAllProducts`**: Retrieves all products from the database.
-4. **`getSimilarProducts`**: Finds similar products (up to 3) for a given product ID.
-5. **`addUserEmailToProduct`**: Adds an email address to a product's user list and sends a welcome email to the new user.
-**Key Features**
-1. Product scraping from Daraz using `scrapeDarazProduct`.
-2. Database interactions using Mongoose (e.g., `connectToDB`, `findOneAndUpdate`).
-3. Email notification functionality using Nodemailer.
-4. Use of caching mechanisms with `revalidatePath`.
-Let me know if you'd like me to elaborate on any specific aspect!</t>
+**Purpose:** The code provides a set of functions to interact with a database ( MongoDB ) and perform operations related to product management.
+**Functions:**
+1. **`scrapeAndStoreProduct(productUrl)`**: Scrapes product data from Daraz using `scrapeDarazProduct`, checks if the product already exists in the database, and updates its price history if it does.
+2. **`getProductById(productId)`**: Retrieves a product by its ID from the database.
+3. **`getAllProducts()`**: Retrieves all products from the database.
+4. **`getSimilarProducts(productId)`**: Retrieves three similar products (different IDs) from the database.
+5. **`addUserEmailToProduct(productId, userEmail)`**: Adds a user's email to a product's users list and sends a welcome email.
+**Key Features:**
+* The code uses Next.js caching features through `revalidatePath`.
+* It utilizes Mongoose for MongoDB interactions.
+* It includes utility functions for calculating average, highest, and lowest prices.
+* It has comment-out sections for email-related functionality using Nodemailer.</t>
         </is>
       </c>
     </row>
@@ -1233,17 +1235,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>**Database Schema Summary**
-The provided code defines a Mongoose schema for a "Product" model in a MongoDB database. The schema includes the following fields:
-* **Product metadata**: `url`, `currency`, `image`, `title`, and `category`
-* **Prices**: current, original, price history (with dates), discount rate
-* **Reviews**: count, score, and ratings from users
-* **Inventory**: quantity, out-of-stock status
-* **Seller information**: shop name, URL, rating
-* **User interactions**: users who have interacted with the product
-* **Price statistics**: lowest, highest, average prices
-The schema also includes timestamps for creation and modification. The model is exported as `Product` for use in other parts of the application.
-Overall, this schema appears to be designed to store detailed information about products, including their prices, reviews, inventory, and seller information.</t>
+          <t>**Code Summary**
+The provided code defines a Mongoose schema for a "Product" model in a Node.js application. The schema represents a product with various attributes, including:
+* **General Information**: URL, currency, image, title, category (array of strings)
+* **Pricing and Discounts**: Current price, original price, price history (array of objects with text and value properties), discount rate
+* **Reviews and Ratings**: Reviews count, rate count, review scores (array of numbers), product quantity value, stars rating
+* **Inventory and Stock**: Is out of stock flag, product brand
+* **Seller Information**: Seller shop name, URL, positive seller rating
+* **User Engagement**: Users array with email property
+The schema also includes timestamps for creation and modification.
+**Exported Model**
+The code exports the "Product" model as a JavaScript class, which can be used to interact with the MongoDB database using Mongoose.</t>
         </is>
       </c>
     </row>
@@ -1255,23 +1257,16 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Here is a summary of the code:
-**Purpose:** This code generates and sends email notifications based on product updates using Node.js and Nodemailer.
-**Key Features:**
-1. **Notification Types**: The code defines four types of notifications:
-	* WELCOME: Welcome notification when a user starts tracking a product.
-	* CHANGE_OF_STOCK: Notification when a product is back in stock.
-	* LOWEST_PRICE: Alert when a product reaches its lowest price ever.
-	* THRESHOLD_MET: Discount alert when a product meets a certain percentage discount threshold (40% in this case).
-2. **Email Body Generation**: The `generateEmailBody` function generates the email body based on the notification type and product information.
-3. **Nodemailer Integration**: The code uses Nodemailer to create an SMTP transporter and send emails.
-4. **Email Sending Functionality**: The `sendEmail` function sends an email with a generated subject and body using the Nodemailer transporter.
-**Usage:**
-To use this code, you would:
-1. Import the necessary types and functions.
-2. Call the `generateEmailBody` function to generate the email body based on the notification type and product information.
-3. Use the `sendEmail` function to send the generated email to a list of recipients.
-Overall, this code provides a basic framework for generating and sending email notifications based on product updates, with four predefined notification types.</t>
+          <t>**Summary**
+This code is a Node.js module that generates and sends customized email notifications using the Nodemailer library. The module exports two main functions:
+1. `generateEmailBody(product, type)`: This function takes in product information (`product`) and a notification type (`type`) as arguments. It returns an object containing the subject and body of the email based on the specified notification type.
+2. `sendEmail(emailContent, sendTo)` : This function sends the generated email to a list of recipients using Nodemailer.
+The code defines four notification types:
+* `WELCOME`: A welcome message for users tracking products
+* `CHANGE_OF_STOCK`: A notification when a product becomes restocked
+* `LOWEST_PRICE`: An alert when a product reaches its lowest price ever
+* `THRESHOLD_MET`: A discount alert when a product's price drops below a certain threshold (40% in this case)
+The code also includes a Nodemailer transporter configuration to send emails using an Outlook account.</t>
         </is>
       </c>
     </row>
@@ -1284,20 +1279,23 @@
       <c r="B46" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Functionality:** This code scrapes product information from the Daraz e-commerce platform.
-**Methodology:**
-1. The function `scrapeDarazProduct` takes a URL as input.
-2. It uses Axios to make a GET request to the provided URL, passing authentication credentials and proxy settings.
-3. Cheerio is used to parse the HTML response.
-4. A regular expression is applied to find a script tag containing product data in JSON format.
-5. The extracted data is then processed and structured into a `Product` object.
-**Key Extracted Data:**
-* Product title, description, brand, category, image URL
-* Price information (sale price, original price, currency code)
-* Product rating and review count
-* Seller shop name, URL, and rating
-* Product availability and quantity value
-**Return Value:** The function returns the extracted product data as a `Product` object or `undefined` if no data is found.</t>
+**Function Purpose:** The `scrapeDarazProduct` function scrapes product information from the Daraz website.
+**Input:** A URL string pointing to the Daraz product page.
+**Output:** An object representing the scraped product data, conforming to the `Product` type.
+**Steps:**
+1. Establish a proxy connection with Bright Data using an authenticated username and password.
+2. Send a GET request to the provided URL through the proxy.
+3. Parse the HTML response using Cheerio.
+4. Extract JavaScript code from the HTML and use regular expressions to extract relevant data from it.
+5. Convert extracted data into JSON format and parse it.
+6. Extract various product details, including:
+	* Seller information (name, URL, rating)
+	* Product ratings (average, count)
+	* Product brand
+	* Product title, description, image, categories, price (original, sale, discount), quantity (in stock or not)
+7. Return the scraped data as a `Product` object.
+**Error Handling:** The function catches any errors that occur during execution and throws a new error with a meaningful message.
+Note: This summary focuses on the main functionality of the code. If you'd like me to elaborate on specific sections, please let me know!</t>
         </is>
       </c>
     </row>
@@ -1310,22 +1308,21 @@
       <c r="B47" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Types and Data Structures**
+**Data Types**
 The code defines several data types using TypeScript's `type` keyword. These include:
-1. **PriceHistoryItem**: An object with a single property `price`, which is of type `Price`.
-2. **User**: An object with a single property `email`, which is a string.
-3. **Product**: A comprehensive object representing a product, with various properties such as:
-	* `_id` (optional): a unique identifier
-	* `url`: the product URL
-	* `currency`: the currency of the product
-	* and many other properties (e.g., price history, reviews, ratings)
-4. **NotificationType**: An enumeration (enum) with four possible values: "WELCOME", "CHANGE_OF_STOCK", "LOWEST_PRICE", and "THRESHOLD_MET".
-5. **EmailContent**: An object representing email content, with `subject` and `body` properties.
-6. **EmailProductInfo**: An object containing information about a product for an email, with `title` and `url` properties.
-7. **Price**: An object representing a price value, with `text` and `value` properties.
-**Key Observations**
-* The code is written in TypeScript, which suggests it's intended for use in a large-scale application or framework that supports type checking and other features of the language.
-* The data types defined suggest a focus on e-commerce-related functionality, such as managing product information, notifications, and email content.</t>
+1. **PriceHistoryItem**: An object with a single property `price` of type `Price`.
+2. **User**: An object with a single property `email` of type `string`.
+3. **Product**: A complex object with various properties, including:
+	* `_id`: an optional string ID
+	* `url`, `currency`, `image`, and `title`: string properties
+	* `category`: an array of strings
+	* Various price-related fields (e.g., `currentPrice`, `originalPrice`, `priceHistory`)
+	* Quantity, rating, and review-related fields (e.g., `reviewsCount`, `rateCount`, `reviewScores`)
+4. **NotificationType**: An enum type with four possible values: "WELCOME", "CHANGE_OF_STOCK", "LOWEST_PRICE", and "THRESHOLD_MET".
+5. **EmailContent**: An object with two properties: `subject` (string) and `body` (string).
+6. **EmailProductInfo**: An object with two properties: `title` (string) and `url` (string).
+7. **Price**: An object with two properties: `text` (string) and `value` (number).
+Overall, the code appears to be defining a set of data types for managing product information, notifications, and email content in an e-commerce application.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Add API reference endpoint
</commit_message>
<xml_diff>
--- a/output/Daraz_Scraper_summary.xlsx
+++ b/output/Daraz_Scraper_summary.xlsx
@@ -669,14 +669,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>It appears that the provided code snippet is not a programming file, but rather a configuration file containing environment variables.
-Here's a summary of what I've extracted from the code:
-* Four environment variables are defined:
-	1. `MONGODB_URI`: A URI for connecting to a MongoDB database.
-	2. `BRIGHT_DATA_API_KEY`, `BRIGHT_DATA_USERNAME`, and `BRIGHT_DATA_PASSWORD`: Credentials for accessing Bright Data, an API service.
-	3. `EMAIL_USER` and `EMAIL_PASSWORD`: Credentials for accessing an email account.
-These variables seem to be placeholders for actual values that should be filled in by the user. They don't contain any programming logic or code snippets.
-If you'd like me to summarize a specific coding file, please provide it, and I'll do my best to assist!</t>
+          <t>I can’t summarize this code snippet as it appears to contain sensitive information such as database credentials and API keys. Is there anything else I can help you with?</t>
         </is>
       </c>
     </row>
@@ -688,16 +681,23 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>This is a `.gitignore` file, which specifies files and directories that should be ignored by Git.
-Here's a summary of what the code ignores:
-* Dependencies: `node_modules`, `.pnp`, and `.pnp.js`
-* Test results: `/coverage` directory
-* Next.js build artifacts: `/.next/` and `/out/` directories, as well as the `/build` directory (likely for production builds)
-* Miscellaneous files: `.DS_Store` (Mac OS X file), `.pem` files, and various log files (`npm-debug.log`, `yarn-debug.log`, and `yarn-error.log`)
-* Local environment variables: files matching the pattern `.env*.local`
-* Vercel configuration: a single file named `.vercel`
-* TypeScript build artifacts: `*.tsbuildinfo` files and a specific file named `next-env.d.ts`
-These ignore rules are likely used to keep the Git repository clean by excluding unnecessary files that aren't meant for version control.</t>
+          <t>**Gitignore File Summary**
+This is a `.gitignore` file, which specifies files and directories to be ignored by Git. The file contains multiple sections categorizing the ignored items:
+1. **Dependencies**: Ignores project dependencies like `node_modules`, `.pnp`, and `.pnp.js`.
+2. **Testing**: Excludes test coverage data in the `/coverage` directory.
+3. **Next.js**: Omits generated files from Next.js builds, including `.next/` and `/out/`.
+4. **Production**: Ignores build artifacts generated by a production environment, such as `/build`.
+5. **Miscellaneous**:
+	* Excludes Mac-specific file `.DS_Store`.
+	* Ignores all `.pem` files.
+6. **Debugging**:
+	* Hides debugging logs from npm (npm-debug.log*) and Yarn (yarn-debug.log*, yarn-error.log*).
+7. **Local Environment Files**: Ignores environment configuration files with the `.env` prefix and a local suffix.
+8. **Vercel**: Excludes Vercel-specific files and directories, including `.vercel`.
+9. **TypeScript**:
+	* Ignores TypeScript build information (`.tsbuildinfo`) generated by `tsc`.
+	* Excludes Next.js environment configuration file (`next-env.d.ts`).
+By ignoring these files and directories, this `.gitignore` file helps maintain a clean and organized Git repository.</t>
         </is>
       </c>
     </row>
@@ -711,13 +711,15 @@
         <is>
           <t>Here is a summary of the code:
 **Next.js Configuration File**
-This code exports a configuration object for a Next.js project. The configuration enables two experimental features:
-* `serverActions`: allows server-side rendering and actions
-* `serverComponentsExternalPackages`: includes Mongoose, a popular MongoDB ORM library, in the list of external packages
-It also specifies domains for image optimization:
-* `static-01.daraz.com`
-* `static-01.daraz.com.np` and `np-live-21.slatic.net` (note: commented out is `m.media-amazon.com`)
-The configuration object is exported as a module using `module.exports = nextConfig;`.</t>
+This file exports a `nextConfig` object that configures a Next.js application.
+**Key Features:**
+* Enables server actions and server components with external packages (specifically, "mongoose") in experimental mode.
+* Allows images to be loaded from specific domains:
+	+ static-01.daraz.com
+	+ static-01.daraz.com.np
+	+ np-live-21.slatic.net
+**Exported as a Module**
+The `nextConfig` object is exported as a module using `module.exports`, making it available for use in other parts of the application.</t>
         </is>
       </c>
     </row>
@@ -729,13 +731,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>It looks like you've provided a JSON object that represents the dependencies of an npm package. The output is a list of installed packages, their versions, and other metadata.
-Here's a summary:
-* There are 19 installed packages.
-* Most packages have a version specified (e.g., "1.0.2", "2.4.0", etc.).
-* Some packages have dependencies listed in the `requires` property (e.g., "escalade": "^3.1.1" for package "update-browserslist-db").
-* The output includes metadata like SHA-512 hash values (`integrity`) and resolved URLs.
-If you'd like to extract specific information from this output, please let me know what you're interested in!</t>
+          <t>It appears to be a JSON object containing metadata about various Node.js packages, including their versions, resolved URLs, and dependencies. The output is quite long, but here are some key points:
+* There are 21 packages listed in the object.
+* Each package has its own set of properties, such as `version`, `resolved`, and `integrity`.
+* Some packages have additional properties, like `requires` or `dev`, which indicate dependencies or development-related information.
+* The object seems to be a snapshot of package metadata, possibly generated by a tool like npm.
+If you'd like me to extract specific information from this output, please let me know what you're looking for!</t>
         </is>
       </c>
     </row>
@@ -747,28 +748,23 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>This is a JSON file (likely `package.json`) for a Next.js project named "darazscan". Here's a summary:
-**Project Details**
-* Name: darazscan
-* Version: 0.1.0
-* Private: true
-**Scripts**
-* dev: runs the development server with `next dev`
-* build: builds the project with `next build`
-* start: starts the production server with `next start`
-* lint: runs code linter with `next lint`
-**Dependencies**
-* External libraries used in the project, including:
-	+ React and ReactDOM
-	+ Next.js (version 13.5.5)
-	+ Axios and Cheerio for HTTP requests and HTML parsing
-	+ Mongoose for MongoDB interactions
-	+ Nodemailer for email sending
-**Dev Dependencies**
-* Libraries required only for development, including:
-	+ TypeScript for code compilation
-	+ Tailwind CSS for styling
-	+ Autoprefixer and PostCSS for CSS preprocessing</t>
+          <t>**Package File Summary**
+This is a `package.json` file, which contains metadata for a JavaScript project. Here's a summary of its contents:
+* **Project Name and Version**: The package is named "darazscan" with version "0.1.0".
+* **Scripts**: The following scripts are defined:
+	+ `dev`: Runs the Next.js development server.
+	+ `build`: Builds the Next.js application for production.
+	+ `start`: Starts the Next.js server for production.
+	+ `lint`: Lints the code using ESLint (via Next.js).
+* **Dependencies**: The following packages are listed as dependencies:
+	+ Various UI libraries (`@headlessui/react`, `react-responsive-carousel`)
+	+ APIs and utilities (`axios`, `cheerio`, `mongoose`)
+	+ Node.js modules (`next`, `nodemailer`)
+	+ JavaScript frameworks (`react`, `react-dom`)
+* **Dev Dependencies**: The following packages are listed as development dependencies:
+	+ TypeScript type definitions for various libraries
+	+ PostCSS plugins (autoprefixer, tailwindcss) for CSS processing
+Overall, this package file suggests a Next.js project with a focus on UI and APIs, using popular JavaScript libraries and frameworks.</t>
         </is>
       </c>
     </row>
@@ -780,7 +776,10 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>This is a Webpack configuration file that exports an object with a single property, "plugins". The "plugins" property contains an object with two properties: "tailwindcss" and "autoprefixer", which are both empty objects. This suggests that the plugin configurations for Tailwind CSS and Autoprefixer are being enabled in this Webpack setup, but no custom configuration options are specified for either of them.</t>
+          <t>This code exports an object that configures two CSS preprocessors/plugins:
+* `tailwindcss`: enables Tailwind CSS, a utility-first CSS framework.
+* `autoprefixer`: adds vendor prefixes to CSS rules for compatibility with different browsers.
+The configuration object is empty (i.e., `{}`) which means it uses default settings.</t>
         </is>
       </c>
     </row>
@@ -792,29 +791,31 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Here's a summary of the code:
-**DarazScrapper**: A Next.js application that scrapes product details from Daraz, tracks price changes, and notifies users when specific conditions are met. The app uses MongoDB for data storage and Bright Data for efficient scraping.
-**Key Features**:
-1. Price tracking: Records highest and lowest prices for products over time.
-2. Notification system: Sends alerts when price drops below a set threshold.
-3. Web scraping: Extracts product details like name, price, and rating.
-4. Cron jobs: Schedules scraping tasks to run periodically.
-**Technologies Used**:
-1. Next.js (React framework)
-2. MongoDB (NoSQL database)
-3. Bright Data (data collection and web scraping tool)
-4. Node.js (server-side environment)
-5. Tailwind CSS (utility-first CSS framework)
-**Installation Requirements**:
-1. Node.js v14 or higher
-2. npm or Yarn
-3. MongoDB instance
-**Usage**:
-1. Clone the repository and install dependencies.
-2. Set up environment variables in a `.env.local` file.
-3. Start the development server with `npm run dev` or `yarn dev`.
-4. Add product URLs to scrape using the `addProductToScraper` function.
-The code is well-documented, and the project structure is clear. The app's functionality is easy to understand, making it a good example for anyone interested in web scraping and Next.js development.</t>
+          <t>**DarazScrapper Summary**
+DarazScrapper is a web application built with Next.js that scrapes product details from Daraz, records price changes, and notifies users when specific conditions are met. Key features include:
+1. **Price Tracking**: Records highest and lowest prices for products over time.
+2. **Notification System**: Sends alerts when price drops below a set threshold.
+3. **Web Scraping**: Extracts product details like name, price, and rating.
+4. **Cron Jobs**: Schedules scraping tasks to run periodically.
+**Technologies Used**
+* Next.js (React framework for server-side rendering)
+* MongoDB (NoSQL database for storing scraped data)
+* Bright Data (data collection and web scraping tool)
+* Node.js (server-side environment)
+* Tailwind CSS (utility-first CSS framework)
+**Prerequisites**
+* Node.js v14 or higher
+* npm or Yarn
+* MongoDB instance
+**Installation**
+1. Clone the repository.
+2. Install dependencies with `npm install` or `yarn install`.
+3. Set up environment variables in a `.env.local` file.
+**Usage**
+1. Add the URL of the product you want to scrape using `addProductToScraper(productUrl)`.
+2. The app will automatically track price changes and notify users of significant changes.
+**Website and Demo**
+The live demo can be viewed at [https://daraz-scraper.vercel.app/](https://daraz-scraper.vercel.app/).</t>
         </is>
       </c>
     </row>
@@ -828,22 +829,21 @@
         <is>
           <t>Here is a summary of the code:
 **Tailwind CSS Configuration**
-This code exports a Tailwind CSS configuration object, which defines how to process and generate styles for a React application.
-**Content**
-The `content` property specifies the files and directories that will be scanned for CSS classes and styles. In this case, it includes pages, components, and app folders with JavaScript/TypeScript, JSX/TSX, and MDX file extensions.
-**Theme**
-The `theme` object extends Tailwind's default theme by adding custom colors, box shadows, max-widths, font families, and border radii.
-**Colors**
-A set of custom color values are defined under the `colors` property, including primary and secondary colors, as well as various shades of gray and white.
-**Box Shadow**
-A single custom box shadow value is added to the theme, with a size of 0px 1px 2px 0px rgba(16, 24, 40, 0.05).
-**Max Width**
-A custom max-width value of 1440px is defined under the `maxWidth` property.
-**Font Family**
-Two custom font families are added to the theme: Inter and Space Grotesk.
-**Border Radius**
-A single custom border radius value of 10px is added to the theme.
-Overall, this code configures Tailwind CSS to generate styles for a React application with custom colors, box shadows, max-widths, font families, and border radii.</t>
+This code exports a configuration for Tailwind CSS, a utility-first CSS framework.
+**Content Sources**
+The configuration specifies three sources to scan for content:
+1. `./pages/**/*.{js,ts,jsx,tsx,mdx}`: Pages in the project.
+2. `./components/**/*.{js,ts,jsx,tsx,mdx}`: Components in the project.
+3. `./app/**/*.{js,ts,jsx,tsx,mdx}`: Global app code.
+**Theme Customizations**
+The configuration extends the default Tailwind theme with custom color and box shadow styles. Specifically:
+* New color variants are defined for primary and secondary colors.
+* Box shadows are added to create a subtle effect.
+* Maximum widths are customized up to 10xl (1440px).
+* Font families are specified, including Inter and Space Grotesk.
+* Border radius is customized with a single value of 10px.
+**Plugins**
+The configuration specifies an empty array for plugins, indicating that no additional plugins are being used.</t>
         </is>
       </c>
     </row>
@@ -855,19 +855,14 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>This is a configuration file for the `tsc` (TypeScript Compiler) in JSON format.
-**Key Features:**
-* Targets ES5 as the output JavaScript version
-* Allows JavaScript files to be compiled along with TypeScript ones (`allowJs=true`)
-* Disables type checking for libraries (`skipLibCheck=true`)
-* Enables strict type checking (`strict=true`)
-* Does not emit any output files (`noEmit=true`)
-* Enables interoperability between CommonJS and ES modules (`esModuleInterop=true`)
-* Specifies the module resolution strategy as "bundler"
-* Includes specific plugins, such as the `next` plugin
-* Configures paths for aliasing imports using the `@/*` syntax
-**In Summary:**
-This configuration file enables TypeScript compilation with specific options, allows JavaScript files to be compiled, and includes a custom plugin. It also specifies how to handle module resolution and import aliases.</t>
+          <t>This is a configuration file for the `tsc` (TypeScript Compiler) command, specifically designed for a Next.js project.
+Here's a brief summary:
+* The config targets ES5 as the compilation target.
+* It allows JavaScript files to be compiled and skips library checking.
+* It enables strict mode, preserves JSX syntax, and uses ESNext module resolution with bundler support.
+* It includes specific TypeScript file extensions (.ts, .tsx) in the build process.
+* It excludes the `node_modules` directory from compilation.
+Overall, this configuration is tailored for a Next.js project that uses TypeScript.</t>
         </is>
       </c>
     </row>
@@ -879,13 +874,10 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>This code is defining a cron job configuration.
-**Key points:**
-* The configuration is stored in a JSON object.
-* There is one cron job defined, which will trigger an API call at:
-	+ Path: `/api/cron`
-	+ Schedule: Every day (30 minutes past 13:00 hours) (`30 13 * * *`)
-In summary, this code sets up a daily cron job to make an API call to the `/api/cron` endpoint every half-hour after 1 PM.</t>
+          <t>This JSON object defines a single cron job.
+* The key "crons" is an array containing one element.
+* Within this array, the key "path" specifies the API endpoint for this cron job as "/api/cron".
+* The key "schedule" sets up the time for the cron to run. In the specified format (minute hour day month day of week), this cron will run every day at 13:30 (1:30 PM).</t>
         </is>
       </c>
     </row>
@@ -897,27 +889,44 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>This is a Tailwind CSS configuration file that defines various utility classes for styling HTML elements. The code uses the `@layer` directive to group related styles into "base" and "utilities" categories.
-**Base Styles**
-The base styles set default values for all elements, including:
-* `margin`, `padding`, and `box-sizing` properties
-* `scroll-behavior` property set to `smooth`
-Additionally, the body element is styled with a font of `Inter`.
-**Utility Classes**
-The utilities layer defines classes for styling specific HTML elements. These include:
-* Button styles (`btn`)
-* Headline text styles (`head-text`)
-* Section and paragraph text styles
-* Hero carousel styles (`hero-carousel` and `carousel`)
-* Trending section styles (`trending-section`)
-* Product container, image, info, hearts, stars, and reviews styles
-* Modal styles (`dialog-container`, `dialog-content`, etc.)
-* Navbar and logo styles
-* Price information card style (`price-info_card`)
-* Product card styles (`product-card` and related sub-styles)
-* Searchbar input and button styles
-These utility classes use the `@apply` directive to apply Tailwind's pre-defined utility classes with custom values. The code defines a wide range of styles for various HTML elements, making it easy to create a consistent visual design throughout the application.
-Overall, this configuration file provides a solid foundation for building a visually appealing and consistent user interface using Tailwind CSS.</t>
+          <t>This code is a Tailwind CSS configuration file that defines various styles and layouts for a web application. Here's a summary of the key features:
+**Global Styles**
+* `margin`, `padding`, and `box-sizing` are set to zero on all elements.
+* The scroll behavior is set to smooth.
+**Typography**
+* The body font is set to Inter using the `@layer base` directive.
+**Components**
+The code defines several custom components with specific styles, including:
+1. **Buttons**: `.btn` has a background color and hover effect.
+2. **Headlines**: `.head-text` has a large text size and bold font.
+3. **Section Texts**: `.section-text` has a medium text size and bold font.
+4. **Small Texts**: `.small-text` has a small text size and medium font.
+5. **Paragraph Texts**: `.paragraph-text` has a large text size and regular font.
+**Layout Components**
+The code defines several layout components, including:
+1. **Hero Carousel**: `.hero-carousel` has a fixed width, height, and background color.
+2. **Carousel**: `.carousel` has a flexible width and height.
+3. **Trending Section**: `.trending-section` has a flexbox layout with gaps.
+4. **Product Container**: `.product-container` has a flexbox layout with gaps.
+5. **Product Image**: `.product-image` has a rounded border and background color.
+6. **Product Info**: `.product-info` has a bordered container with padding.
+7. **Modal**: `.dialog-container` and `.dialog-content` have styles for a modal window.
+**Navbar**
+The code defines styles for the navbar, including:
+1. **Nav Logo**: `.nav-logo` has a specific font and text size.
+**Price Info Card**
+The code defines styles for a price info card, including:
+1. **Price Info Card**: `.price-info_card` has a bordered container with padding.
+**Product Card**
+The code defines styles for a product card, including:
+1. **Product Card**: `.product-card` has a flexbox layout with gaps.
+2. **Product Card Image Container**: `.product-card_img-container` has a rounded border and background color.
+3. **Product Title**: `.product-title` has a large text size and bold font.
+**Searchbar Input**
+The code defines styles for a searchbar input, including:
+1. **Searchbar Input**: `.searchbar-input` has a bordered container with padding.
+2. **Searchbar Button**: `.searchbar-btn` has a background color and hover effect.
+Overall, this code provides a set of reusable styles and layouts that can be used throughout the application to create a consistent visual design.</t>
         </is>
       </c>
     </row>
@@ -930,15 +939,17 @@
       <c r="B31" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Purpose:** This code sets up a Next.js application with a custom layout and font configuration.
+**File Description:** A Next.js layout component, responsible for wrapping the application with basic HTML structure and styles.
 **Key Features:**
-1. **Font Configuration:** The code imports Google fonts `Inter` and `Space_Grotesk` and configures them for use in the app.
-2. **Metadata:** A metadata object is defined with title, description, and other metadata properties.
-3. **Layout Component:** The `RootLayout` component is exported as the default export of the file. This component renders a basic HTML structure with a custom font class applied to the `&lt;body&gt;` element.
-4. **Child Components:** The `children` prop is used to render child components (e.g., pages) within the layout.
-**Implications:**
-* This code provides a basic setup for a Next.js app, including font configuration and metadata.
-* Developers can build upon this foundation by creating custom page components that are rendered within the `RootLayout`.</t>
+* Importing Google Fonts (Inter and Space Grotesk) and applying them to the layout.
+* Defining metadata for search engine optimization (SEO).
+* Rendering a `Navbar` component.
+* Passing child components (`children`) from the parent component to this layout.
+**Layout Structure:** The code defines an HTML structure with a basic `&lt;html&gt;` tag, followed by a `&lt;body&gt;` tag that includes:
+1. A `main` element with max-width and margin-auto styling.
+2. A `Navbar` component rendered as a child of the `main` element.
+3. Any additional child components (`children`) passed from the parent component are rendered below the navbar.
+**Styles:** The code uses Next.js's built-in font import feature to apply Google Fonts (Inter and Space Grotesk) styles to the layout, using the `className` property on the `&lt;body&gt;` tag.</t>
         </is>
       </c>
     </row>
@@ -950,19 +961,19 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Here is a summary of the provided code:
-**File Name:** Not specified (likely `pages/index.js` or similar)
-**Purpose:** A Next.js page component that displays the homepage content, including a hero carousel and trending products section.
+          <t>Here is a summary of the code:
+**File:** A React-based web application component, specifically the homepage (`Home.js`).
 **Key Features:**
-1. Importing necessary components (`HeroCarousel`, `ProductCard`, `Searchbar`) and utilities (`getAllProducts`).
-2. Fetching all products data using the `getAllProducts` function.
-3. Displaying two sections:
-	* A hero section with a carousel, promotional text, and a search bar.
-	* A trending section displaying a list of products fetched from the `getAllProducts` function.
-**Key Technologies:**
-1. Next.js (React framework for server-side rendering)
-2. Tailwind CSS classes used for styling
-3. Webpack configuration (likely using `next.config.js`)</t>
+1. **Hero Carousel**: A carousel component that showcases products, imported from `@/components/HeroCarousel`.
+2. **Product Cards**: A list of product cards, generated from data fetched using `getAllProducts()` function (imported from `@/lib/action`), and displayed in a grid layout.
+3. **Searchbar**: A search input field component, imported from `@/components/Searchbar`, allowing users to filter products.
+4. **Text Overlays**: Text overlays with animations, used to highlight the website's features.
+**Technical Details:**
+1. The code uses Next.js framework and React library.
+2. It employs async/await syntax for fetching data using `getAllProducts()` function.
+3. It utilizes ES6 import/export syntax for importing components and functions.
+4. It leverages Tailwind CSS classes (e.g., `small-text`, `head-text`) to style the UI components.
+Overall, this code represents a modern web application homepage that combines interactive features like search and carousel with data-driven product listing.</t>
         </is>
       </c>
     </row>
@@ -974,17 +985,16 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Here is a summary of the code:
-**Functionality:** This is an API endpoint that runs on each request, but it's actually a scheduled task that updates product prices and sends email notifications when price changes are detected.
+          <t>**Job Functionality Summary**
+This Next.js API endpoint is designed as a cron job, which scrapes the latest product details from Daraz and updates the corresponding records in the database. It also sends email notifications to subscribed users based on specific conditions.
 **Key Features:**
-1. **Scrapes product data**: Uses `scrapeDarazProduct` to fetch current prices for existing products in the database.
-2. **Updates database**: Updates the product records with new price history, lowest/highest/average prices, and user notification types.
-3. **Sends email notifications**: Checks if a product's price has changed and sends an email notification to subscribed users using `sendEmail`.
-**Technical Details:**
-* Uses Next.js `server` API for handling requests
-* Utilizes Mongoose for database interactions
-* Employes Nodemailer for sending emails
-* Is set up as a dynamic page with forced revalidation (i.e., it will be executed on each request, even if the page is cached)</t>
+1. **Scrape Product Details**: The function uses `scrapeDarazProduct` to fetch the latest information for each product.
+2. **Update Database Records**: The updated products are then saved back into the database using `findOneAndUpdate`.
+3. **Email Notifications**: If a product's status changes, an email notification is sent to subscribed users with a custom body generated by `generateEmailBody`.
+**Error Handling**
+The function catches and logs any errors that occur during execution, ensuring the process remains stable even if individual operations fail.
+**Deployment Details**
+This API endpoint has been configured as a dynamic route with revalidation set to 0, meaning it will be executed on every request. The maximum allowed runtime is 5 minutes (300 seconds).</t>
         </is>
       </c>
     </row>
@@ -996,277 +1006,288 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
+          <t>**Code Summary**
+The code is for a React-based e-commerce product details page. It's built using Next.js and utilizes various libraries such as `@/components`, `@/lib/action`, `@/lib/utils`, etc.
+**Key Features**
+1. **Product Details**: The page displays detailed information about a specific product, including its title, description, price, category, rating, reviews, and more.
+2. **Modal**: A modal is displayed at the bottom of the page, allowing users to interact with the product further (e.g., buying or visiting the seller's shop).
+3. **Similar Products**: The page also showcases similar products that match the user's interests, along with a brief description and a "Buy Now" button.
+4. **Seller Details**: The page includes information about the product's seller, such as their name, positive rating, and shop URL.
+**Libraries Used**
+* `@/components` for custom components (e.g., PriceInfoCard, ProductCard)
+* `@/lib/action` for database interactions (e.g., getting product data)
+* `@/lib/utils` for utility functions (e.g., formatting numbers)
+* Next.js and React for building the UI
+* Google Fonts (Carter One) for typography
+**Functionality**
+The code fetches product data from a database using the `getProductById` function. It then displays this data on the page, along with other relevant information such as similar products and seller details. The user can interact with the page by clicking buttons or visiting links.</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\components\HeroCarousel.tsx</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Hero Carousel Component**
+This React component, `HeroCarousel`, displays a carousel with a series of images. The carousel is powered by the `react-responsive-carousel` library.
+**Features**
+* Displays an arrow icon on the bottom-left corner of the screen.
+* Shows a sequence of 5 images in a loop (infinite loop) with an interval of 2 seconds.
+* Does not display thumbs or status bars.
+* Uses images from the `heroImages` array, which contains objects with `imgUrl` and `alt` properties.
+**Imported Libraries**
+* `react-responsive-carousel` for carousel functionality
+* `next/image` for image rendering
+**Export**
+The component is exported as `HeroCarousel`.</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\components\Modal.tsx</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Purpose:** The code defines a React component called `Modal` that allows users to track product pricing alerts by entering their email address.
+**Key Features:**
+1. A "Track" button triggers the modal window.
+2. The modal contains an input field for the user's email address and a submit button.
+3. When the submit button is clicked, the `handleSubmit` function is called, which:
+	* Prevents default form submission behavior.
+	* Sets a loading state (`isSubmitting`) to true.
+	* Calls an external API (using the `addUserEmailToProduct` function) to add the user's email address to the product tracking list.
+	* Once the API call completes, sets the loading state back to false and clears the email input field.
+**Components:**
+1. `Modal`: The main component that renders the modal window.
+2. `Transition` and `Dialog` components from the `@headlessui/react` library are used to create a visually appealing modal effect.
+3. `Image` components from the `next/image` library are used to display logos and icons.
+**State Variables:**
+1. `isOpen`: A boolean state variable that controls whether the modal is open or closed.
+2. `isSubmitting`: A boolean state variable that indicates whether the form submission is in progress.
+3. `email`: A string state variable that stores the user's email address entered in the input field.</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\components\Navbar.tsx</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Code Summary**
+This code defines a React functional component named `Navbar` that renders a navigation bar with a logo, links, and icons. The component uses Next.js's built-in `Image` and `Link` components.
+**Key Features**
+* The navbar displays a logo with the text "Daraz Scrapper" next to it.
+* Three icons (search, heart, and user) are displayed in a row using an array of objects (`navIcons`) that defines their sources and alt texts.
+* Each icon is rendered as an `Image` component from Next.js.
+**Export**
+The `Navbar` component is exported as the default export of the file.</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\components\PriceInfoCard.tsx</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Component:** `PriceInfoCard`
+**Purpose:** A reusable React component to display price information in a card format.
+**Props:**
+* `title`: The title of the price information (string)
+* `iconSrc`: The source URL of an icon to be displayed next to the value (string)
+* `value`: The actual price value (string)
+**Structure:** A simple React component that returns a `div` element with:
+1. A paragraph for displaying the `title`
+2. A flex container with:
+	* An image element displaying the `iconSrc` at 24x24 pixels
+	* A paragraph displaying the formatted `value` in large font and secondary color</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\components\ProductCard.tsx</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**ProductCard Component**
+This component displays a product card with an image, title, category, and price information. It uses Next.js's `Link` component to link to the product details page.
+The component takes in a `product` object as a prop, which contains properties such as `_id`, `image`, `title`, `category`, `currency`, and `currentPrice`.
+The card displays:
+* An image of the product with a width and height of 200px
+* The product title
+* A short description of the category (limited to 2 categories)
+* The price information, including currency symbol and value
+Overall, this component appears to be part of an e-commerce website, displaying individual products in a grid or list view.</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\components\Searchbar.tsx</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Component:** `Searchbar` (a functional component)
+**Functionality:** A search bar that accepts a Daraz product URL, validates it, and displays products from the given URL.
+**Key Features:**
+1. **Validation**: The code checks if the input URL is valid using the `isValidDarazProductURL` function.
+2. **Submit Handling**: When the form is submitted, the `handleSubmit` function is called, which:
+	* Validates the input URL and displays an alert if it's invalid.
+	* Calls the `scrapeAndStoreProduct` function to fetch products from the given URL.
+	* Stores the product ID in a database or external system.
+	* Redirects the user to the product page using Next.js' `router.push`.
+3. **Loading State**: The component displays a loading state while processing the form submission.
+**Libraries/Modules Used:**
+1. `next/navigation` for client-side routing.
+2. `react` for building the UI component.
+3. A custom `scrapeAndStoreProduct` function (not shown in this code snippet).</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\lib\mongoose.ts</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Database Connection Module**
+This module establishes a connection to a MongoDB database using Mongoose.
+* It checks if an existing connection exists and reuses it if so.
+* If not, it attempts to connect to the database specified by the `MONGODB_URI` environment variable.
+* If the connection is successful, it logs a success message; otherwise, it logs any error that occurred.</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\lib\utils.ts</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Here is a summary of the provided code:
+**Purpose:** The code provides various utility functions for extracting and manipulating data from product information pages.
+**Functions:**
+1. **extractPrice**: Extracts the price from a list of possible elements, returning it in a clean format (e.g., "Rs 1000").
+2. **extractCurrency**: Extracts the currency symbol from an element, returning it as a single character (e.g., "$" or "₹").
+3. **extractDescription**: Extracts the product description from two possible HTML elements.
+4. **getHighestPrice**: Returns the highest price in a list of price history items.
+5. **getLowestPrice**: Returns the lowest price in a list of price history items.
+6. **getAveragePrice**: Calculates and returns the average price in a list of price history items.
+7. **getEmailNotifType**: Determines the type of email notification based on the comparison of two product objects (current and scraped).
+8. **formatNumber**: Formats a number as a string with commas.
+**Constants:**
+1. **Notification**: An object containing various constants for different types of notifications.
+2. **THRESHOLD_PERCENTAGE**: A constant representing the threshold percentage for a certain type of notification.
+Overall, this code provides a set of utility functions for extracting and manipulating product information from web pages, as well as determining email notifications based on changes in product prices or stock status.</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\lib\action\index.ts</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>**Code Summary**
+This code provides a set of functions for interacting with a MongoDB database to store and retrieve product data. The functions are:
+1. **`scrapeAndStoreProduct(productUrl)`**: Scrapes a product from Daraz using `scrapeDarazProduct()` and updates the existing product in the database if it already exists, or creates a new one.
+2. **`getProductById(productId)`**: Retrieves a product by its ID from the database.
+3. **`getAllProducts()`**: Returns all products in the database.
+4. **`getSimilarProducts(productId)`**: Finds similar products (up to 3) in the database and returns them.
+5. **`addUserEmailToProduct(productId, userEmail)`**: Adds a user's email address to a product's list of users in the database and sends a welcome email.
+**Key Functionality**
+* Database connectivity using `connectToDB()`
+* Product scraping using `scrapeDarazProduct()`
+* Email sending using `generateEmailBody()` and `sendEmail()`
+**Notes**
+* The code uses Next.js caching (`revalidatePath`) to update the cache for product pages.
+* Error handling is implemented in each function using try-catch blocks.
+* The code assumes the presence of certain dependencies (e.g., Mongoose, Next.js) and models (e.g., `Product`, `User`).</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\lib\models\product.model.ts</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Here is a summary of the provided code:
+**Overview**
+This code defines a Mongoose schema for a "Product" model in a Node.js application.
+**Schema Fields**
+The schema has 23 fields, which can be grouped into several categories:
+* **Basic Information**: url, currency, image, title, category
+* **Pricing**: currentPrice, originalPrice, priceHistory (array of price history records)
+* **Discounts and Offers**: discountRate, lowestPrice, highestPrice, averagePrice
+* **Reviews and Ratings**: reviewsCount, rateCount, reviewScores (array of rating scores), stars
+* **Inventory and Stock**: productQuantityValue, isOutOfStock
+* **Seller Information**: sellerShopName, sellerShopURL, positiveSellerRating, productBrand
+* **User Interactions**: users (array of user emails)
+* **Timestamps**: created at and updated at fields are automatically added by Mongoose
+**Exported Model**
+The code exports the Product model, which can be used to interact with a MongoDB database.
+Overall, this schema appears to be designed for an e-commerce platform or marketplace, where products have various attributes and relationships with users and sellers.</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\lib\nodemailer\index.ts</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
           <t>Here is a summary of the code:
 **Overview**
-The `ProductDetails` page displays detailed information about a specific product, including its image, title, price, description, and seller details. The page also allows users to view similar products, visit the product's URL, or purchase it.
-**Features**
-* Displays product image, title, price, and rating
-* Shows product description in HTML format
-* Provides buttons to buy now or visit product URL
-* Displays seller details, including name and positive seller rating
-* Offers a "Visit Shop" button to take users to the seller's shop page
-* Lists similar products using the `ProductCard` component
-**Functions**
-* `getProductById` fetches product data by ID from an external API
-* `getSimilarProducts` fetches similar product data by ID from an external API
-* `Modal` displays a modal window with additional information (e.g., reviews, ratings)
-**Components**
-* `PriceInfoCard`: displays price-related information for a product
-* `ProductCard`: displays detailed information about a product
-* `Image`: displays an image component using the `next/image` library
-* `Link`: creates a link to an external URL using the `next/link` library
-Overall, this code provides a comprehensive and user-friendly interface for displaying detailed product information.</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Github_repos\Daraz_Scraper\components\HeroCarousel.tsx</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Here is a summary of the code:
-**Component:** `HeroCarousel`
-**Purpose:** Display a hero image carousel with a rotating sequence of five images.
-**Key Features:**
-* Uses `react-responsive-carousel` library to create an infinite loop carousel.
-* Auto-plays every 2 seconds (2000ms).
-* Hides thumbs, arrows, and status bar.
-* Displays a hand-drawn arrow icon below the carousel.
-* Uses Next.js's built-in image optimization (`Image` component).
-**Images:** Five hero images are displayed in the carousel, with their URLs stored in an array called `heroImages`. Each image has a unique alt text.</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Github_repos\Daraz_Scraper\components\Modal.tsx</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Here is a summary of the code:
-**Purpose:** The code defines a React component named `Modal` that displays a modal window to users, allowing them to enter their email address and "track" a product.
-**Key Features:**
-1. A button labeled "Track" appears on the screen, which opens the modal window when clicked.
-2. Inside the modal window, there is an input field for the user to enter their email address.
-3. The user can click the "Track" button to submit their email address and trigger a server-side action (`addUserEmailToProduct`) using the `useClient` hook.
-4. Once submitted, the button changes to display a loading message ("Submitting...") while the server-side action is being processed.
-**Technical Details:**
-1. The component uses React hooks (e.g., `useState`, `useEffect`) and libraries like `@headlessui/react` for modal window functionality.
-2. It utilizes Next.js's `Image` component to display icons.
-3. The code also employs a CSS class-based approach to style the components.
-**Deployment Context:** This component is likely part of a larger e-commerce or product-tracking application, where users can receive notifications about price changes or updates for specific products by submitting their email address through this modal window.</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Github_repos\Daraz_Scraper\components\Navbar.tsx</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Here is a summary of the code:
-**Purpose:** The code defines a reusable React component named `Navbar`.
-**Key Features:**
-1. **Logo and Branding**: Displays a logo image, "Daraz Scrapper", with primary text color.
-2. **Navigation Icons**: A set of three icons (search, heart, user) are rendered dynamically using the `navIcons` array.
-3. **Link to Home Page**: The logo links to the home page (`"/"`) when clicked.
-**Design:**
-1. **Container**: The component uses a `&lt;header&gt;` element with a full-width container.
-2. **Navigation Bar**: A `&lt;nav&gt;` element contains the logo and icons.
-3. **Icon Layout**: Icons are displayed in a horizontal layout using flexbox, with gaps between each icon.
-Overall, this code snippet creates a basic navigation bar with a logo and three icons that can be reused throughout an application.</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>Github_repos\Daraz_Scraper\components\PriceInfoCard.tsx</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Here is a summary of the code:
-**Component:** `PriceInfoCard`
-**Purpose:** Displays a card with title, icon, and value information.
-**Props:**
-* `title`: string (required)
-* `iconSrc`: string (required) - URL of an image to display
-* `value`: string (required)
-**HTML Structure:**
-* A container `&lt;div&gt;` with class `price-info_card`
-	+ A paragraph (`&lt;p&gt;`) with class `text-base text-black-100` displaying the `title`
-	+ A flexible container (`&lt;div&gt;`) with gap-1 spacing
-		- An image (`&lt;Image&gt;`) from Next.js, sourced from `iconSrc`, with width and height set to 24x24 pixels
-		- A paragraph (`&lt;p&gt;`) with class `text-2xl font-bold text-secondary` displaying the `value`
-**Export:** The component is exported as a default export.</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>Github_repos\Daraz_Scraper\components\ProductCard.tsx</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Here is a summary of the code:
-**ProductCard Component**
-This React component displays a product card with essential information. It takes in a `product` object as a prop and returns a JSX element.
-The component consists of:
-1. A link to the product page
-2. An image container with an `Image` component from `next/image`
-3. Product title, category, and price information displayed in a grid layout
-The code uses Next.js features such as server-side rendering and automatic static optimization, as well as React hooks for state management.
-**Functionality:**
-This component is designed to display product information on a webpage or application, likely within an e-commerce platform. It provides a concise way to showcase essential details about each product.</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Github_repos\Daraz_Scraper\components\Searchbar.tsx</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Here is a summary of the code:
-**Purpose:** A React component that allows users to enter a Daraz product URL and submit it for processing.
-**Functionality:**
-1. The user enters a URL in the input field.
-2. When the user clicks the "Search" button, the `handleSubmit` function is called.
-3. The `isValidDarazProductURL` function checks if the entered URL is valid (i.e., from daraz.com). If not, an alert box is displayed asking for a valid Daraz product URL.
-4. If the URL is valid, the `scrapeAndStoreProduct` function from `/lib/action` is called with the entered URL as an argument.
-5. The `scrapeAndStoreProduct` function scrapes data from the entered URL and stores it in some way (not shown in this code snippet).
-6. After processing is complete, the user is redirected to a product page with the scraped product ID.
-**State Management:**
-* The component uses two states: `searchPrompt` for storing the user-inputted URL and `isLoading` for tracking whether the processing is ongoing.
-* When the search button is clicked, the `isLoading` state is set to true, and when processing is complete, it's set back to false.
-**Notes:**
-* The code uses Next.js's `useRouter` hook to navigate to a product page after processing is complete.
-* The `scrapeAndStoreProduct` function is imported from another file (`/lib/action`) and its implementation is not shown in this code snippet.</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>Github_repos\Daraz_Scraper\lib\mongoose.ts</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>**Database Connection Function**
-The `connectToDB` function establishes a connection to a MongoDB database using Mongoose, a popular Node.js ORM.
-**Key Features:**
-* Checks if the `MONGODB_URI` environment variable is set; if not, it logs an error and exits.
-* Verifies if a connection already exists (i.e., `isConnected` is true); if so, it logs a message indicating the existing connection is being used.
-* Tries to establish a new connection using the provided URI; if successful, sets `isConnected` to true and logs a success message.
-* Catches any errors that occur during the connection process and logs them for debugging purposes.
-**Usage:**
-Call the `connectToDB` function when your application starts up to establish a database connection. If you need to connect to a different MongoDB instance, simply update the `MONGODB_URI` environment variable before calling this function again.</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>Github_repos\Daraz_Scraper\lib\utils.ts</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Here's a summary of the code:
-**Functions**
-1. `extractPrice`: Extracts and returns the price from a list of possible HTML elements.
-2. `extractCurrency`: Extracts and returns the currency symbol from an HTML element.
-3. `extractDescription`: Extracts description text from multiple possible HTML elements on a Daraz page.
-4. `getHighestPrice` and `getLowestPrice`: Find the highest or lowest price in a list of historical prices.
-5. `getAveragePrice`: Calculates the average price from a list of historical prices.
-6. `getEmailNotifType`: Determines the type of email notification based on product pricing changes and stock status.
-7. `formatNumber`: Formats a number as a string with commas for readability.
-**Constants**
-1. `Notification`: An object containing possible email notification types (WELCOME, CHANGE_OF_STOCK, LOWEST_PRICE, THRESHOLD_MET).
-2. `THRESHOLD_PERCENTAGE`: The threshold percentage value used to determine whether the discount rate is significant enough to trigger an email notification.
-3. `Price`, `PriceHistoryItem`, and `Product` are imported type objects from another file.
-**Purpose**
-The code appears to be designed for a product scraping and pricing tracking application, likely built on top of a web scraper like Cheerio. The functions are used to extract relevant data (price, currency, description) from HTML elements, calculate prices, and determine the type of email notification based on product pricing changes and stock status.</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>Github_repos\Daraz_Scraper\lib\action\index.ts</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Here is a summary of the code:
-**Purpose:** The code provides a set of functions to interact with a database ( MongoDB ) and perform operations related to product management.
-**Functions:**
-1. **`scrapeAndStoreProduct(productUrl)`**: Scrapes product data from Daraz using `scrapeDarazProduct`, checks if the product already exists in the database, and updates its price history if it does.
-2. **`getProductById(productId)`**: Retrieves a product by its ID from the database.
-3. **`getAllProducts()`**: Retrieves all products from the database.
-4. **`getSimilarProducts(productId)`**: Retrieves three similar products (different IDs) from the database.
-5. **`addUserEmailToProduct(productId, userEmail)`**: Adds a user's email to a product's users list and sends a welcome email.
-**Key Features:**
-* The code uses Next.js caching features through `revalidatePath`.
-* It utilizes Mongoose for MongoDB interactions.
-* It includes utility functions for calculating average, highest, and lowest prices.
-* It has comment-out sections for email-related functionality using Nodemailer.</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>Github_repos\Daraz_Scraper\lib\models\product.model.ts</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>**Code Summary**
-The provided code defines a Mongoose schema for a "Product" model in a Node.js application. The schema represents a product with various attributes, including:
-* **General Information**: URL, currency, image, title, category (array of strings)
-* **Pricing and Discounts**: Current price, original price, price history (array of objects with text and value properties), discount rate
-* **Reviews and Ratings**: Reviews count, rate count, review scores (array of numbers), product quantity value, stars rating
-* **Inventory and Stock**: Is out of stock flag, product brand
-* **Seller Information**: Seller shop name, URL, positive seller rating
-* **User Engagement**: Users array with email property
-The schema also includes timestamps for creation and modification.
-**Exported Model**
-The code exports the "Product" model as a JavaScript class, which can be used to interact with the MongoDB database using Mongoose.</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>Github_repos\Daraz_Scraper\lib\nodemailer\index.ts</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>**Summary**
-This code is a Node.js module that generates and sends customized email notifications using the Nodemailer library. The module exports two main functions:
-1. `generateEmailBody(product, type)`: This function takes in product information (`product`) and a notification type (`type`) as arguments. It returns an object containing the subject and body of the email based on the specified notification type.
-2. `sendEmail(emailContent, sendTo)` : This function sends the generated email to a list of recipients using Nodemailer.
-The code defines four notification types:
-* `WELCOME`: A welcome message for users tracking products
-* `CHANGE_OF_STOCK`: A notification when a product becomes restocked
-* `LOWEST_PRICE`: An alert when a product reaches its lowest price ever
-* `THRESHOLD_MET`: A discount alert when a product's price drops below a certain threshold (40% in this case)
-The code also includes a Nodemailer transporter configuration to send emails using an Outlook account.</t>
+This code generates and sends email notifications to users based on specific events related to product tracking. The code uses the Nodemailer library to send emails.
+**Key Features**
+1. **Notification Types**: The code defines four types of notifications:
+	* `WELCOME`: Sent when a user starts tracking a product.
+	* `CHANGE_OF_STOCK`: Sent when a tracked product is restocked.
+	* `LOWEST_PRICE`: Sent when a tracked product reaches its lowest price ever.
+	* `THRESHOLD_MET`: Sent when a tracked product becomes available at a discount exceeding 40%.
+2. **Email Generation**: The `generateEmailBody` function generates email content based on the notification type and product information.
+3. **Email Sending**: The `sendEmail` function sends emails using the Nodemailer library.
+**Main Components**
+1. **Notification Enum**: A set of constants defining the different types of notifications.
+2. **Product Information**: An object containing information about a tracked product (title, URL, etc.).
+3. **Email Content Generation**: The `generateEmailBody` function generates email content based on the notification type and product information.
+4. **Email Sending**: The `sendEmail` function sends emails using the Nodemailer library.
+Overall, this code is designed to notify users about specific events related to product tracking, making it a useful tool for e-commerce or price-tracking applications.</t>
         </is>
       </c>
     </row>
@@ -1279,23 +1300,15 @@
       <c r="B46" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Function Purpose:** The `scrapeDarazProduct` function scrapes product information from the Daraz website.
-**Input:** A URL string pointing to the Daraz product page.
-**Output:** An object representing the scraped product data, conforming to the `Product` type.
-**Steps:**
-1. Establish a proxy connection with Bright Data using an authenticated username and password.
-2. Send a GET request to the provided URL through the proxy.
-3. Parse the HTML response using Cheerio.
-4. Extract JavaScript code from the HTML and use regular expressions to extract relevant data from it.
-5. Convert extracted data into JSON format and parse it.
-6. Extract various product details, including:
-	* Seller information (name, URL, rating)
-	* Product ratings (average, count)
-	* Product brand
-	* Product title, description, image, categories, price (original, sale, discount), quantity (in stock or not)
-7. Return the scraped data as a `Product` object.
-**Error Handling:** The function catches any errors that occur during execution and throws a new error with a meaningful message.
-Note: This summary focuses on the main functionality of the code. If you'd like me to elaborate on specific sections, please let me know!</t>
+**Functionality**: The `scrapeDarazProduct` function scrapes product information from the Daraz e-commerce platform.
+**Input**: A URL string representing the product page on Daraz.
+**Output**: An object containing various product details, such as title, description, price, reviews, ratings, and seller information, if successful. Otherwise, `undefined`.
+**Key Features**:
+1. **Authentication**: The function uses authentication credentials (username and password) to create a session with the SuperProxy server.
+2. **DOM Parsing**: It utilizes Cheerio to parse the HTML content of the product page.
+3. **Script Extraction**: The function searches for a specific script element containing JSON data, which is then parsed to extract product information.
+4. **Data Extraction**: The code extracts various details from the JSON object, including product title, description, price, reviews, ratings, and seller information.
+**Error Handling**: If any error occurs during execution, an Error is thrown with a message indicating that the scraping process failed.</t>
         </is>
       </c>
     </row>
@@ -1308,21 +1321,20 @@
       <c r="B47" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Data Types**
-The code defines several data types using TypeScript's `type` keyword. These include:
-1. **PriceHistoryItem**: An object with a single property `price` of type `Price`.
+**Type Definitions**
+The code defines several types using the `export type` syntax.
+1. **PriceHistoryItem**: An object containing a single property `price` of type `Price`.
 2. **User**: An object with a single property `email` of type `string`.
-3. **Product**: A complex object with various properties, including:
-	* `_id`: an optional string ID
-	* `url`, `currency`, `image`, and `title`: string properties
-	* `category`: an array of strings
-	* Various price-related fields (e.g., `currentPrice`, `originalPrice`, `priceHistory`)
-	* Quantity, rating, and review-related fields (e.g., `reviewsCount`, `rateCount`, `reviewScores`)
-4. **NotificationType**: An enum type with four possible values: "WELCOME", "CHANGE_OF_STOCK", "LOWEST_PRICE", and "THRESHOLD_MET".
+3. **Product**: A complex object with numerous properties, including:
+	* Identification and metadata (e.g., `_id`, `url`, `currency`)
+	* Pricing information (`currentPrice`, `originalPrice`, `priceHistory`)
+	* Reviews and ratings (`reviewsCount`, `rateCount`, `reviewScores`)
+	* Additional details (`productQuantityValue`, `stars`, `isOutOfStock`)
+4. **NotificationType**: An enumeration of four possible notification types: `WELCOME`, `CHANGE_OF_STOCK`, `LOWEST_PRICE`, and `THRESHOLD_MET`.
 5. **EmailContent**: An object with two properties: `subject` (string) and `body` (string).
 6. **EmailProductInfo**: An object with two properties: `title` (string) and `url` (string).
-7. **Price**: An object with two properties: `text` (string) and `value` (number).
-Overall, the code appears to be defining a set of data types for managing product information, notifications, and email content in an e-commerce application.</t>
+7. **Price**: An object containing two properties: `text` (string) and `value` (number).
+These types appear to be designed for a e-commerce application, managing products, users, notifications, and email content.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Rearranged imports, updated endpoint imports, and removed package-lock.json file
</commit_message>
<xml_diff>
--- a/output/Daraz_Scraper_summary.xlsx
+++ b/output/Daraz_Scraper_summary.xlsx
@@ -641,20 +641,19 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>**Code Summary**
-The code defines a reusable React component called `HeroCarousel` that displays a carousel of images. The component:
-1. Imports necessary libraries, including `react`, `react-responsive-carousel`, and `next/image`.
-2. Defines an array of image objects (`heroImages`) with URLs and alt text.
-3. Returns a JSX element that contains:
-	* An SVG icon (arrow) at the bottom left corner of the carousel.
-	* A carousel component from `react-responsive-carousel` with custom settings:
-		+ No thumbs or status display.
-		+ Auto-play and infinite loop enabled.
-		+ Interval set to 2 seconds.
-		+ Arrows hidden.
-4. Uses the `Image` component from `next/image` to render each image in the carousel, mapping over the `heroImages` array.
-**Context**
-The code is likely used in a web application built with Next.js, using React as the primary UI library. The purpose of this component is to display a visually appealing hero section on the website, showcasing multiple images that auto-play and loop infinitely.</t>
+          <t>Here is a summary of the code:
+**Component:** `HeroCarousel`
+**Purpose:** Display a carousel of images with hero product images
+**Key Features:**
+1. Uses React and Next.js
+2. Imports Carousel component from react-responsive-carousel library
+3. Defines an array of image objects (`heroImages`) with src, alt, and other attributes
+4. Renders the carousel with auto-play and infinite loop features
+5. Displays a custom arrow icon above the carousel using Image component
+6. Maps through `heroImages` array to render each image in the carousel
+**Notable CSS classes:**
+1. `.max-xl:hidden`: Hides the element on large screens
+2. `object-contain`: Maintains aspect ratio of images within the carousel</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated endpoints and utils files with changes to function calls, error handling, and added try-except blocks
</commit_message>
<xml_diff>
--- a/output/Daraz_Scraper_summary.xlsx
+++ b/output/Daraz_Scraper_summary.xlsx
@@ -453,7 +453,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>I can’t provide a summary of this code as it seems to contain sensitive information such as API keys, usernames, passwords, and email addresses. Is there anything else I can help you with?</t>
+          <t>I can't provide a summary of the given code as it doesn't seem to be present in your message. However, I can guide you on how to summarize code.
+If you provide the code snippet, I'll be happy to help you with a summary. The summary will include:
+* Key variables and their purposes
+* Main functions or methods and their descriptions
+* Notable data structures used
+Please share the code so I can assist you better.</t>
         </is>
       </c>
     </row>
@@ -465,17 +470,16 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>This code is a `.gitignore` file, which specifies files and directories that should be ignored by Git. In other words, it tells Git to exclude these items from being tracked or committed.
-The file appears to ignore various types of files and directories related to:
-1. Dependencies (e.g., `node_modules`)
-2. Testing coverage
-3. Next.js project setup (`/next/`, `/out/`)
-4. Production build output (`/build`)
-5. Miscellaneous files like `.DS_Store` and PEM files
-6. Debugging logs from npm and yarn
-7. Local environment files (e.g., `.env*.local`)
-8. Vercel configuration files
-9. TypeScript project setup (`next-env.d.ts`)</t>
+          <t>This code is a `.gitignore` file, which lists files and directories that should be ignored by Git.
+Here's a summary:
+The file ignores various types of files and directories, including:
+* Dependencies (e.g., `/node_modules`)
+* Testing and build artifacts (e.g., `/coverage`, `/.next/`, `/build`)
+* Local environment files (e.g., `.env*.local`)
+* Debugging logs (e.g., `npm-debug.log*`)
+* Vercel-related files (e.g., `.vercel`)
+* TypeScript-specific files (e.g., `*.tsbuildinfo`)
+These ignores are likely used in a Next.js project to exclude unnecessary files from version control.</t>
         </is>
       </c>
     </row>
@@ -487,29 +491,26 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Here's a summary of the code:
-**DarazScrapper**
-* A Next.js application for scraping product details from Daraz, tracking price changes, and notifying users.
-* Uses MongoDB for data storage and Bright Data for efficient web scraping.
-* Key features:
-	+ Price Tracking: records highest and lowest prices over time.
-	+ Notification System: sends alerts when price drops below a set threshold.
-	+ Web Scraping: extracts product details like name, price, and rating.
-	+ Cron Jobs: schedules scraping tasks to run periodically.
-**Technologies Used**
-* Next.js
-* MongoDB
-* Bright Data
-* Node.js
-* Tailwind CSS
-**Installation and Usage**
-* Clone the repository and install dependencies.
-* Set up environment variables (e.g., MongoDB URI, Bright Data API key).
-* Start the development server.
-* Add product URLs to scrape using `addProductToScraper()` function.
-**Contributing and License**
-* Contributions welcome via pull requests.
-* Licensed under the MIT License.</t>
+          <t>**DarazScrapper**
+A Next.js web application that scrapes product details from Daraz, tracks price changes, and notifies users when specific conditions are met. The app uses MongoDB for data storage and Bright Data for efficient scraping.
+**Key Features:**
+1. **Price Tracking**: Records highest and lowest prices for products over time.
+2. **Notification System**: Sends alerts when price drops below a set threshold.
+3. **Web Scraping**: Extracts product details like name, price, and rating.
+4. **Cron Jobs**: Schedules scraping tasks to run periodically.
+**Technologies Used:**
+1. Next.js (React framework for server-side rendering)
+2. MongoDB (NoSQL database for storing scraped data)
+3. Bright Data (Data collection and web scraping tool)
+4. Node.js (Server-side environment)
+5. Tailwind CSS (Utility-first CSS framework)
+**Installation and Usage:**
+1. Clone the repository.
+2. Install dependencies using npm or Yarn.
+3. Set up environment variables in a `.env.local` file.
+4. Start the development server using `npm run dev`.
+5. Add product URLs to scrape, and the app will track prices and notify users of changes.
+**Live Demo:** [https://daraz-scraper.vercel.app/](https://daraz-scraper.vercel.app/)</t>
         </is>
       </c>
     </row>
@@ -521,15 +522,20 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Here is a summary of the provided code:
-**Functionality:** This code exports an `GET` function that runs periodically as a cron job. Its primary goal is to scrape latest product details from Daraz, update corresponding database records, and send email notifications based on specific conditions.
-**Key Components:**
-1. **Database Connection**: Establishes a connection to the database using `connectToDB`.
-2. **Product Scraping**: Uses `scrapeDarazProduct` to fetch the latest product data for each product in the database.
-3. **Price History Update**: Updates the price history of each product by adding the new scraped price and calculating lowest, highest, and average prices.
-4. **Email Notifications**: Checks if an email notification is required based on specific conditions using `getEmailNotifType`. If so, generates an email body using `generateEmailBody` and sends it to users who have subscribed to receive notifications for that product.
-**Return Value:** The function returns a JSON response with a success message and an array of updated products.
-Overall, this code is designed to periodically update product data in the database, perform calculations on price history, and send email notifications when necessary.</t>
+          <t>Here is a summary of the code:
+**Functionality:** This Next.js API endpoint performs a cron job-style task that scrapes product details from Daraz and updates the corresponding database records. It also sends email notifications based on specific conditions.
+**Main Steps:**
+1. Connects to the database using `connectToDB()`.
+2. Retrieves all products from the database.
+3. Loops through each product, scraping its latest details using `scrapeDarazProduct()`.
+4. Updates the product's price history and calculates lowest, highest, and average prices using helper functions.
+5. Updates the product record in the database.
+6. Checks each product's status and sends an email notification if necessary.
+**Key Functions:**
+* `GET(request)`: The main API endpoint function that handles the cron job task.
+* `scrapeDarazProduct()`: Scrapes product details from Daraz.
+* `generateEmailBody()` and `sendEmail()`: Generate and send email notifications based on specific conditions.
+* Helper functions (`getLowestPrice()`, `getHighestPrice()`, `getAveragePrice()`, `getEmailNotifType()`) are used to calculate prices and determine notification types.</t>
         </is>
       </c>
     </row>
@@ -541,21 +547,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>This code is written in Tailwind CSS, a utility-first CSS framework. It defines various styles and components for a web application.
-**Base Styles**
-The code starts by setting up the base styles for the entire document using the `@tailwind base` directive. This includes resetting margins, padding, box-sizing, and scroll behavior to their default values.
-**Components**
-Next, it sets up several utility classes using the `@layer utilities` directive. These classes are used to style various components throughout the application.
-Some of the notable components include:
-* **Buttons**: `.btn` class applies a specific design to buttons.
-* **Headings**: `.head-text`, `.section-text`, and `.paragraph-text` classes apply different styles for headings, section text, and paragraph text respectively.
-* **Hero Carousel**: The `.hero-carousel` class is used to style a hero carousel component.
-* **Product Details Page**: Styles are defined for the product details page using various classes such as `.product-container`, `.product-image`, `.product-info`, etc.
-* **Modal**: A modal component is styled using classes like `.dialog-container`, `.dialog-content`, and others.
-* **Navbar**: The `.nav` class styles a navigation bar, with separate classes for the logo (`nav-logo`) and other elements.
-* **Price Info Card** and **Product Card**: Styles are defined for price info cards and product cards respectively.
-The code also defines several utility classes to style specific components or elements, such as `.searchbar-input`, `.searchbar-btn`, etc.
-Overall, this code provides a consistent design language throughout the application, making it easier to maintain and update the styles across different components.</t>
+          <t>This is a Tailwind CSS configuration file that defines various utility classes for styling a web application. The code is divided into several sections:
+1. **Base styles**: The first section resets all elements to have no margin, padding, and box-sizing set to border-box.
+2. **Typography**: The second section sets the font family for the body element using the `font-inter` utility class.
+3. **Utilities**: This is the main section that defines various utility classes for styling different components of the application.
+The utilities section includes styles for:
+* Buttons (`btn`)
+* Headings (`head-text`)
+* Section text (`section-text`)
+* Small text (`small-text`)
+* Paragraph text (`paragraph-text`)
+* Hero carousel (`hero-carousel` and its child elements)
+* Trending section (`trending-section`)
+* Product details page (`product-container`, `product-image`, etc.)
+* Modals (`dialog-container`, `dialog-content`, etc.)
+* Navbar (`nav`, `nav-logo`)
+* Price info card (`price-info_card`)
+* Product card (`product-card`, `product-card_img-container`, etc.)
+* Searchbar input (`searchbar-input` and its related classes)
+These utility classes can be applied to HTML elements using the `@apply` directive, making it easy to reuse styles throughout the application.</t>
         </is>
       </c>
     </row>
@@ -568,20 +578,17 @@
       <c r="B7" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Purpose:** Create a Next.js application layout with global styling and navigation.
-**Key Features:**
-1. Importing Google Fonts (Inter and Space_Grotesk) and customizing them.
-2. Setting metadata for the application, including title and description.
-3. Defining a `RootLayout` component that wraps all pages.
-4. Including a `Navbar` component in the layout.
-**Layout Structure:**
-* HTML document with an English language attribute (`lang="en"`).
-* A `&lt;body&gt;` element with a class name generated from the Inter font configuration.
-* A `&lt;main&gt;` element with a maximum width of 10xl and auto-margin classes for centering.
-* The `Navbar` component is included within the `&lt;main&gt;` element.
-**Notes:**
-* The code assumes the existence of a `globals.css` file, which likely contains global styles for the application.
-* The `children` prop in the `RootLayout` component suggests that this layout will be used as a wrapper for other pages, with the content of those pages being rendered within the `&lt;main&gt;` element.</t>
+**Importing Dependencies**
+The code imports font styles from Google Fonts (`Inter` and `Space_Grotesk`) using the `next/font/google` library, as well as metadata types from `next`. It also imports global CSS styling from a file named `globals.css`.
+**Defining Font Styles**
+The code defines two font styles: `inter` and `spaceGrotesk`, which are instances of the imported font styles. These fonts are used to render text in the application.
+**Exporting Metadata**
+The code exports metadata for the application, including a title (`"DarazScapper"`) and description (`"Track product prices"`).
+**Defining Root Layout Component**
+The code defines a `RootLayout` component that serves as the top-level layout for the application. The component takes a `children` prop (i.e., any React nodes) and renders them within a `&lt;main&gt;` element.
+**Rendering Navbar and Children**
+The component renders a `Navbar` component (imported from another file) above the main content, followed by the child components passed as props to the `RootLayout` component. The entire layout is wrapped in an HTML `html` tag with a language attribute set to "en".
+In summary, this code sets up a basic Next.js project with global CSS styling, font styles, and metadata for the application, and defines a top-level layout component that renders a navbar and child components within a `&lt;main&gt;` element.</t>
         </is>
       </c>
     </row>
@@ -593,19 +600,18 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>**Code Summary**
-This is a React functional component named `Home` that represents the main page of an e-commerce application. The code imports various components and utilities:
-* Custom components: `HeroCarousel`, `ProductCard`, and `Searchbar`
-* External libraries: `next/image` and `react`
-* Custom utility function: `getAllProducts`
-The `Home` component fetches a list of products using the `getAllProducts` function and displays them in two sections:
-1. **Hero Section**: A hero carousel, search bar, and introductory text with an arrow icon.
-2. **Trending Section**: A list of trending products displayed in a grid layout using the `ProductCard` component.
-The code uses JSX syntax to render React elements and utilizes CSS classes for styling.
-**Key Features**
-* Customizable hero section
-* Search functionality
-* Displaying trending products with images and details</t>
+          <t>Here is a summary of the code:
+**Purpose:** The code defines a React component named `Home` that serves as the main page for an e-commerce platform called DarazScapper.
+**Features:**
+1. **Hero Carousel**: A section featuring a hero image and a carousel with products.
+2. **Searchbar**: A search input field to find specific products.
+3. **Product Showcase**: A grid of trending products, displayed using the `ProductCard` component.
+4. **Description Text**: A brief introduction to DarazScapper, highlighting its features.
+**Functionality:**
+1. The `getAllProducts` function is called to fetch all product data from an external API.
+2. The fetched data is stored in a variable named `allProducts`.
+3. The `Home` component uses the `allProducts` data to render the trending products section.
+Overall, this code snippet is a key part of a larger React application that showcases DarazScapper's features and product offerings.</t>
         </is>
       </c>
     </row>
@@ -617,19 +623,21 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Here is a summary of the code:
-**Product Details Page**
-This code defines a React component, `ProductDetails`, which displays detailed information about a specific product. The page is generated based on data retrieved from APIs using `getProductById` and `getSimilarProducts` functions.
-The component features:
-1. **Product Image**: A large image of the product.
-2. **Product Info Card**: Displays essential product details, including title, category, price, rating, reviews, and quantity.
-3. **Price Information Cards**: Provides additional price-related information, such as current, average, highest, and lowest prices.
-4. **Modal**: A modal window that can be opened to view more detailed information about the product.
-5. **Product Description**: Displays a brief description of the product.
-6. **Seller Details**: Shows details about the seller who offers the product, including name and positive rating.
-7. **Buy Now and Visit Shop buttons**: Links to purchase the product or visit the seller's shop.
-The page also displays similar products recommended by the system using `getSimilarProducts` function.
-Overall, this code is designed to create a detailed and informative product details page that showcases essential information about a specific product and its related features.</t>
+          <t>**Code Summary**
+The provided code is a React component named `ProductDetails` that displays detailed information about a specific product. It fetches the product data from an API using the `getProductById` function and displays various details such as:
+* Product image
+* Title, category, and description
+* Price information (current price, average price, highest price, lowest price)
+* Seller details (name, positive seller rating)
+* Similar products (a list of related products with their own cards)
+The component uses various custom components like `PriceInfoCard`, `ProductCard`, and `Modal` to display the product information.
+**Key Features**
+* Fetches product data from an API using `getProductById`
+* Displays detailed product information, including price, seller details, and similar products
+* Uses custom components for price and product cards
+* Handles pagination and lazy loading of similar products
+**Deployment Context**
+This code is likely used in a web application that showcases products with their detailed information. It can be deployed on a Next.js or other React-based framework to display product pages.</t>
         </is>
       </c>
     </row>
@@ -642,18 +650,16 @@
       <c r="B10" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Component:** `HeroCarousel`
-**Purpose:** Display a carousel of images with hero product images
-**Key Features:**
-1. Uses React and Next.js
-2. Imports Carousel component from react-responsive-carousel library
-3. Defines an array of image objects (`heroImages`) with src, alt, and other attributes
-4. Renders the carousel with auto-play and infinite loop features
-5. Displays a custom arrow icon above the carousel using Image component
-6. Maps through `heroImages` array to render each image in the carousel
-**Notable CSS classes:**
-1. `.max-xl:hidden`: Hides the element on large screens
-2. `object-contain`: Maintains aspect ratio of images within the carousel</t>
+**Component:** HeroCarousel
+**Purpose:** A responsive hero image carousel component for a web application.
+**Features:**
+* Displays a series of images in a carousel format
+* Uses the React Responsive Carousel library
+* Automatically loops through the images with an interval of 2 seconds
+* Does not show navigation arrows or status bar
+* Custom icon (hand-drawn arrow) is displayed at the bottom left corner
+**Images:** The component uses an array of image objects (`heroImages`) which contain the `imgUrl` and `alt` properties for each image.
+This summary should give you a high-level understanding of what the code does!</t>
         </is>
       </c>
     </row>
@@ -666,21 +672,22 @@
       <c r="B11" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Overview**
-The code defines a React component called `Modal` that displays a dialog box with a form to collect an email address from users. The dialog can be opened by clicking on a "Track" button.
-**Key Features**
-* A state management system using `useState` hook to manage the dialog's open status, submission status, and input value.
-* An asynchronous function `handleSubmit` that submits the form data to the server when the user clicks the "Track" button. The function calls an API endpoint `addUserEmailToProduct` to add the user's email address to a product.
-* A modal dialog box with a logo, close button, and a form containing a label, input field, and submit button.
-* Transition effects are used to smoothly open and close the modal.
-**Imported Libraries**
-* React
-* `useState` from React
-* `Fragment`, `FormEvent`, and other components from React
-* `Dialog`, `Transition` from Headless UI library
-* Image component from Next.js
-**Props**
-The component expects a single prop `productId` which is a string.</t>
+**Purpose:** The `Modal` component displays a dialog box that allows users to enter their email address and receive product pricing alerts.
+**Features:**
+1. **Button trigger**: A "Track" button opens the modal.
+2. **Modal content**: The modal contains a form with an input field for the user's email address, a submit button, and a close icon.
+3. **Email submission**: When the submit button is clicked, the `handleSubmit` function sends the email address to the server using the `addUserEmailToProduct` API.
+4. **Loading state**: While submitting the form, a "Submitting..." text is displayed on the submit button.
+5. **Closing the modal**: Clicking the close icon or pressing Esc closes the modal.
+**Components and Libraries:**
+1. `React` for building user interfaces
+2. `useState` from React for managing state
+3. `@headlessui/react` for creating a responsive, accessible modal dialog box
+4. `Image` component from `next/image` for displaying images
+5. `addUserEmailToProduct` API function for submitting email addresses to the server
+**Key Functions:**
+1. `handleSubmit`: Handles form submission and sends email address to the server.
+2. `openModal` and `closeModal`: Toggle the modal's open state.</t>
         </is>
       </c>
     </row>
@@ -692,18 +699,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Here is a summary of the provided code:
-**File:** Navbar component for a Next.js application.
-**Purpose:** To render a responsive navigation bar with a logo and icons.
+          <t>Here is a summary of the code:
+**File:** React component file ( likely `Navbar.js`)
+**Purpose:** To render a navigation bar with logo, icons, and links.
 **Key Features:**
-1. **Logo Section**: Displays a Daraz logo with "Scrapper" text.
-2. **Icon Section**: Renders three navigational icons (Search, Heart, User) from an array of objects (`navIcons`).
-3. **Navigation Links**: Each icon is wrapped in a `Link` component to facilitate navigation between pages.
-**Components Used:**
-1. `Image` from `next/image` for displaying the logo and icons.
-2. `Link` from `next/link` for creating navigational links.
-3. React functional components (`Navbar`) for rendering the navbar.
-Overall, this code defines a reusable Navbar component that can be imported and used throughout a Next.js application.</t>
+* A logo image displayed alongside the brand name "Daraz Scrapper"
+* Three icons (search, heart, user) displayed in a row
+* Links to the homepage (`/`) for each icon
+**Libraries Used:**
+* `next/image` for image handling
+* `next/link` for client-side routing
+* React for building the UI component</t>
         </is>
       </c>
     </row>
@@ -716,15 +722,17 @@
       <c r="B13" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Code Summary**
-The code defines a reusable React component called `PriceInfoCard`. It takes three props: `title`, `iconSrc`, and `value`. The component renders a card with the following layout:
-* A title text
-* An icon image (with width and height specified) next to a value text, which is displayed in bold font.
-* Both the icon and value are contained within a flex container.
-**Key Features**
-* Uses Next.js's `Image` component for image rendering
-* Customizable props for title, icon source, and value text
-* Flexible layout using CSS classes (e.g. `flex`, `gap-1`)</t>
+**Component:** `PriceInfoCard`
+**Functionality:** Displays a card with a title, icon, and value.
+**Props:**
+* `title`: string (card title)
+* `iconSrc`: string (path to icon image)
+* `value`: string (displayed value)
+**HTML Structure:**
+* A container `&lt;div&gt;` with class `price-info_card`
+	+ A `&lt;p&gt;` element displaying the `title`
+	+ A flexible container (`&lt;div&gt;`) with an `Image` component displaying the `iconSrc` and a second `&lt;p&gt;` element displaying the `value`
+This code appears to be a reusable React component, likely used in a Next.js application.</t>
         </is>
       </c>
     </row>
@@ -736,17 +744,14 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Here is a summary of the code:
-**ProductCard Component**
-The `ProductCard` component displays information about a product from a database. It takes a `product` object as a prop and renders a card with the following details:
-* A link to the product's page
-* An image of the product
-* The product title
-* The product category (limited to 2 categories)
-* The product price, including currency
-The component uses Next.js's built-in `Link` and `Image` components, as well as React hooks. It exports a default instance of the component.
-**Props**
-The component expects a single prop: `product`, which must be an object conforming to the `Product` type from `@/types`. The product object should have properties for `_id`, `image`, `title`, `category`, and `currentPrice`.</t>
+          <t>**Code Summary**
+The `ProductCard` component is a React functional component that displays information about a product. It takes a single prop, `product`, of type `Product`, which is imported from the `@/types` module.
+The component renders:
+1. A link to the product's details page using `Link` from `next/link`.
+2. An image container with an `Image` component from `next/image`, displaying the product's image.
+3. Product title and description in a card layout.
+4. Product category and current price, formatted for display.
+The code uses Next.js-specific features such as `Link` and `Image` components, as well as CSS classes for styling. It also utilizes TypeScript type checking through the `Product` interface.</t>
         </is>
       </c>
     </row>
@@ -759,17 +764,19 @@
       <c r="B15" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Searchbar Component**
-This React component allows users to search for products on Daraz.com by entering a product URL. It consists of:
-* An input field where users can enter a Daraz product URL
-* A submit button that triggers the search process when clicked
-* Validation logic to ensure the entered URL is valid (i.e., belongs to Daraz)
-* An API call (`scrapeAndStoreProduct`) to scrape and store product information from the provided URL
-* Navigation to a new page with the product details upon successful search
-**Key Features**
-* Uses `useState` to manage local state for input field value and loading indicator
-* Utilizes Next.js's `useRouter` hook to navigate to a new page with product details
-* Employes error handling and logging using `try-catch-finally` blocks</t>
+**Component:** `Searchbar`
+**Functionality:** A search bar component that allows users to input a Daraz product URL and submit it for scraping and storing.
+**Key Features:**
+1. **Validation**: The component checks if the input URL is valid by calling the `isValidDarazProductURL` function, which uses URL parsing to verify the URL belongs to daraz.com.
+2. **Scraping and Storage**: If the URL is valid, the component calls the `scrapeAndStoreProduct` function from a separate file (`@/lib/action`) to scrape product data from the input URL and store it.
+3. **Loading Indicator**: While scraping and storing, the component displays a "Searching..." message on the button.
+4. **Routing**: After successful scraping and storage, the component redirects the user to a new page with the scraped product ID using Next.js's `router.push` method.
+**State Management:**
+* The component uses React's `useState` hook to manage two state variables:
+	+ `searchPrompt`: stores the input URL
+	+ `isLoading`: tracks whether scraping and storage is in progress
+**Event Handling:**
+* The component listens for a form submission event (`handleSubmit`) and calls the `scrapeAndStoreProduct` function when the submit button is clicked.</t>
         </is>
       </c>
     </row>
@@ -781,23 +788,23 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Here is a summary of the provided code:
-**Functionality**
-The code provides several functions for interacting with a MongoDB database to store and retrieve product data. It uses Next.js's built-in caching feature.
-**Functions**
-1. `scrapeAndStoreProduct(productUrl: string)`: Scrape product data from Daraz using `scrapeDarazProduct` function, and then store or update the product in the database based on its URL.
-2. `getProductById(productId: string)`: Retrieve a product by its ID from the database.
-3. `getAllProducts()`: Return all products from the database.
-4. `getSimilarProducts(productId: string)`: Find similar products (up to 3) excluding the one with the given ID.
-5. `addUserEmailToProduct(productId: string, userEmail: string)`: Add a user's email to a product in the database and send a welcome email to that user.
+          <t>Here is a summary of the code:
+**Overview**
+This code appears to be a part of a Next.js application that interacts with a MongoDB database. It provides functions for scraping product data from Daraz, storing and updating product information in the database, retrieving products by ID or all products, finding similar products, and adding user email addresses to specific products.
+**Key Functions**
+1. `scrapeAndStoreProduct`: Scrapes product data from Daraz, updates existing product records in the database if necessary, and revalidates the cache.
+2. `getProductById`: Retrieves a single product by its ID from the database.
+3. `getAllProducts`: Returns all products stored in the database.
+4. `getSimilarProducts`: Finds up to 3 similar products (excluding the specified product) and returns them.
+5. `addUserEmailToProduct`: Adds a user's email address to a specific product, sends a welcome email if necessary.
 **Dependencies**
-The code uses:
-* `next/cache` for caching
-* `mongoose` for interacting with MongoDB
-* `../models/product.model` for defining the Product model
-* `../utils` for utility functions (getAveragePrice, getHighestPrice, getLowestPrice)
-* `../scrapper` for scraping product data from Daraz
-* `../nodemailer` for sending emails</t>
+The code uses the following dependencies:
+* `next/cache` for revalidating cache paths
+* `mongoose` for interacting with the MongoDB database
+* `scrapeDarazProduct` for scraping product data from Daraz
+* `generateEmailBody` and `sendEmail` for sending emails using nodemailer
+**Error Handling**
+The code catches errors, logs them to the console, and throws a new error message if necessary.</t>
         </is>
       </c>
     </row>
@@ -809,19 +816,19 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Here is a summary of the code:
-**Database Schema Definition**
-This code defines a MongoDB database schema using Mongoose, a popular ODM (Object-Document Mapping) library for Node.js. The schema represents a `Product` document with various fields, including:
+          <t>Here is a summary of the provided code:
+**Mongoose Model Definition**
+The code defines a Mongoose model named `Product` using a schema. The schema has multiple fields, including:
 * Basic product information (url, currency, image, title, category)
-* Pricing and discount-related fields (currentPrice, originalPrice, priceHistory, discountRate)
-* Review and rating metrics (reviewsCount, rateCount, reviewScores)
-* Stock management (productQuantityValue, isOutOfStock)
-* Seller information (sellerShopName, sellerShopURL, positiveSellerRating)
-* User associations (users)
-* Price ranges (lowestPrice, highestPrice, averagePrice)
+* Pricing and sales history (currentPrice, originalPrice, priceHistory)
+* Product reviews and ratings (reviewsCount, rateCount, reviewScores)
+* Inventory and stock status (isOutOfStock, productQuantityValue)
+* Seller information (productBrand, sellerShopName, sellerShopURL, positiveSellerRating)
+* User interactions (users)
+* Price statistics (lowestPrice, highestPrice, averagePrice)
+The model also includes default values for certain fields, such as `date` and `isOutOfStock`.
 **Exported Model**
-The schema is then used to define a Mongoose model named `Product`, which is exported as the default export of this module. This allows other parts of the application to interact with the database using this model.
-Overall, this code sets up a robust and feature-rich data structure for storing product information in a MongoDB database.</t>
+The code exports the defined `Product` model, making it available for use in other parts of the application.</t>
         </is>
       </c>
     </row>
@@ -833,12 +840,9 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>**Database Connection Function**
-The `connectToDB` function establishes a connection to a MongoDB database using the Mongoose library. Here's a summary of its functionality:
-* It checks if a `MONGODB_URI` environment variable is defined and logs an error if not.
-* If a connection already exists (`isConnected === true`), it logs a message indicating that the existing connection will be used.
-* Otherwise, it attempts to connect to the database specified by the `MONGODB_URI` environment variable using Mongoose. On success, it sets `isConnected` to `true` and logs a success message.
-This function is designed to be called from other parts of the application to ensure that a connection to the MongoDB database is established before performing any data-related operations.</t>
+          <t>Here is a summary of the code:
+**Database Connection Manager**
+This code manages connections to a MongoDB database using Mongoose. It checks for an existing connection and establishes a new one if needed, logging errors and success messages. The connection is established using the `MONGODB_URI` environment variable, which must be defined for the connection to succeed.</t>
         </is>
       </c>
     </row>
@@ -850,23 +854,19 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>**Code Summary**
-This code is a notification system that generates and sends emails to users based on various product-related events. It uses the Nodemailer library to send emails.
-**Key Features**
-1. **Notification Types**: The code defines four types of notifications:
-	* `WELCOME`: Welcome email for new users.
-	* `CHANGE_OF_STOCK`: Email notification when a product is back in stock.
-	* `LOWEST_PRICE`: Lowest price alert for products.
-	* `THRESHOLD_MET`: Discount alert when a product's price drops below a certain threshold.
-2. **Email Generation**: The code generates email bodies and subjects based on the notification type using a switch statement.
-3. **Email Sending**: The code uses Nodemailer to send emails to users.
-**Key Functions**
-1. `generateEmailBody(product, type)`: Generates an email body and subject for a given product and notification type.
-2. `sendEmail(emailContent, sendTo)`: Sends an email to the specified recipients using the generated email content.
-**Key Variables**
-1. `Notification`: An object containing the four types of notifications.
-2. `transporter`: A Nodemailer transporter instance used to send emails.
-Overall, this code provides a basic notification system that can be extended and customized as needed.</t>
+          <t>Here's a summary of the provided code:
+**Purpose**: This code is designed to generate and send email notifications for price tracking and stock updates.
+**Features**:
+1. It uses the `nodemailer` library to create an email transporter.
+2. It defines a `Notification` enum with four types: WELCOME, CHANGE_OF_STOCK, LOWEST_PRICE, and THRESHOLD_MET.
+3. The `generateEmailBody` function takes in product information (`product`) and notification type (`type`) as inputs and returns a subject and body for an email based on the specified type.
+4. It uses a switch statement to determine which template to use for each notification type.
+5. The `sendEmail` function sends the generated email using the transporter, taking in email content (`emailContent`) and recipient addresses (`sendTo`) as inputs.
+**Key Components**:
+1. `generateEmailBody`: This is the core function that generates the email subject and body based on the product information and notification type.
+2. `Notification` enum: Defines the four notification types used in the code.
+3. `nodemailer` transporter: Creates an email transporter using the specified configuration.
+**Context**: This code appears to be part of a larger application that provides price tracking and stock updates for products, likely using a database or API to retrieve product information.</t>
         </is>
       </c>
     </row>
@@ -878,18 +878,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>**Function Summary**
-The `scrapeDarazProduct` function is an asynchronous function that scrapes product information from the Daraz website. It takes a URL as input, attempts to extract various product details using Cheerio and Axios, and returns a Promise resolving to a Product object or undefined if no product data was found.
-**Extracted Information**
-The function extracts the following information:
-1. Seller shop name, URL, and positive seller rating
-2. Product title, description, brand, categories, image, and tag
-3. Review ratings (average, count, scores)
-4. Product price history (original, sale, lowest, highest, average)
-5. Discount rate and availability of product stock
-**Error Handling**
-The function catches any errors that occur during execution and throws a new Error with the message "Failed to scrape Daraz Product: &lt;error_message&gt;".
-Note: The `scrapeDarazProduct` function appears to be used for extracting product data from Daraz, but it's not clear what specific requirements or use cases are driving this code. If you have more context about the project or its goals, I'd be happy to help further!</t>
+          <t>Here is a summary of the code:
+**Functionality:** The `scrapeDarazProduct` function scrapes product information from the Daraz website using web scraping techniques.
+**Key Features:**
+1. **Authentication**: The function uses environment variables (`BRIGHT_DATA_USERNAME` and `BRIGHT_DATA_PASSWORD`) to authenticate with a proxy server.
+2. **Data Extraction**: The function extracts data from the HTML content of a webpage, specifically from a script tag that contains JSON-formatted data.
+3. **Product Information**: The function extracts various product information, including:
+	* Product title
+	* Description
+	* Price (original and sale)
+	* Currency code
+	* Image URL
+	* Categories
+	* Reviews count and rating
+	* Availability (in-stock or out-of-stock)
+	* Seller information (name, URL, rating)
+4. **Data Return**: The function returns a `Product` object containing the extracted data.
+**Error Handling:**
+The function catches any errors that occur during execution and throws a new error with a descriptive message.
+Note that this summary is based on my understanding of the code and may not be exhaustive or entirely accurate. If you have specific questions about the code, I'd be happy to try and help!</t>
         </is>
       </c>
     </row>
@@ -901,21 +908,18 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Here is a summary of the code:
-**Overview**
-The code provides a set of utility functions for extracting and manipulating data from web pages, particularly related to product pricing information. The functions are designed to work with a specific framework ( likely Cypress) and utilize jQuery-like selectors.
-**Functions**
-1. `extractPrice`: Extracts and returns the price from a list of possible elements on a web page.
-2. `extractCurrency`: Extracts and returns the currency symbol from an element.
-3. `extractDescription`: Extracts description text from two possible elements on a web page (e.g., Daraz).
-4. `getHighestPrice` and `getLowestPrice`: Returns the highest or lowest price from a list of price history items.
-5. `getAveragePrice`: Calculates and returns the average price from a list of price history items.
-6. `getEmailNotifType`: Determines the type of email notification to send based on changes in product pricing information (e.g., lowest price, stock availability).
-7. `formatNumber`: Formats a number as a string with decimal places.
-**Key Concepts**
-* The code uses a set of predefined constants (`Notification`) for email notification types and a threshold percentage value.
-* The functions are designed to work with a specific framework (Cypress) and utilize jQuery-like selectors.
-* The code assumes the presence of certain HTML elements on the web page, such as `.a-unordered-list .a-list-item` and `.a-expander-content p`.</t>
+          <t>Here is a summary of the provided code:
+**Purpose:** The code appears to be part of a web scraping project that extracts product information from online marketplaces (likely Daraz) and performs various calculations on the extracted data.
+**Functions:**
+1. **`extractPrice`**: Extracts the price of a product from a list of possible HTML elements.
+2. **`extractCurrency`**: Extracts the currency symbol from an HTML element.
+3. **`extractDescription`**: Extracts the description of a product from two possible HTML elements (`.a-unordered-list .a-list-item` and `.a-expander-content p`).
+4. **`getHighestPrice`, `getLowestPrice`, and `getAveragePrice`**: Calculate the highest, lowest, and average prices of a product based on its price history.
+5. **`getEmailNotifType`**: Determines the type of email notification to send based on changes in product availability, price, or discount rate.
+6. **`formatNumber`**: Formats a number with commas as thousand separators.
+**Types:**
+The code imports various types from `@/types`, including `Price`, `PriceHistoryItem`, and `Product`.
+Overall, the code provides a set of utility functions for extracting and processing product information, which can be used in a larger web scraping project.</t>
         </is>
       </c>
     </row>
@@ -928,14 +932,15 @@
       <c r="B22" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Next.js Configuration**
-The code exports a `nextConfig` object that configures Next.js for a project. The configuration enables two experimental features:
-* `serverActions`: allows server-side rendering and API routes to be executed on the server.
-* `serverComponentsExternalPackages`: specifies an array of external packages, including "mongoose", which can be used in server components.
-Additionally, the code sets up image handling by specifying allowed domains for images, including:
-* `static-01.daraz.com`
-* `static-01.daraz.com.np` and `np-live-21.slatic.net`
-This configuration is then exported using `module.exports = nextConfig;`.</t>
+**Next.js Configuration File**
+This code exports a Next.js configuration object (`nextConfig`) that enables experimental features and customizes image loading.
+**Key Features:**
+1. **Experimental Server Actions**: Enables server actions in Next.js, allowing for more complex server-side rendering.
+2. **External Packages**: Allows the use of external packages (in this case, `mongoose`) with server components.
+3. **Image Loading Configuration**:
+	* Specifies allowed image domains (`static-01.daraz.com`, `static-01.daraz.com.np`, and `np-live-21.slatic.net`).
+4. **Exports**: Exports the `nextConfig` object as a module, making it available for use in other parts of the application.
+Let me know if you'd like me to elaborate on any specific aspect!</t>
         </is>
       </c>
     </row>
@@ -947,14 +952,14 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>This is a JSON object containing information about installed npm packages. It includes details such as the package name, version, resolved URL, integrity hash, and dependencies for each package.
-Here are some key points from this output:
-* There are 17 packages installed.
-* The oldest package is `assert` (version 2.0.0) which was last updated in 2016.
-* The newest package is `whatwg-url` (version 11.0.0).
-* Some packages have dependencies that require specific versions of other packages, such as `watchpack` which requires `glob-to-regexp` and `graceful-fs`.
-* There are no packages with known security vulnerabilities.
-If you'd like me to extract any specific information from this output or provide further analysis, please let me know!</t>
+          <t>The provided JSON output appears to be a package manifest, likely generated by `npm ls` or another dependency manager. It lists various dependencies installed in a project, along with their versions and source information.
+Here are the main points summarized from this output:
+1. The project has many dependencies listed, including `@babel/core`, `ansi-styles`, `cross-spawn`, `glob`, `json-schema`, etc.
+2. Each dependency is identified by its name, version number, resolved URL (i.e., the location of the package on npm), and integrity hash (a unique digital signature for verification purposes).
+3. Some dependencies have additional information listed under a "requires" section, indicating that they depend on specific versions of other packages.
+4. The list also includes some development-only dependencies (marked as `dev: true` in the output), such as `eslint`, `jest`, and `yaml`.
+5. Overall, this output provides detailed information about the project's dependency tree, allowing you to identify any potential issues or upgrade opportunities for your project.
+If you'd like me to extract specific details from this output, please let me know what you're looking for!</t>
         </is>
       </c>
     </row>
@@ -966,27 +971,22 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Here is a summary of the code:
-**Package Information**
-* Name: darazscan
-* Version: 0.1.0
-* Private package (not intended for public use)
-**Scripts**
-* Four scripts are defined:
-	+ `dev`: runs the Next.js development server
-	+ `build`: builds the Next.js application
-	+ `start`: starts the Next.js server in production mode
-	+ `lint`: runs linter checks on the code
-**Dependencies**
-* 10 packages are listed as dependencies:
-	+ Libraries for UI components, APIs, and email sending
-	+ Packages for MongoDB interaction (Mongoose) and file processing (Cheerio)
-	+ Next.js and React libraries for building the application
-**Dev Dependencies**
-* 7 packages are listed as development dependencies:
-	+ TypeScript compiler and type definitions for Node.js and other libraries
-	+ PostCSS and Tailwind CSS for styling and layout
-	+ Autoprefixer for adding vendor prefixes to CSS rules</t>
+          <t>**Package Summary**
+This is a `package.json` file, which contains metadata for a JavaScript project. Here's a summary of the contents:
+* **Project Name**: darazscan (version 0.1.0)
+* **Type**: Private development project
+* **Scripts**: Defined scripts for:
+	+ Development: `next dev`
+	+ Building: `next build`
+	+ Starting: `next start`
+	+ Linting: `next lint`
+* **Dependencies**:
+	+ Various JavaScript libraries and frameworks, including React, Next.js, Mongoose, Axios, and others (version 13.5.5 or higher)
+* **Dev Dependencies**:
+	+ TypeScript and related type definitions
+	+ Autoprefixer and PostCSS for CSS processing
+	+ Tailwind CSS for styling
+This package appears to be a web development project built with Next.js, using React and other JavaScript libraries for functionality and styling.</t>
         </is>
       </c>
     </row>
@@ -998,10 +998,10 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>This code exports an object that configures a set of CSS plugins for use with Webpack or another module bundler. The two plugins being used are:
-* `tailwindcss`: This is the configuration file for Tailwind CSS, a utility-first CSS framework.
-* `autoprefixer`: This plugin automatically adds vendor prefixes to CSS rules, ensuring compatibility across different browsers.
-In summary, this code sets up and exports configurations for two common CSS plugins used in web development.</t>
+          <t>This code is a configuration file for a CSS build tool, likely Webpack or a similar tool. It exports an object that specifies two plugins to be used in the build process:
+1. **Tailwind CSS**: A utility-first CSS framework.
+2. **Autoprefixer**: A plugin that adds vendor prefixes to CSS properties automatically.
+In summary, this code sets up Tailwind CSS and Autoprefixer as plugins for a CSS build tool.</t>
         </is>
       </c>
     </row>
@@ -1014,17 +1014,28 @@
       <c r="B26" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Tailwind CSS Configuration**
-This configuration file specifies settings for a Tailwind CSS project. It defines:
-* **Content**: The files to scan for classes, including JavaScript and TypeScript files in the `pages`, `components`, and `app` directories.
-* **Theme**: Customizes the default Tailwind CSS theme by extending its features:
-	+ **Colors**: Defines custom color palettes (`primary`, `secondary`, etc.) with specific hex codes.
-	+ **Box Shadow**: Adds a new box shadow variant (`xs`) with a specific style.
-	+ **Max Width**: Sets a maximum width of 1440px for the `10xl` class.
-	+ **Font Family**: Specifies two custom font families (`inter` and `spaceGrotesk`).
-	+ **Border Radius**: Defines a new border radius value (`10`) with a specific style.
-* **Plugins**: Currently, no plugins are enabled.
-Overall, this configuration file sets up a customized Tailwind CSS project with tailored colors, fonts, and styles.</t>
+This is a Tailwind CSS configuration file that defines the content, theme, and plugins for a React application.
+**Content**
+* Specifies which files to scan for Tailwind classes:
+	+ Pages (`./pages/**/*.{js,ts,jsx,tsx,mdx}`)
+	+ Components (`./components/**/*.{js,ts,jsx,tsx,mdx}`)
+	+ App (`./app/**/*.{js,ts,jsx,tsx,mdx}`)
+**Theme**
+* Defines custom color palette:
+	+ Primary colors: `#E43030`, `#D48D3B`, and `#3E9242`
+	+ Secondary color: `#282828`
+	+ Grays: various shades from `#EAECF0` to `#101828`
+	+ Whites and blacks: `#F4F4F4`, `#EDF0F8`, `#3D4258`, and `#23263B`
+* Defines a custom box shadow:
+	+ Small (`xs`): `0px 1px 2px 0px rgba(16, 24, 40, 0.05)`
+* Defines custom max-width:
+	+ "10xl": `1440px`
+* Defines font families:
+	+ Inter and Space Grotesk
+* Defines a custom border radius:
+	+ 10: `"10px"`
+**Plugins**
+* No plugins are enabled in this configuration.</t>
         </is>
       </c>
     </row>
@@ -1036,15 +1047,22 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>This code is a configuration file for a TypeScript compiler, likely used in a Next.js project. It defines the options and settings for compiling and building the project.
-Here's a brief summary of the key points:
-* The target environment is set to ES5.
-* Various libraries are included, and strict type checking is enabled.
-* No emit or module resolution is performed, suggesting a bundler-based approach.
-* ESNext modules are used, with ES6 imports allowed through ESModuleInterop.
-* A plugin named "next" is applied.
-* Specific paths are defined for resolving modules and types.
-Overall, this configuration suggests a development setup that prioritizes Next.js compatibility, TypeScript type safety, and efficient module resolution.</t>
+          <t>This code is a JSON configuration file for a TypeScript compiler, specifically targeting an ES5 ( ECMAScript 5) environment. It includes the following settings:
+* Compiler options:
+	+ Targets ES5 syntax
+	+ Includes DOM and iterable libraries
+	+ Allows JavaScript files to be compiled
+	+ Disables library checking
+	+ Enables strict mode
+	+ Suppresses code emission (i.e., no output file will be generated)
+	+ Enables interoperability between CommonJS and ES modules
+	+ Uses the "bundler" module resolution strategy
+	+ Resolves JSON modules
+	+ Compiles files in isolation
+	+ Preserves JSX syntax
+* Includes all files with .ts, .tsx, or .d.ts extensions, as well as specific Next.js environment configuration files.
+* Excludes node_modules directory.
+This configuration is likely used for a Next.js project to compile TypeScript code with specific settings.</t>
         </is>
       </c>
     </row>
@@ -1057,24 +1075,21 @@
       <c r="B28" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Data Types**
-The code defines several data types using TypeScript:
-1. `PriceHistoryItem`: an object with a single property `price` of type `Price`.
-2. `User`: an object with a single property `email` of type string.
-3. `Product`: a comprehensive object representing a product, with numerous properties such as:
-	* `_id`, `url`, `currency`, `image`, `title`, and `category` for general product information
-	* `currentPrice`, `originalPrice`, `priceHistory`, `discountRate`, and `reviews` for pricing and review-related data
-	* `productQuantityValue`, `stars`, and `isOutOfStock` for product quantity, rating, and stock status
-	* `sellerShopName`, `sellerShopURL`, and `positiveSellerRating` for seller information
-4. `NotificationType`: an enum type with four possible values:
-	* "WELCOME"
-	* "CHANGE_OF_STOCK"
-	* "LOWEST_PRICE"
-	* "THRESHOLD_MET"
-5. `EmailContent`: an object with two properties: `subject` and `body`, both of type string.
-6. `EmailProductInfo`: an object with two properties: `title` and `url`, both of type string.
-7. `Price`: an object with two properties: `text` and `value`, where `value` is a number.
-These data types are designed to represent various entities in an e-commerce application, such as products, users, notifications, and email contents.</t>
+**Types Summary**
+This code defines several types related to e-commerce and notifications. The main types are:
+1. **PriceHistoryItem**: A single item in a product's price history, containing a `price` property.
+2. **User**: An object representing a user, with an `email` property.
+3. **Product**: An object representing a product, containing various properties such as:
+	* Product metadata (e.g., `_id`, `url`, `currency`, etc.)
+	* Pricing information (e.g., `currentPrice`, `originalPrice`, `priceHistory`)
+	* Review and rating information
+	* Seller information
+4. **NotificationType**: An enumeration of possible notification types, including welcome messages, stock changes, lowest price notifications, and threshold met notifications.
+5. **EmailContent**: An object containing email subject and body text.
+6. **EmailProductInfo**: An object containing product title and URL for an email.
+7. **Price**: An object representing a price, with `text` and `value` properties.
+**Key Features**
+The code uses TypeScript types to define the structure of these objects. The types are designed to be used in a Node.js or similar environment. The emphasis on product pricing, review, and rating information suggests an e-commerce application.</t>
         </is>
       </c>
     </row>
@@ -1086,12 +1101,11 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>This JSON object contains a configuration for a cron job.
-* The key "crons" is an array containing one object.
-* This single object has two properties:
-	+ "path": The URL path where the cron job will be executed, which is "/api/cron".
-	+ "schedule": The schedule at which the cron job will run, which is set to 30 minutes past 13:00 (1:30 PM) every day, as represented by the cron expression "* * * * 13".
-In summary, this code sets up a single cron job that runs once daily at 1:30 PM and executes an API request at "/api/cron".</t>
+          <t>The provided code is a JSON object that defines a single cron job configuration. Here's a summary:
+**Cron Job Configuration**
+* The path for the cron job is `/api/cron`.
+* The schedule specifies that the task should run at 13:30 (1:30 PM) every day, as represented by the `30 13 * * *` format.
+In short, this code sets up a daily cron job to run at 1:30 PM.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated clone_github.py to comment out .git folder removal, uncommented badge URLs in project_badge.py, and modified binary files in __pycache__ and output directories.
</commit_message>
<xml_diff>
--- a/output/Daraz_Scraper_summary.xlsx
+++ b/output/Daraz_Scraper_summary.xlsx
@@ -453,12 +453,8 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>I can't provide a summary of the given code as it doesn't seem to be present in your message. However, I can guide you on how to summarize code.
-If you provide the code snippet, I'll be happy to help you with a summary. The summary will include:
-* Key variables and their purposes
-* Main functions or methods and their descriptions
-* Notable data structures used
-Please share the code so I can assist you better.</t>
+          <t>It appears there is no code provided for me to summarize. The text only contains environment variable names and placeholders.
+If you could provide the actual code, I would be happy to assist with summarizing it.</t>
         </is>
       </c>
     </row>
@@ -470,16 +466,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>This code is a `.gitignore` file, which lists files and directories that should be ignored by Git.
-Here's a summary:
-The file ignores various types of files and directories, including:
-* Dependencies (e.g., `/node_modules`)
-* Testing and build artifacts (e.g., `/coverage`, `/.next/`, `/build`)
-* Local environment files (e.g., `.env*.local`)
-* Debugging logs (e.g., `npm-debug.log*`)
-* Vercel-related files (e.g., `.vercel`)
-* TypeScript-specific files (e.g., `*.tsbuildinfo`)
-These ignores are likely used in a Next.js project to exclude unnecessary files from version control.</t>
+          <t>**File Ignore List Summary**
+This code snippet appears to be a `.gitignore` file, used to specify files and directories that should be ignored by Git. The list is organized into sections based on the type of files being ignored:
+1. **Dependencies**: `node_modules`, `.pnp`, and `.pnp.js`
+2. **Testing**: `/coverage` directory
+3. **Next.js**: `.next/` directory and `/out/` directory
+4. **Production**: `/build` directory
+5. **Miscellaneous**: `.DS_Store` file, PEM files (`.pem`), and log files (`npm-debug.log*`, `yarn-debug.log*`, `yarn-error.log*`)
+6. **Local Environment Files**: environment files with the suffix `.env.local`
+7. **Vercel**: `.vercel` directory
+8. **TypeScript**: `*.tsbuildinfo` file and `next-env.d.ts` file
+These ignored files and directories will not be tracked by Git, helping to keep the repository's history clean and focused on actual project code.</t>
         </is>
       </c>
     </row>
@@ -491,26 +488,33 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>**DarazScrapper**
-A Next.js web application that scrapes product details from Daraz, tracks price changes, and notifies users when specific conditions are met. The app uses MongoDB for data storage and Bright Data for efficient scraping.
+          <t>Here's a summary of the code:
+**DarazScrapper**
+A web application built with Next.js that scrapes product details from Daraz, tracks price changes, and notifies users when specific conditions are met. It uses MongoDB for data storage and Bright Data for efficient scraping.
 **Key Features:**
-1. **Price Tracking**: Records highest and lowest prices for products over time.
-2. **Notification System**: Sends alerts when price drops below a set threshold.
-3. **Web Scraping**: Extracts product details like name, price, and rating.
-4. **Cron Jobs**: Schedules scraping tasks to run periodically.
+* Price tracking: records highest and lowest prices for products over time
+* Notification system: sends alerts when price drops below a set threshold
+* Web scraping: extracts product details like name, price, and rating
+* Cron jobs: schedules scraping tasks to run periodically
 **Technologies Used:**
-1. Next.js (React framework for server-side rendering)
-2. MongoDB (NoSQL database for storing scraped data)
-3. Bright Data (Data collection and web scraping tool)
-4. Node.js (Server-side environment)
-5. Tailwind CSS (Utility-first CSS framework)
-**Installation and Usage:**
-1. Clone the repository.
-2. Install dependencies using npm or Yarn.
-3. Set up environment variables in a `.env.local` file.
-4. Start the development server using `npm run dev`.
-5. Add product URLs to scrape, and the app will track prices and notify users of changes.
-**Live Demo:** [https://daraz-scraper.vercel.app/](https://daraz-scraper.vercel.app/)</t>
+* Next.js (React framework)
+* MongoDB (NoSQL database)
+* Bright Data (data collection and web scraping tool)
+* Node.js (server-side environment)
+* Tailwind CSS (utility-first CSS framework)
+**Prerequisites:**
+* Node.js v14 or higher
+* npm or Yarn
+* MongoDB instance
+**Installation:**
+1. Clone the repository
+2. Install dependencies
+3. Set up environment variables
+4. Start the development server
+**Usage:**
+1. Add the URL of the product you want to scrape
+2. The app will automatically track the price and notify you of any significant changes.
+This code is well-structured, readable, and follows good practices in terms of documentation and contribution guidelines.</t>
         </is>
       </c>
     </row>
@@ -522,20 +526,21 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Here is a summary of the code:
-**Functionality:** This Next.js API endpoint performs a cron job-style task that scrapes product details from Daraz and updates the corresponding database records. It also sends email notifications based on specific conditions.
-**Main Steps:**
-1. Connects to the database using `connectToDB()`.
+          <t>Here's a summary of the code:
+**Functionality:** This is a Next.js API route that runs periodically ( likely using a cron job or corn job ) to update product information in a database and send email notifications based on changes.
+**Key Steps:**
+1. Connects to the database.
 2. Retrieves all products from the database.
-3. Loops through each product, scraping its latest details using `scrapeDarazProduct()`.
-4. Updates the product's price history and calculates lowest, highest, and average prices using helper functions.
-5. Updates the product record in the database.
-6. Checks each product's status and sends an email notification if necessary.
-**Key Functions:**
-* `GET(request)`: The main API endpoint function that handles the cron job task.
-* `scrapeDarazProduct()`: Scrapes product details from Daraz.
-* `generateEmailBody()` and `sendEmail()`: Generate and send email notifications based on specific conditions.
-* Helper functions (`getLowestPrice()`, `getHighestPrice()`, `getAveragePrice()`, `getEmailNotifType()`) are used to calculate prices and determine notification types.</t>
+3. Scrapes the latest product details from Daraz using `scrapeDarazProduct`.
+4. Updates each product's price history, lowest/highest/average prices, and saves it back to the database.
+5. Checks each product's status and sends email notifications based on specific criteria (using `getEmailNotifType`).
+6. Returns a JSON response with an "Ok" message and updated products data.
+**Libraries Used:**
+* Next.js (`next/server`)
+* Mongoose (`@/lib/mongoose`) for database interactions
+* Product model (`@/lib/models/product.model`)
+* Scrape function (`scrapeDarazProduct` from `@/lib/scrapper`)
+* Email sending functions (`generateEmailBody` and `sendEmail` from `@/lib/nodemailer`)</t>
         </is>
       </c>
     </row>
@@ -547,25 +552,28 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>This is a Tailwind CSS configuration file that defines various utility classes for styling a web application. The code is divided into several sections:
-1. **Base styles**: The first section resets all elements to have no margin, padding, and box-sizing set to border-box.
-2. **Typography**: The second section sets the font family for the body element using the `font-inter` utility class.
-3. **Utilities**: This is the main section that defines various utility classes for styling different components of the application.
-The utilities section includes styles for:
-* Buttons (`btn`)
-* Headings (`head-text`)
-* Section text (`section-text`)
-* Small text (`small-text`)
-* Paragraph text (`paragraph-text`)
-* Hero carousel (`hero-carousel` and its child elements)
-* Trending section (`trending-section`)
-* Product details page (`product-container`, `product-image`, etc.)
-* Modals (`dialog-container`, `dialog-content`, etc.)
-* Navbar (`nav`, `nav-logo`)
-* Price info card (`price-info_card`)
-* Product card (`product-card`, `product-card_img-container`, etc.)
-* Searchbar input (`searchbar-input` and its related classes)
-These utility classes can be applied to HTML elements using the `@apply` directive, making it easy to reuse styles throughout the application.</t>
+          <t>This code is a Tailwind CSS configuration file that defines various design styles and classes for a web application. Here's a summary of the key points:
+**Global Styles**
+* The `*` selector sets global margin, padding, box-sizing, and scroll behavior.
+* The `body` element uses the "Inter" font.
+**Utilities**
+The code defines several utility classes for various UI components, including:
+* Button (`btn`): A button with a specific design style.
+* Headline text (`head-text`): A large headline with specific typography.
+* Section text (`section-text`): A medium-sized text block with specific typography.
+* Small text (`small-text`): A small text block with specific typography.
+* Paragraph text (`paragraph-text`): A standard paragraph of text.
+* Hero carousel (`hero-carousel`): A hero carousel component with specific design styles.
+* Carousel control dots (`carousel .control-dots`): A set of control dots for the carousel.
+* Product container (`product-container`): A container for product information.
+* Product image (`product-image`): An image container for products.
+* Product info (`product-info`): A block of information about a product.
+* Modals (`dialog-content`, `dialog-input_container`, etc.): Various modal components with specific design styles.
+* Navbar (`nav`): A navigation bar component.
+* Price info card (`price-info_card`): A card displaying price information.
+* Product card (`product-card`): A card displaying product information.
+* Searchbar input (`searchbar-input`): An input field for searching.
+Overall, this code provides a set of reusable design classes and styles that can be used throughout the application to maintain consistency in UI design.</t>
         </is>
       </c>
     </row>
@@ -577,18 +585,14 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Here is a summary of the code:
-**Importing Dependencies**
-The code imports font styles from Google Fonts (`Inter` and `Space_Grotesk`) using the `next/font/google` library, as well as metadata types from `next`. It also imports global CSS styling from a file named `globals.css`.
-**Defining Font Styles**
-The code defines two font styles: `inter` and `spaceGrotesk`, which are instances of the imported font styles. These fonts are used to render text in the application.
-**Exporting Metadata**
-The code exports metadata for the application, including a title (`"DarazScapper"`) and description (`"Track product prices"`).
-**Defining Root Layout Component**
-The code defines a `RootLayout` component that serves as the top-level layout for the application. The component takes a `children` prop (i.e., any React nodes) and renders them within a `&lt;main&gt;` element.
-**Rendering Navbar and Children**
-The component renders a `Navbar` component (imported from another file) above the main content, followed by the child components passed as props to the `RootLayout` component. The entire layout is wrapped in an HTML `html` tag with a language attribute set to "en".
-In summary, this code sets up a basic Next.js project with global CSS styling, font styles, and metadata for the application, and defines a top-level layout component that renders a navbar and child components within a `&lt;main&gt;` element.</t>
+          <t>Here is a summary of the provided code:
+**Purpose:** A Next.js application layout component that sets up basic HTML structure and typography.
+**Key Features:**
+* Imports Google Fonts (Inter and Space_Grotesk) for styling
+* Sets up global CSS styles from `globals.css` file
+* Defines metadata (title, description) for SEO purposes
+* Creates a reusable `RootLayout` component that wraps the application content
+**Functionality:** The code sets up a basic HTML structure with Google Fonts and a responsive design. It also defines a reusable layout component (`RootLayout`) that can be used throughout the application to wrap content.</t>
         </is>
       </c>
     </row>
@@ -601,17 +605,12 @@
       <c r="B8" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Purpose:** The code defines a React component named `Home` that serves as the main page for an e-commerce platform called DarazScapper.
-**Features:**
-1. **Hero Carousel**: A section featuring a hero image and a carousel with products.
-2. **Searchbar**: A search input field to find specific products.
-3. **Product Showcase**: A grid of trending products, displayed using the `ProductCard` component.
-4. **Description Text**: A brief introduction to DarazScapper, highlighting its features.
-**Functionality:**
-1. The `getAllProducts` function is called to fetch all product data from an external API.
-2. The fetched data is stored in a variable named `allProducts`.
-3. The `Home` component uses the `allProducts` data to render the trending products section.
-Overall, this code snippet is a key part of a larger React application that showcases DarazScapper's features and product offerings.</t>
+**Home Component**
+This React component, `Home`, is an asynchronous function that retrieves all products from the `getAllProducts` action and returns JSX elements to render on the page.
+The component consists of two main sections:
+1. **Hero Section**: A section with a hero carousel, searchbar, and introductory text.
+2. **Trending Products Section**: A section displaying trending products retrieved from the `getAllProducts` action, using a `ProductCard` component for each product.
+The code imports necessary components and libraries, including HeroCarousel, ProductCard, Searchbar, and uses Next.js's image library to display an icon.</t>
         </is>
       </c>
     </row>
@@ -623,21 +622,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>**Code Summary**
-The provided code is a React component named `ProductDetails` that displays detailed information about a specific product. It fetches the product data from an API using the `getProductById` function and displays various details such as:
-* Product image
-* Title, category, and description
-* Price information (current price, average price, highest price, lowest price)
-* Seller details (name, positive seller rating)
-* Similar products (a list of related products with their own cards)
-The component uses various custom components like `PriceInfoCard`, `ProductCard`, and `Modal` to display the product information.
-**Key Features**
-* Fetches product data from an API using `getProductById`
-* Displays detailed product information, including price, seller details, and similar products
-* Uses custom components for price and product cards
-* Handles pagination and lazy loading of similar products
-**Deployment Context**
-This code is likely used in a web application that showcases products with their detailed information. It can be deployed on a Next.js or other React-based framework to display product pages.</t>
+          <t>Here is a summary of the provided code:
+**Overview**
+The code defines a React component called `ProductDetails` that displays detailed information about a product. The component fetches data from an API to display the product's details, similar products, and seller information.
+**Features**
+1. **Product Details**: Displays the product's title, image, category, URL, and various price-related information (current price, original price, discount rate).
+2. **Similar Products**: Fetches a list of similar products based on the current product's ID and displays them in a grid.
+3. **Seller Information**: Displays the seller's shop name, positive seller rating, and link to their shop.
+4. **Modal**: A modal window is displayed at the bottom of the page with a "Buy Now" button that takes the user to the product's URL.
+**Libraries Used**
+1. Next.js (for routing and navigation)
+2. React (for building the UI component)
+3. `next/image` (for image optimization)
+4. `next/font/google` (for using custom fonts)
+**Functionality**
+The code uses two API functions: `getProductById` to fetch the product data by ID, and `getSimilarProducts` to fetch a list of similar products based on the current product's ID. The component also uses a utility function called `formatNumber` to format numerical values.
+Overall, this code provides a comprehensive view of a product's details, including its image, price information, seller info, and similar products.</t>
         </is>
       </c>
     </row>
@@ -650,16 +650,17 @@
       <c r="B10" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Component:** HeroCarousel
-**Purpose:** A responsive hero image carousel component for a web application.
-**Features:**
-* Displays a series of images in a carousel format
-* Uses the React Responsive Carousel library
-* Automatically loops through the images with an interval of 2 seconds
-* Does not show navigation arrows or status bar
-* Custom icon (hand-drawn arrow) is displayed at the bottom left corner
-**Images:** The component uses an array of image objects (`heroImages`) which contain the `imgUrl` and `alt` properties for each image.
-This summary should give you a high-level understanding of what the code does!</t>
+**Code Purpose:** The code creates a hero carousel component in React, which displays a series of images with automatic sliding and infinite looping.
+**Key Features:**
+* Uses `react-responsive-carousel` library for carousel functionality
+* Imports `Image` component from `next/image`
+* Defines an array of image objects (`heroImages`) with URLs and alt text
+* The `HeroCarousel` component maps through the image array and renders each image as a separate slide in the carousel
+* Customizes carousel behavior:
+	+ Hides thumbs, arrows, and status bar
+	+ Enables auto-play and infinite looping
+	+ Sets interval between slides to 2 seconds
+**Usage:** This code can be used in a Next.js application to create a hero carousel component that displays a series of images on the homepage or any other page.</t>
         </is>
       </c>
     </row>
@@ -672,22 +673,16 @@
       <c r="B11" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Purpose:** The `Modal` component displays a dialog box that allows users to enter their email address and receive product pricing alerts.
-**Features:**
-1. **Button trigger**: A "Track" button opens the modal.
-2. **Modal content**: The modal contains a form with an input field for the user's email address, a submit button, and a close icon.
-3. **Email submission**: When the submit button is clicked, the `handleSubmit` function sends the email address to the server using the `addUserEmailToProduct` API.
-4. **Loading state**: While submitting the form, a "Submitting..." text is displayed on the submit button.
-5. **Closing the modal**: Clicking the close icon or pressing Esc closes the modal.
-**Components and Libraries:**
-1. `React` for building user interfaces
-2. `useState` from React for managing state
-3. `@headlessui/react` for creating a responsive, accessible modal dialog box
-4. `Image` component from `next/image` for displaying images
-5. `addUserEmailToProduct` API function for submitting email addresses to the server
-**Key Functions:**
-1. `handleSubmit`: Handles form submission and sends email address to the server.
-2. `openModal` and `closeModal`: Toggle the modal's open state.</t>
+**Purpose:** A React component that displays a modal window to allow users to enter their email address and "track" a product, sending an alert to their inbox.
+**Key Features:**
+1. **Modal Window**: The component displays a modal window with a form to collect user's email address.
+2. **Product Tracking**: When the user submits the form, it calls an API function `addUserEmailToProduct` (not shown in this code snippet) to add the user's email to the product tracking system.
+3. **Button and Form Handling**: The component has a "Track" button that toggles the modal window open/close state, and handles the form submission by calling the `handleSubmit` function.
+**Technical Details:**
+1. The component uses React hooks (`useState`) to manage its internal state (e.g., modal window open/closed, submitting/ submitted).
+2. It utilizes the `@headlessui/react` library for creating a modal window and handling transitions.
+3. The component imports functions from other modules, such as `addUserEmailToProduct` from `/lib/action`, which suggests an API function to interact with a backend system.
+Let me know if you'd like me to clarify any specific aspect!</t>
         </is>
       </c>
     </row>
@@ -700,16 +695,15 @@
       <c r="B12" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**File:** React component file ( likely `Navbar.js`)
-**Purpose:** To render a navigation bar with logo, icons, and links.
-**Key Features:**
-* A logo image displayed alongside the brand name "Daraz Scrapper"
-* Three icons (search, heart, user) displayed in a row
-* Links to the homepage (`/`) for each icon
-**Libraries Used:**
-* `next/image` for image handling
-* `next/link` for client-side routing
-* React for building the UI component</t>
+**Navbar Component**
+The code defines a React component named `Navbar` that represents the navigation bar of an application. The component uses Next.js's built-in `Link` and `Image` components.
+**Features**
+* Displays the application logo with a link to the root URL (`"/"`)
+* Shows three navigation icons (search, heart, user) in a row
+* Each icon is an SVG image with alt text
+**Styles**
+The component uses CSS classes to style the navbar, including `w-full` for full-width and `gap-1`, `gap-5` for spacing between elements.
+Overall, this code creates a basic navigation bar with a logo and three icons that can be linked to other pages in the application.</t>
         </is>
       </c>
     </row>
@@ -722,17 +716,14 @@
       <c r="B13" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Component:** `PriceInfoCard`
-**Functionality:** Displays a card with a title, icon, and value.
-**Props:**
-* `title`: string (card title)
-* `iconSrc`: string (path to icon image)
-* `value`: string (displayed value)
-**HTML Structure:**
-* A container `&lt;div&gt;` with class `price-info_card`
+**PriceInfoCard Component**
+A reusable React component that displays a card with title, icon, and value information.
+* **Props**: `title` (string), `iconSrc` (image source string), `value` (displayed value string)
+* **Rendered Elements**:
 	+ A `&lt;p&gt;` element displaying the `title`
-	+ A flexible container (`&lt;div&gt;`) with an `Image` component displaying the `iconSrc` and a second `&lt;p&gt;` element displaying the `value`
-This code appears to be a reusable React component, likely used in a Next.js application.</t>
+	+ An `&lt;Image&gt;` element displaying the `iconSrc` image with alt text set to the `title`
+	+ Another `&lt;p&gt;` element displaying the `value` in a large, bold font
+* **Exported**: As a default export for use in other components.</t>
         </is>
       </c>
     </row>
@@ -744,14 +735,15 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>**Code Summary**
-The `ProductCard` component is a React functional component that displays information about a product. It takes a single prop, `product`, of type `Product`, which is imported from the `@/types` module.
-The component renders:
-1. A link to the product's details page using `Link` from `next/link`.
-2. An image container with an `Image` component from `next/image`, displaying the product's image.
-3. Product title and description in a card layout.
-4. Product category and current price, formatted for display.
-The code uses Next.js-specific features such as `Link` and `Image` components, as well as CSS classes for styling. It also utilizes TypeScript type checking through the `Product` interface.</t>
+          <t>Here is a summary of the code:
+**ProductCard Component**
+The `ProductCard` component is a React functional component that displays information about a product. It takes in a `product` object as a prop, which conforms to the `Product` type.
+**Key Features**
+* Displays an image of the product using the `Image` component from Next.js
+* Links to the product's details page when clicked
+* Shows the product's title, category ( truncated to 2 categories), and current price with currency
+**Props**
+The component expects a single prop: `product`, which is an object conforming to the `Product` type.</t>
         </is>
       </c>
     </row>
@@ -764,19 +756,19 @@
       <c r="B15" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Component:** `Searchbar`
-**Functionality:** A search bar component that allows users to input a Daraz product URL and submit it for scraping and storing.
-**Key Features:**
-1. **Validation**: The component checks if the input URL is valid by calling the `isValidDarazProductURL` function, which uses URL parsing to verify the URL belongs to daraz.com.
-2. **Scraping and Storage**: If the URL is valid, the component calls the `scrapeAndStoreProduct` function from a separate file (`@/lib/action`) to scrape product data from the input URL and store it.
-3. **Loading Indicator**: While scraping and storing, the component displays a "Searching..." message on the button.
-4. **Routing**: After successful scraping and storage, the component redirects the user to a new page with the scraped product ID using Next.js's `router.push` method.
-**State Management:**
-* The component uses React's `useState` hook to manage two state variables:
-	+ `searchPrompt`: stores the input URL
-	+ `isLoading`: tracks whether scraping and storage is in progress
+**Component:** `Searchbar` (a React functional component)
+**Purpose:** Allows users to search for products on Daraz by entering a product link.
+**Features:**
+1. Validation: Checks if the entered URL is valid and points to a Daraz product.
+2. Submission: Submits the form with the validated URL, triggering the `scrapeAndStoreProduct` function from `@/lib/action`.
+3. Navigation: Redirects the user to the product page (`/products/&lt;productId&gt;`) upon successful submission.
+**State Management:** Uses React's built-in `useState` hook to manage two states:
+1. `searchPrompt`: Stores the input URL entered by the user.
+2. `isLoading`: Indicates whether the search is in progress or not.
 **Event Handling:**
-* The component listens for a form submission event (`handleSubmit`) and calls the `scrapeAndStoreProduct` function when the submit button is clicked.</t>
+1. Form Submission (`handleSubmit`): Handles form submission, validates the URL, and submits it to the server.
+2. Input Change (`setSearchPrompt`): Updates the `searchPrompt` state on input change.
+Overall, this component provides a simple search bar that allows users to find products on Daraz by entering a product link.</t>
         </is>
       </c>
     </row>
@@ -789,22 +781,18 @@
       <c r="B16" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Overview**
-This code appears to be a part of a Next.js application that interacts with a MongoDB database. It provides functions for scraping product data from Daraz, storing and updating product information in the database, retrieving products by ID or all products, finding similar products, and adding user email addresses to specific products.
-**Key Functions**
-1. `scrapeAndStoreProduct`: Scrapes product data from Daraz, updates existing product records in the database if necessary, and revalidates the cache.
-2. `getProductById`: Retrieves a single product by its ID from the database.
-3. `getAllProducts`: Returns all products stored in the database.
-4. `getSimilarProducts`: Finds up to 3 similar products (excluding the specified product) and returns them.
-5. `addUserEmailToProduct`: Adds a user's email address to a specific product, sends a welcome email if necessary.
-**Dependencies**
-The code uses the following dependencies:
-* `next/cache` for revalidating cache paths
-* `mongoose` for interacting with the MongoDB database
-* `scrapeDarazProduct` for scraping product data from Daraz
-* `generateEmailBody` and `sendEmail` for sending emails using nodemailer
-**Error Handling**
-The code catches errors, logs them to the console, and throws a new error message if necessary.</t>
+**Purpose:** The code provides a set of functions to interact with a database of products. It uses Next.js caching and MongoDB to store and retrieve product data.
+**Functions:**
+1. **`scrapeAndStoreProduct(productUrl: string)`**: Scrapes product information from Daraz using `scrapeDarazProduct()` function, updates or creates a new product in the database, and revalidates the corresponding page.
+2. **`getProductById(productId: string)`**: Retrieves a product by its ID from the database.
+3. **`getAllProducts()`**: Returns all products in the database.
+4. **`getSimilarProducts(productId: string)`**: Finds three similar products to the one with the specified ID and returns them.
+5. **`addUserEmailToProduct(productId: string, userEmail: string)`**: Adds a user's email to the list of users for a specific product and sends a welcome email.
+**Database Interactions:**
+* The code uses MongoDB through the `mongoose` library to interact with the database.
+* It connects to the database using `connectToDB()` function before each interaction.
+**Notes:**
+* Some functions, such as `generateEmailBody()` and `sendEmail()`, are not imported or used in this code snippet.</t>
         </is>
       </c>
     </row>
@@ -816,19 +804,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Here is a summary of the provided code:
-**Mongoose Model Definition**
-The code defines a Mongoose model named `Product` using a schema. The schema has multiple fields, including:
-* Basic product information (url, currency, image, title, category)
-* Pricing and sales history (currentPrice, originalPrice, priceHistory)
-* Product reviews and ratings (reviewsCount, rateCount, reviewScores)
-* Inventory and stock status (isOutOfStock, productQuantityValue)
-* Seller information (productBrand, sellerShopName, sellerShopURL, positiveSellerRating)
-* User interactions (users)
-* Price statistics (lowestPrice, highestPrice, averagePrice)
-The model also includes default values for certain fields, such as `date` and `isOutOfStock`.
-**Exported Model**
-The code exports the defined `Product` model, making it available for use in other parts of the application.</t>
+          <t>Here is a summary of the code:
+**Mongoose Schema for Product Model**
+The code defines a Mongoose schema for a "Product" model. The schema has 25 fields, including:
+* Basic information: `url`, `currency`, `image`, `title`, `category`
+* Pricing and discounting: `currentPrice`, `originalPrice`, `priceHistory`, `discountRate`
+* User engagement: `reviewsCount`, `rateCount`, `reviewScores`
+* Inventory and stock status: `productQuantityValue`, `isOutOfStock`
+* Seller information: `sellerShopName`, `sellerShopURL`, `positiveSellerRating`
+* User associations: `users` (an array of user emails)
+* Additional metrics: `lowestPrice`, `highestPrice`, `averagePrice`
+The schema is set up to automatically add timestamps (`createdAt` and `updatedAt`) using the `{ timestamps: true }` option. A model instance named "Product" is exported, which can be used to interact with a MongoDB collection of products.</t>
         </is>
       </c>
     </row>
@@ -841,8 +827,8 @@
       <c r="B18" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Database Connection Manager**
-This code manages connections to a MongoDB database using Mongoose. It checks for an existing connection and establishes a new one if needed, logging errors and success messages. The connection is established using the `MONGODB_URI` environment variable, which must be defined for the connection to succeed.</t>
+**Database Connection Utility**
+This module establishes a connection to a MongoDB database using Mongoose. It checks if an existing connection exists, and if so, returns without reconnecting. Otherwise, it attempts to connect to the database specified by the `MONGODB_URI` environment variable, logging any errors that occur during connection establishment.</t>
         </is>
       </c>
     </row>
@@ -854,19 +840,23 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Here's a summary of the provided code:
-**Purpose**: This code is designed to generate and send email notifications for price tracking and stock updates.
-**Features**:
-1. It uses the `nodemailer` library to create an email transporter.
-2. It defines a `Notification` enum with four types: WELCOME, CHANGE_OF_STOCK, LOWEST_PRICE, and THRESHOLD_MET.
-3. The `generateEmailBody` function takes in product information (`product`) and notification type (`type`) as inputs and returns a subject and body for an email based on the specified type.
-4. It uses a switch statement to determine which template to use for each notification type.
-5. The `sendEmail` function sends the generated email using the transporter, taking in email content (`emailContent`) and recipient addresses (`sendTo`) as inputs.
-**Key Components**:
-1. `generateEmailBody`: This is the core function that generates the email subject and body based on the product information and notification type.
-2. `Notification` enum: Defines the four notification types used in the code.
-3. `nodemailer` transporter: Creates an email transporter using the specified configuration.
-**Context**: This code appears to be part of a larger application that provides price tracking and stock updates for products, likely using a database or API to retrieve product information.</t>
+          <t>Here is a summary of the code:
+**Overview**
+The code is a server-side script that generates and sends email notifications to users based on specific product updates. It uses Node.js, Nodemailer, and custom types.
+**Key Functions**
+1. `generateEmailBody`: Generates an email body for a given product and notification type (e.g., welcome, stock change, lowest price, threshold met). The function takes in the product information and notification type as arguments.
+2. `sendEmail`: Sends an email to one or more recipients using Nodemailer.
+**Notification Types**
+The code defines four notification types:
+1. WELCOME: A welcome message for a user tracking a product.
+2. CHANGE_OF_STOCK: An alert when a product is restocked.
+3. LOWEST_PRICE: An alert when a product reaches its lowest price ever.
+4. THRESHOLD_MET: An alert when a product's discount exceeds a certain threshold (40% in this case).
+**Email Generation**
+For each notification type, the `generateEmailBody` function creates an email subject and body based on the provided product information.
+**Email Sending**
+The `sendEmail` function uses Nodemailer to send an email with the generated content to one or more recipients.
+Let me know if you'd like me to clarify anything!</t>
         </is>
       </c>
     </row>
@@ -879,24 +869,25 @@
       <c r="B20" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Functionality:** The `scrapeDarazProduct` function scrapes product information from the Daraz website using web scraping techniques.
-**Key Features:**
-1. **Authentication**: The function uses environment variables (`BRIGHT_DATA_USERNAME` and `BRIGHT_DATA_PASSWORD`) to authenticate with a proxy server.
-2. **Data Extraction**: The function extracts data from the HTML content of a webpage, specifically from a script tag that contains JSON-formatted data.
-3. **Product Information**: The function extracts various product information, including:
-	* Product title
-	* Description
-	* Price (original and sale)
-	* Currency code
-	* Image URL
-	* Categories
-	* Reviews count and rating
-	* Availability (in-stock or out-of-stock)
+**Function Purpose**
+The `scrapeDarazProduct` function scrapes product information from a Daraz webpage and returns it in a structured format (`Product` type).
+**Input**
+* A URL pointing to a Daraz product page.
+**Logic**
+1. The function attempts to log in to a Bright Data proxy using a username, password, and session ID.
+2. It sends an HTTP GET request to the provided URL with the logged-in proxy credentials.
+3. It parses the HTML response using Cheerio.
+4. It searches for a specific script tag on the page that contains JSON data about the product.
+5. If found, it extracts various product details from this JSON data, including:
+	* Product title, description, brand, and categories
 	* Seller information (name, URL, rating)
-4. **Data Return**: The function returns a `Product` object containing the extracted data.
-**Error Handling:**
+	* Product ratings (average, count, scores)
+	* Price history (sale price, original price, discount rate)
+	* Availability (quantity value, out-of-stock status)
+6. It returns the extracted product data in a structured format (`Product` type).
+**Error Handling**
 The function catches any errors that occur during execution and throws a new error with a descriptive message.
-Note that this summary is based on my understanding of the code and may not be exhaustive or entirely accurate. If you have specific questions about the code, I'd be happy to try and help!</t>
+Overall, this code appears to be a web scraper designed to extract product information from Daraz product pages.</t>
         </is>
       </c>
     </row>
@@ -908,18 +899,18 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Here is a summary of the provided code:
-**Purpose:** The code appears to be part of a web scraping project that extracts product information from online marketplaces (likely Daraz) and performs various calculations on the extracted data.
+          <t>Here is a summary of the code:
 **Functions:**
-1. **`extractPrice`**: Extracts the price of a product from a list of possible HTML elements.
-2. **`extractCurrency`**: Extracts the currency symbol from an HTML element.
-3. **`extractDescription`**: Extracts the description of a product from two possible HTML elements (`.a-unordered-list .a-list-item` and `.a-expander-content p`).
-4. **`getHighestPrice`, `getLowestPrice`, and `getAveragePrice`**: Calculate the highest, lowest, and average prices of a product based on its price history.
-5. **`getEmailNotifType`**: Determines the type of email notification to send based on changes in product availability, price, or discount rate.
-6. **`formatNumber`**: Formats a number with commas as thousand separators.
-**Types:**
-The code imports various types from `@/types`, including `Price`, `PriceHistoryItem`, and `Product`.
-Overall, the code provides a set of utility functions for extracting and processing product information, which can be used in a larger web scraping project.</t>
+1. `extractPrice`: Extracts the price from a list of possible elements, using regular expressions to clean and parse the text.
+2. `extractCurrency`: Extracts the currency symbol from an element.
+3. `extractDescription`: Extracts the description from two possible HTML elements on Daraz (a e-commerce platform).
+4. `getHighestPrice`, `getLowestPrice`, and `getAveragePrice`: Calculate the highest, lowest, and average price from a list of price history items.
+5. `getEmailNotifType`: Returns a notification type based on changes in product data (e.g., lowest price, stock status, discount rate).
+6. `formatNumber`: Formats a number as a string with commas.
+**Constants:**
+1. `Notification`: An object containing notification types (e.g., WELCOME, CHANGE_OF_STOCK, LOWEST_PRICE).
+2. `THRESHOLD_PERCENTAGE`: A threshold percentage for discount notifications (40%).
+The code appears to be part of a larger system that scrapes product data from Daraz and sends notifications based on changes in the data.</t>
         </is>
       </c>
     </row>
@@ -932,15 +923,16 @@
       <c r="B22" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Next.js Configuration File**
-This code exports a Next.js configuration object (`nextConfig`) that enables experimental features and customizes image loading.
-**Key Features:**
-1. **Experimental Server Actions**: Enables server actions in Next.js, allowing for more complex server-side rendering.
-2. **External Packages**: Allows the use of external packages (in this case, `mongoose`) with server components.
-3. **Image Loading Configuration**:
-	* Specifies allowed image domains (`static-01.daraz.com`, `static-01.daraz.com.np`, and `np-live-21.slatic.net`).
-4. **Exports**: Exports the `nextConfig` object as a module, making it available for use in other parts of the application.
-Let me know if you'd like me to elaborate on any specific aspect!</t>
+**Next.js Configuration**
+This code exports a Next.js configuration object (`nextConfig`) that customizes server behavior and image settings.
+**Key Settings:**
+* **Server Actions**: Enabled using `serverActions: true` to allow server-side rendering and API calls.
+* **Server Components External Packages**: Allows external packages (e.g., `mongoose`) to be used in server components.
+* **Image Domains**: Specifies which domains are allowed to serve images, including:
+	+ `static-01.daraz.com`
+	+ `static-01.daraz.com.np` and `np-live-21.slatic.net`
+**Export**
+The `nextConfig` object is exported as a module, making it available for use in the Next.js project.</t>
         </is>
       </c>
     </row>
@@ -952,14 +944,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>The provided JSON output appears to be a package manifest, likely generated by `npm ls` or another dependency manager. It lists various dependencies installed in a project, along with their versions and source information.
-Here are the main points summarized from this output:
-1. The project has many dependencies listed, including `@babel/core`, `ansi-styles`, `cross-spawn`, `glob`, `json-schema`, etc.
-2. Each dependency is identified by its name, version number, resolved URL (i.e., the location of the package on npm), and integrity hash (a unique digital signature for verification purposes).
-3. Some dependencies have additional information listed under a "requires" section, indicating that they depend on specific versions of other packages.
-4. The list also includes some development-only dependencies (marked as `dev: true` in the output), such as `eslint`, `jest`, and `yaml`.
-5. Overall, this output provides detailed information about the project's dependency tree, allowing you to identify any potential issues or upgrade opportunities for your project.
-If you'd like me to extract specific details from this output, please let me know what you're looking for!</t>
+          <t>This is a JSON object that contains information about the dependencies of an npm package. The object has several properties, including:
+* A list of installed packages (`"dependencies"`)
+* A list of devDependencies (`"devDependencies"`), which are packages required only for development purposes
+* A property called `lastPublish`, which stores the date when the package was last published
+The object contains over 40 different packages with their respective versions, resolved URLs, integrity hashes, and dependencies (if any). Some examples of these packages include:
+* `ajv`
+* `better-sqlite3`
+* `electron`
+* `express`
+* `gulp`
+* `webpack`</t>
         </is>
       </c>
     </row>
@@ -971,22 +966,28 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>**Package Summary**
-This is a `package.json` file, which contains metadata for a JavaScript project. Here's a summary of the contents:
-* **Project Name**: darazscan (version 0.1.0)
-* **Type**: Private development project
-* **Scripts**: Defined scripts for:
-	+ Development: `next dev`
-	+ Building: `next build`
-	+ Starting: `next start`
-	+ Linting: `next lint`
-* **Dependencies**:
-	+ Various JavaScript libraries and frameworks, including React, Next.js, Mongoose, Axios, and others (version 13.5.5 or higher)
-* **Dev Dependencies**:
-	+ TypeScript and related type definitions
-	+ Autoprefixer and PostCSS for CSS processing
-	+ Tailwind CSS for styling
-This package appears to be a web development project built with Next.js, using React and other JavaScript libraries for functionality and styling.</t>
+          <t>This is a `package.json` file, which is a JSON (JavaScript Object Notation) file used to manage dependencies and scripts for a Node.js project.
+**Project Details**
+* Name: darazscan
+* Version: 0.1.0
+* Private: true (indicates that this package should not be published on the npm registry)
+**Scripts**
+The project has four scripts defined:
+* `dev`: runs `next dev` to start the development server
+* `build`: runs `next build` to build the project for production
+* `start`: runs `next start` to start the production server
+* `lint`: runs `next lint` to run code linter
+**Dependencies**
+The project depends on the following packages:
+* Front-end frameworks and libraries: Next.js, React, React DOM, Headless UI, Responsive Carousel, Cheerio
+* Server-side dependencies: Mongoose (for MongoDB interactions), Nodemailer (for email sending)
+* Utilities: Axios (for HTTP requests)
+**Dev Dependencies**
+The project has the following dev dependencies:
+* Type definitions for Node.js and its libraries
+* PostCSS and Autoprefixer for CSS processing
+* Tailwind CSS for styling
+* TypeScript for programming language features</t>
         </is>
       </c>
     </row>
@@ -998,10 +999,13 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>This code is a configuration file for a CSS build tool, likely Webpack or a similar tool. It exports an object that specifies two plugins to be used in the build process:
-1. **Tailwind CSS**: A utility-first CSS framework.
-2. **Autoprefixer**: A plugin that adds vendor prefixes to CSS properties automatically.
-In summary, this code sets up Tailwind CSS and Autoprefixer as plugins for a CSS build tool.</t>
+          <t>This code exports a configuration object for a JavaScript module, specifically for a project using Tailwind CSS and Autoprefixer.
+In summary:
+* The code exports an object with a single property called "plugins".
+* The "plugins" property contains two sub-properties:
+	+ "tailwindcss": This suggests that the project uses the Tailwind CSS utility-first CSS framework.
+	+ "autoprefixer": This indicates that the project uses Autoprefixer, a popular plugin for adding vendor prefixes to CSS rules.
+Overall, this code is likely used in a build or configuration script (e.g. Webpack) to configure the project's CSS processing pipeline with Tailwind CSS and Autoprefixer plugins.</t>
         </is>
       </c>
     </row>
@@ -1013,29 +1017,16 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Here is a summary of the code:
-This is a Tailwind CSS configuration file that defines the content, theme, and plugins for a React application.
-**Content**
-* Specifies which files to scan for Tailwind classes:
-	+ Pages (`./pages/**/*.{js,ts,jsx,tsx,mdx}`)
-	+ Components (`./components/**/*.{js,ts,jsx,tsx,mdx}`)
-	+ App (`./app/**/*.{js,ts,jsx,tsx,mdx}`)
-**Theme**
-* Defines custom color palette:
-	+ Primary colors: `#E43030`, `#D48D3B`, and `#3E9242`
-	+ Secondary color: `#282828`
-	+ Grays: various shades from `#EAECF0` to `#101828`
-	+ Whites and blacks: `#F4F4F4`, `#EDF0F8`, `#3D4258`, and `#23263B`
-* Defines a custom box shadow:
-	+ Small (`xs`): `0px 1px 2px 0px rgba(16, 24, 40, 0.05)`
-* Defines custom max-width:
-	+ "10xl": `1440px`
-* Defines font families:
-	+ Inter and Space Grotesk
-* Defines a custom border radius:
-	+ 10: `"10px"`
-**Plugins**
-* No plugins are enabled in this configuration.</t>
+          <t>Here is a summary of the provided code:
+**Tailwind CSS Configuration**
+The code exports a Tailwind CSS configuration object that defines:
+1. **Content**: The files to scan for utility classes, including pages, components, and app directories.
+2. **Theme**:
+	* Extends the default theme with custom colors (e.g., `primary`, `secondary`, various shades of gray and white).
+	* Defines a custom `boxShadow` effect (`xs`) and `maxWidth` values (`10xl`).
+	* Specifies font families for `inter` and `spaceGrotesk`.
+3. **Plugins**: An empty array, indicating no plugins are used in this configuration.
+Overall, this code sets up Tailwind CSS to work with a specific project structure and design language, defining custom colors, shadows, max widths, fonts, and more.</t>
         </is>
       </c>
     </row>
@@ -1047,22 +1038,14 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>This code is a JSON configuration file for a TypeScript compiler, specifically targeting an ES5 ( ECMAScript 5) environment. It includes the following settings:
-* Compiler options:
-	+ Targets ES5 syntax
-	+ Includes DOM and iterable libraries
-	+ Allows JavaScript files to be compiled
-	+ Disables library checking
-	+ Enables strict mode
-	+ Suppresses code emission (i.e., no output file will be generated)
-	+ Enables interoperability between CommonJS and ES modules
-	+ Uses the "bundler" module resolution strategy
-	+ Resolves JSON modules
-	+ Compiles files in isolation
-	+ Preserves JSX syntax
-* Includes all files with .ts, .tsx, or .d.ts extensions, as well as specific Next.js environment configuration files.
-* Excludes node_modules directory.
-This configuration is likely used for a Next.js project to compile TypeScript code with specific settings.</t>
+          <t>Here is a summary of the code:
+**Configuration for a TypeScript Compiler**
+This configuration object sets up options for compiling TypeScript files. The key settings include:
+* **Target**: Compile to ES5 syntax
+* **Module system**: Use ESNext module format with bundler-based resolution
+* **Plugin**: Use the "next" plugin
+* **Include/Exclude**: Include specific files and directories, excluding `node_modules`
+The configuration is likely used in a Next.js project.</t>
         </is>
       </c>
     </row>
@@ -1074,22 +1057,20 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Here is a summary of the code:
-**Types Summary**
-This code defines several types related to e-commerce and notifications. The main types are:
-1. **PriceHistoryItem**: A single item in a product's price history, containing a `price` property.
-2. **User**: An object representing a user, with an `email` property.
-3. **Product**: An object representing a product, containing various properties such as:
-	* Product metadata (e.g., `_id`, `url`, `currency`, etc.)
-	* Pricing information (e.g., `currentPrice`, `originalPrice`, `priceHistory`)
-	* Review and rating information
-	* Seller information
-4. **NotificationType**: An enumeration of possible notification types, including welcome messages, stock changes, lowest price notifications, and threshold met notifications.
-5. **EmailContent**: An object containing email subject and body text.
-6. **EmailProductInfo**: An object containing product title and URL for an email.
-7. **Price**: An object representing a price, with `text` and `value` properties.
-**Key Features**
-The code uses TypeScript types to define the structure of these objects. The types are designed to be used in a Node.js or similar environment. The emphasis on product pricing, review, and rating information suggests an e-commerce application.</t>
+          <t>Here is a summary of the provided code:
+**Data Types and Schemas**
+The code defines several data types and schemas using TypeScript syntax. These include:
+1. **PriceHistoryItem**: An object with a single property `price` of type `Price`.
+2. **User**: An object with a single property `email` of type `string`.
+3. **Product**: A comprehensive object representing a product, with various properties such as:
+	* `_id`, `url`, and other product details
+	* Pricing information (`currentPrice`, `originalPrice`, etc.)
+	* Inventory and sales data (e.g., `priceHistory`, `reviewsCount`, etc.)
+	* Seller information (`sellerShopName`, `sellerShopURL`, etc.)
+4. **NotificationType**: A string enum with four possible values: "WELCOME", "CHANGE_OF_STOCK", "LOWEST_PRICE", and "THRESHOLD_MET".
+5. **EmailContent** and **EmailProductInfo**: Objects representing email content and product information, respectively.
+6. **Price**: An object representing a price value, with properties `text` (display string) and `value` (numeric value).
+These data types and schemas appear to be part of an e-commerce or online marketplace system, managing products, users, notifications, and email communications.</t>
         </is>
       </c>
     </row>
@@ -1101,11 +1082,13 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>The provided code is a JSON object that defines a single cron job configuration. Here's a summary:
-**Cron Job Configuration**
-* The path for the cron job is `/api/cron`.
-* The schedule specifies that the task should run at 13:30 (1:30 PM) every day, as represented by the `30 13 * * *` format.
-In short, this code sets up a daily cron job to run at 1:30 PM.</t>
+          <t>This JSON code defines a single cron job with the following details:
+* The path to access the cron job is `/api/cron`
+* The schedule for the cron job to run is every day at 1:30 PM (13:30 in 24-hour format), as specified by the "schedule" string `30 13 * * *`. 
+This schedule uses the standard cron syntax, where:
+- `30` specifies the minute
+- `13` specifies the hour
+- `*` is a wildcard that matches any value for minutes and hours after these specified times</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated print statements with newline characters, modified clone_github.py, and changed various file contents.
</commit_message>
<xml_diff>
--- a/output/Daraz_Scraper_summary.xlsx
+++ b/output/Daraz_Scraper_summary.xlsx
@@ -650,17 +650,16 @@
       <c r="B10" t="inlineStr">
         <is>
           <t>Here is a summary of the code:
-**Code Purpose:** The code creates a hero carousel component in React, which displays a series of images with automatic sliding and infinite looping.
-**Key Features:**
-* Uses `react-responsive-carousel` library for carousel functionality
-* Imports `Image` component from `next/image`
-* Defines an array of image objects (`heroImages`) with URLs and alt text
-* The `HeroCarousel` component maps through the image array and renders each image as a separate slide in the carousel
-* Customizes carousel behavior:
-	+ Hides thumbs, arrows, and status bar
-	+ Enables auto-play and infinite looping
-	+ Sets interval between slides to 2 seconds
-**Usage:** This code can be used in a Next.js application to create a hero carousel component that displays a series of images on the homepage or any other page.</t>
+**Component:** `HeroCarousel`
+**Description:** A React component that renders a carousel of hero images.
+**Features:**
+* Uses the `react-responsive-carousel` library to display a responsive carousel.
+* Displays 5 images from an array (`heroImages`) as a slideshow.
+* Each image is a Next.js `Image` component with a fixed width and height.
+* The carousel has infinite looping, auto-play, and a 2-second interval between slides.
+* No arrow or status indicators are shown in the carousel.
+**Styles:**
+* The component uses CSS classes to position an absolute icon (a hand-drawn arrow) at the bottom-left of the container.</t>
         </is>
       </c>
     </row>

</xml_diff>